<commit_message>
Unit test working for display rules and events
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6D5D51E0-64BE-4FA8-A405-A1019B3E8D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D3ACE042-ABED-4667-BAB9-1501573829FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="16520" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -78,20 +78,6 @@
     <t>r20.13</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.2 Advance Scenario&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An Advance scenario represents the fluid situations that developed as the Division was driving through enemy territory and meeting only scattered groups of defenders. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An Advance scenario follows the Sequence of Play as described in &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r20.3 Battle Scenario&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A Battle scenario represents an assault by the Division against prepared and well-defended positions. Resistance will be higher than for advance scenarios. Only limited amounts of territory will be gained. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Battle scenario follows the Sequence of Play as described in &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r20.13 Expected Enemy Resistance&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The resistance code for the day will affect the probabiliity of battle when a new area is entered on the Movement Board and the number of enemy units activated on the Battle Board. 
@@ -110,21 +96,6 @@
 If the number rolled is higher than the code number, you miss combat this day. Mark the day off as completed on teh calender, and go on to the next day.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.4 CounterAttack Scenario&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A Counterattack scenario represents the Division on defense against an enemy counterattack. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Because the enemy is coming at you, the Sequence of Play &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; changes. The Sequence of Play is modified as follows after the Time Check &lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; determines how much time has passed since sunrise:&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1.) &lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r40.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for Preparations&lt;LineBreak/&gt;
-2.) &lt;InlineUIContainer&gt;&lt;Button Content='r4.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for Movement&lt;LineBreak/&gt;
-3.) &lt;InlineUIContainer&gt;&lt;Button Content='r4.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for Battle</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r20.41 CounterAttack - Preparations&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For step &lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, you deploy automatically to Stopped/Hull Down state. Place a Hull Down marker on your tank. Steps &lt;InlineUIContainer&gt;&lt;Button Content='r4.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; through &lt;InlineUIContainer&gt;&lt;Button Content='r4.47' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; remain unchanged.</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;r20.1 Combat Calendar&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 For each day of the campaign, the Combat Calendar shows either the notation 'Refitting' or a three part scenario code such as 'A-2-L'. 
@@ -145,11 +116,34 @@
 When daylight runs out, the day is over. Go to the Evening DeBriefing. If a battle does occur, mark off 15 minutes and go to Battle &lt;InlineUIContainer&gt;&lt;Button Content='r4.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;r20.42 CounterAttack - Retreat from Battle Board&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you retreat from the Battle Board, mark off 15 minutes and record the loss of one area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Move your Task Force marker one area on the Movement Board in the direction of the Exit marker by the shortest route. If two or more areas are equally close, you may choose either one.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Go back to Prepare for Battle &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r20.2 Advance Scenario&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An Advance scenario represents the fluid situations that developed as the Division was driving through enemy territory and meeting only scattered groups of defenders. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An Advance scenario follows the Sequence of Play &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r20.3 Battle Scenario&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A Battle scenario represents an assault by the Division against prepared and well-defended positions. Resistance will be higher than for advance scenarios. Only limited amounts of territory will be gained. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Battle scenario follows the Sequence of Play &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r20.43 CounterAttack - Battle&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Delete steps &lt;InlineUIContainer&gt;&lt;Button Content='r4.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and &lt;InlineUIContainer&gt;&lt;Button Content='r4.64' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. If no Ambush occurs, go to the Battle Round Sequence &lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. If an Ambush does occur, do not conduct Enemy Actions, but instead perform the following steps:
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- For your tank, go to Battle Round Sequence &lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; through &lt;InlineUIContainer&gt;&lt;Button Content='r4.74' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+-- For your tank, go to Battle Sequence &lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; -&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r4.74' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
 -- Perform step &lt;InlineUIContainer&gt;&lt;Button Content='r4.76' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: Friendly Action Phase &lt;LineBreak/&gt;
 -- Perform step &lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: Random Events Phase&lt;LineBreak/&gt;
 -- Go to step 4.7: Battle Round Sequence
@@ -160,18 +154,24 @@
   <si>
     <t>&lt;Bold&gt;r20.42 CounterAttack - Clear Battle Board&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If battle (or even your Ambush) clears the board of enemy units, return to Time Check to determine how mnay hours pass before a battle becomes possible again. 
+If battle (or even your Ambush) clears the board of enemy units, return to Time Check to determine how many hours pass before a battle becomes possible again. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Mark off the hours that pass, and go to Prepare for Battle &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.42 CounterAttack - Retreat from Battle Board&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If you retreat from the Battle Board, mark off 15 minutes and record the loss of one area. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Move your Task Force marker one area on the Movement Board in the direction of the Exit marker by the shortest route. If two or more areas are equally close, you may choose either one.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Go back to Prepare for Battle &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+    <t>&lt;Bold&gt;r20.41 CounterAttack - Preparations&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For step &lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, you deploy automatically to Hull Down state. Place a Hull Down marker on your tank. Steps &lt;InlineUIContainer&gt;&lt;Button Content='r4.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; through &lt;InlineUIContainer&gt;&lt;Button Content='r4.47' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; remain unchanged.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r20.4 CounterAttack Scenario&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A Counterattack scenario represents the Division on defense against an enemy counterattack. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Because the enemy is coming at you, the Sequence of Play &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; changes. The Sequence of Play is modified as follows after the Time Check &lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; determines how much time has passed since sunrise:&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) &lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for Preparations&lt;LineBreak/&gt;
+2.) &lt;InlineUIContainer&gt;&lt;Button Content='r4.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r20.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for Movement&lt;LineBreak/&gt;
+3.) &lt;InlineUIContainer&gt;&lt;Button Content='r4.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; --&gt; &lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for Battle</t>
   </si>
 </sst>
 </file>
@@ -540,14 +540,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.125" style="2"/>
-    <col min="2" max="2" width="143.25" style="2" customWidth="1"/>
+    <col min="2" max="2" width="149.875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -579,23 +579,23 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
@@ -603,15 +603,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="214" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
@@ -635,7 +635,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
checkpointing - working on start
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6425ACD-C948-4792-927F-02EF79C9D040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3F0CFC1-AC5F-4C9C-ABBF-DD6992B238B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -89,24 +89,6 @@
 H = Heavy</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.12 Probability of Combat&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D. If the number rolled is less than or equal to the number shown on the scenario code, you go to action this day and begin the Sequence of Play &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the number rolled is higher than the code number, you miss combat this day. Mark the day off as completed on teh calender, and go on to the next day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r20.1 Combat Calendar&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each day of the campaign, the Combat Calendar shows either the notation 'Refitting' or a three part scenario code such as 'A-2-L'. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When Patton's Division is refitting, it is in reserve absorbing replacements and retraining &lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. The presence of a scenario code indicates: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Type of scenario &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Probability of being in combat&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Expected enemy resistance. </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r20.42 CounterAttack - Movement&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Delete step &lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and all operations of step &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; except for Ammo Resupply. 
@@ -177,9 +159,27 @@
     <t>r1.1</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;Bold&gt;r20.1 Combat Calendar&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each day of the campaign, the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; shows either the notation 'Refitting' or a three part scenario code such as 'A-2-L'. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When Patton's Division is refitting, it is in reserve absorbing replacements and retraining &lt;InlineUIContainer&gt;&lt;Button Content='r27.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. The presence of a scenario code indicates: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Type of scenario &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Probability of being in combat&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Expected enemy resistance. </t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r1.1 Description&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Bold&gt;PATTON'S BEST&lt;/Bold&gt; recreates the World War II campaing in nothern Europe through the eyes of a tank commander in George Patton's most famous unit, the 4th Armored Division. Patton's Best is designed as a solitaire game, with you acting as the commander of a Sherman tank. As the commander, you control the actions of your crew, and through them, fight and maneuver your tank. The actions of the enemy tanks and troops, as well as friendly forces  on your side, are randomly generated by various game aides and tables. Each scenario consists of a single engagement or a day  of movement and battle. However, the game realizes is full interest when played as a campaign which allows you to take part in every historical battle of the 4th Armored Division. You and your crew can witness and participate in the great drives across Europe, the battles for the Siegfried Line, the relief of Bastogne, and the crossing of the Rhine.</t>
+&lt;Bold&gt;PATTON'S BEST&lt;/Bold&gt; recreates the World War II campaing in nothern Europe through the eyes of a tank commander in George Patton's most famous unit, the 4th Armored Division. Patton's Best is designed as a solitaire game, with you acting as the commander of a Sherman tank. As the commander, you control the actions of your crew, and through them, fight and maneuver your tank. The actions of the enemy tanks and troops, as well as friendly forces  on your side, are randomly generated by various game aides and tables. Each scenario consists of a single engagement or a day  of movement and battle. However, the game realizes its full interest when played as a campaign which allows you to take part in every historical battle of the 4th Armored Division. You and your crew can witness and participate in the great drives across Europe, the battles for the Siegfried Line, the relief of Bastogne, and the crossing of the Rhine.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r20.12 Probability of Combat&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D. If the number rolled is less than or equal to the number shown on the scenario code, you go to action this day and begin the Sequence of Play &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the number rolled is higher than the code number, you miss combat this day. Skip this day on the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, and go on to the next day.</t>
   </si>
 </sst>
 </file>
@@ -548,33 +548,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="2"/>
-    <col min="2" max="2" width="149.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="149.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -582,12 +582,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
@@ -598,68 +598,68 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="1"/>
     </row>
-    <row r="128" spans="2:2" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="1"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding new rules for Crew Ratings
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{06CEFDB0-AEF8-4C24-8C24-916A9B6D705A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{29D40DE5-6127-47CA-86F3-0E5FA6345499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>r20.1</t>
   </si>
@@ -311,6 +311,45 @@
 Numbers shown around the edge of the movement board distinguish those areas that may be start or exit areas. Roads shown are of two types: improved highwas (gray black) and dirt country roads (brown).
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                               &lt;InlineUIContainer&gt;&lt;Image Name='MapMovement' Height='200' Width='200'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r7.0</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r7.0 Crew Ratings&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Each crew member is given a numerical rating of his skill at his position. The rating range from 1 (poorest) to 10 (best). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The higher the crew member's rating, the more successful he will be trying to spot enemy units, hit enemy units with his weapons, repair malfunctioning guns, etc. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The crew ratings are recorded on the After Action Report (AAR) &lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Ratings for New Men&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rating Improvements&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>r7.1</t>
+  </si>
+  <si>
+    <t>r7.2</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r7.1 Ratings for New Men&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine the rating for a new crew member by rolling 1D/2 rounded up. For example, a roll of five results in a rating of 3.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When rolling for more than one new crewman, assign the rating after all have been rolled for. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, if rolling for an entire crew, roll five ratings and then assign to men as you wish. It is suggested that the higher ratings be allocated in this order: Commander, Gunner, Driver, Loader, and Assistant Driver.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r7.2 Ratings Improvement&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At the end of the day of action, check for each surviving crew member to see if his rating improves. Roll 1D separately for each. If the number rolled is higher than the current rating, the rating is increased by one. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, your gunner has a rating of 5 and you roll a 9. The gunner's rating increases to 6.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Crew ratings cannot be greater than 10 and never decrease. Ratings cannot improve if you avoid action for the day per &lt;InlineUIContainer&gt;&lt;Button Content='r20.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ratings may also improve during refitting periods per &lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -677,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B240"/>
+  <dimension ref="A1:B243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -769,110 +808,125 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="99.85" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="171.2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="85.6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="185.45" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:2" ht="114.15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -971,7 +1025,7 @@
       <c r="B57" s="1"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
+      <c r="B58" s="1"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="1"/>
@@ -980,7 +1034,7 @@
       <c r="B60" s="1"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
+      <c r="B61" s="3"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
@@ -1207,7 +1261,7 @@
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="1"/>
     </row>
-    <row r="137" spans="2:2" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="1"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
@@ -1216,7 +1270,7 @@
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="1"/>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="1"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
@@ -1519,9 +1573,18 @@
     <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
     </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B241" s="1"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B242" s="1"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B243" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A65:B240">
-    <sortCondition ref="A65:A240"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A68:B243">
+    <sortCondition ref="A68:A243"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
workin gon more rules
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5699D6B6-C586-43DF-8134-348D306654D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C3D3E8-2406-412A-8C51-02A761967B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>r20.1</t>
   </si>
@@ -191,14 +191,6 @@
   </si>
   <si>
     <t>r7.2</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r7.1 Ratings for New Men&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Determine the rating for a new crew member by rolling 1D/2 rounded up. For example, a roll of five results in a rating of 3.  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When rolling for more than one new crewman, assign the rating after all have been rolled for. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For example, if rolling for an entire crew, roll five ratings and then assign to men as you wish. It is suggested that the higher ratings be allocated in this order: Commander, Gunner, Driver, Loader, and Assistant Driver.</t>
   </si>
   <si>
     <t>r19.0</t>
@@ -502,6 +494,86 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.47' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; remain unchanged.</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;r20.42 Counterattack - Movement&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Delete step &lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and all operations of step &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; except for Ammo Resupply. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Instead each 15 minutes, roll 1D on the Resistance Table 
+&lt;InlineUIContainer&gt;&lt;Button Content='t002' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to determine if a battle occurs. If not, mark off 15 minutes and roll again. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When daylight runs out, the day is over. Go to the Evening DeBriefing. If a battle does occur, mark off 15 minutes and go to Battle 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r19.22 Serious Wounds&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If a crew member takes a wound that uts him out of action for one week or more, he is incapacitated and immediately ceases performing any crew actions. 
+Note incapacitated crewmen in the notes section of the After Action Report (AAR) 
+&lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The assistant driver may move through the tank to replace any one incapacitated crewmen. An incapacitated driver is moved to the assistant driver's position, and incapacitated men in the turret are placed on the turret floor.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+While occupying any other position except driver, the assistant driver's rating is havled (rounded down). This change takes one full round.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r7.2 Ratings Improvement&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At the end of the day of action, check for each surviving crew member to see if his rating improves. Roll 1D separately for each. If the number rolled is higher than the current rating, the rating is increased by one. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, your gunner has a rating of 5 and you roll a 9. The gunner's rating increases to 6.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Crew ratings cannot be greater than 10 and never decrease. Ratings cannot improve if you avoid action for the day per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ratings may also improve during refitting periods per &lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r19.0 Crew Casualties&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When playing, it is possible for the crewmen of your tank to be wounded or killed. Crew casualties can occur when you tank is knocked out 
+or when a crewman at an open hatch is hit by artillery/small arms fire. In both cases, the degree of injury is determined by the Wounds Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Inside the Tank&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; With Open Hatches&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Replacing Crew Casualties&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r19.1 Inside the Tank&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Crewman with no hatch or with a closed hatch are inside the tank and can only be hurt by gunfire or a Panzerfaust attack which penetrates the tank's armor. 
+When an enemy attack successfully rolls To Kill your tank, it has been knocked out and your must check crew casualties.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Exploding Tank&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Non-Exploding Tank&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Bail Out&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Crew Rescue&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r7.1 Ratings for New Men&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine the rating for a new crew member by rolling 1D/2 rounded up. For example, a roll of five results in a rating of 3.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When rolling for more than one new crewman, assign the rating after all rolls have been performed for all new men. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, if rolling for an entire crew, roll five ratings and then assign to men as you wish. It is suggested that the higher ratings be allocated in this order: Commander, Gunner, Driver, Loader, and Assistant Driver.</t>
+  </si>
+  <si>
+    <t>r20.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r20.0 Campaign&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The campaign recreates actions of the 4th Armored Division from late July, 1944 through April, 1945. Each day the 4th Armored saw action,
+there is a chance your tank will fight; when the Division is refitting, you will be resting. Each day begins with a check of the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;Combat Calendar&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advance Scenario&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Battle Scenario&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; CounterAttack Scenario&lt;LineBreak/&gt;
+</t>
+  </si>
+  <si>
+    <t>r21.0</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r20.43 CounterAttack - Battle&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Delete steps &lt;InlineUIContainer&gt;&lt;Button Content='r4.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and 
@@ -509,69 +581,50 @@
 If no Ambush occurs, go to the Battle Round Sequence 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. If an Ambush does occur, do not conduct Enemy Actions, but instead perform the following steps:
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- For your tank, go to Battle Sequence &lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; -&gt; 
+For your tank, go to Battle Sequence &lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; -&gt; 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.74' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
--- Perform step &lt;InlineUIContainer&gt;&lt;Button Content='r4.76' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: Friendly Action Phase &lt;LineBreak/&gt;
--- Perform step &lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: Random Events Phase&lt;LineBreak/&gt;
--- Go to step 4.7: Battle Round Sequence
+Perform step &lt;InlineUIContainer&gt;&lt;Button Content='r4.76' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: Friendly Action Phase &lt;LineBreak/&gt;
+Perform step &lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;: Random Events Phase&lt;LineBreak/&gt;
+Go to Battle Round Sequence &lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If you clear the Battle Board, go to &lt;InlineUIContainer&gt;&lt;Button Content='r20.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; &lt;LineBreak/&gt;
 If you retreat from the Battle Board, go to &lt;InlineUIContainer&gt;&lt;Button Content='r20.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.42 Counterattack - Movement&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Delete step &lt;InlineUIContainer&gt;&lt;Button Content='r4.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and all operations of step &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; except for Ammo Resupply. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Instead each 15 minutes, roll 1D on the Resistance Table 
-&lt;InlineUIContainer&gt;&lt;Button Content='t002' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to determine if a battle occurs. If not, mark off 15 minutes and roll again. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When daylight runs out, the day is over. Go to the Evening DeBriefing. If a battle does occur, mark off 15 minutes and go to Battle 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r19.22 Serious Wounds&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If a crew member takes a wound that uts him out of action for one week or more, he is incapacitated and immediately ceases performing any crew actions. 
-Note incapacitated crewmen in the notes section of the After Action Report (AAR) 
-&lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The assistant driver may move through the tank to replace any one incapacitated crewmen. An incapacitated driver is moved to the assistant driver's position, and incapacitated men in the turret are placed on the turret floor.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-While occupying any other position except driver, the assistant driver's rating is havled (rounded down). This change takes one full round.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r7.2 Ratings Improvement&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-At the end of the day of action, check for each surviving crew member to see if his rating improves. Roll 1D separately for each. If the number rolled is higher than the current rating, the rating is increased by one. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For example, your gunner has a rating of 5 and you roll a 9. The gunner's rating increases to 6.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Crew ratings cannot be greater than 10 and never decrease. Ratings cannot improve if you avoid action for the day per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Ratings may also improve during refitting periods per &lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r19.0 Crew Casualties&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When playing, it is possible for the crewmen of your tank to be wounded or killed. Crew casualties can occur when you tank is knocked out 
-or when a crewman at an open hatch is hit by artillery/small arms fire. In both cases, the degree of injury is determined by the Wounds Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Inside the Tank&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; With Open Hatches&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Replacing Crew Casualties&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r19.1 Inside the Tank&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Crewman with no hatch or with a closed hatch are inside the tank and can only be hurt by gunfire or a Panzerfaust attack which penetrates the tank's armor. 
-When an enemy attack successfully rolls To Kill your tank, it has been knocked out and your must check crew casualties.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Exploding Tank&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Non-Exploding Tank&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Bail Out&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Crew Rescue&lt;LineBreak/&gt;</t>
+    <t>r21.1</t>
+  </si>
+  <si>
+    <t>r21.2</t>
+  </si>
+  <si>
+    <t>r21.3</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r21.1 Sunrise&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r21.2 Marking Time&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r21.3 Sunset&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r21.0 Time&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The length of a day of battle is determined by the passage of time. On the After Action Report (AAR) 
+&lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+is a section to mark time, where the hours 0500 through 1900 are each divided into four 15 minute blocks. The exception is 1900 because sunset will occur no later than 19:15.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the Time Check Phase &lt;InlineUIContainer&gt;&lt;Button Content='r4.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+of the sequence of play, the &lt;InlineUIContainer&gt;&lt;Button Content='Sunrise-Sunset' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table is used to determine the nours of sunrise and sunset. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Time is marked out according to rolls on this table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r21.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sunrise &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r21.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Marking Time&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r21.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sunset</t>
   </si>
 </sst>
 </file>
@@ -944,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B157"/>
+  <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -958,18 +1011,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="235.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="146.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -977,7 +1030,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="188.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -993,7 +1046,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="119.55" customHeight="1" x14ac:dyDescent="0.25">
@@ -1001,23 +1054,23 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="107.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="125" customHeight="1" x14ac:dyDescent="0.25">
@@ -1025,15 +1078,15 @@
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="122.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="161.69999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1041,7 +1094,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.25">
@@ -1057,7 +1110,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -1065,7 +1118,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="135.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,7 +1134,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -1089,216 +1142,256 @@
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="117.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="136.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="78.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="119.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="159.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="135.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="181.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="71.349999999999994" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="57.1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="63.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="156.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="156.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="76.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="76.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="35" spans="1:2" ht="177.3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="76.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="203.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="177.3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="76.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="203.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="2" t="s">
+    <row r="39" spans="1:2" ht="90.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="90.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B38" s="2" t="s">
+    <row r="40" spans="1:2" ht="156.9" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="150.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="219.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:2" ht="219.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="78.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="78.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="104.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:2" ht="104.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
-    </row>
-    <row r="157" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+    </row>
+    <row r="158" ht="154.55000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A85:B260">
-    <sortCondition ref="A85:A260"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A86:B261">
+    <sortCondition ref="A86:A261"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished tables on orange card
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C3D3E8-2406-412A-8C51-02A761967B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43364363-1CA6-4973-9534-F1485F5B6D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25974" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -505,17 +505,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r19.22 Serious Wounds&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If a crew member takes a wound that uts him out of action for one week or more, he is incapacitated and immediately ceases performing any crew actions. 
-Note incapacitated crewmen in the notes section of the After Action Report (AAR) 
-&lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The assistant driver may move through the tank to replace any one incapacitated crewmen. An incapacitated driver is moved to the assistant driver's position, and incapacitated men in the turret are placed on the turret floor.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-While occupying any other position except driver, the assistant driver's rating is havled (rounded down). This change takes one full round.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r7.2 Ratings Improvement&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 At the end of the day of action, check for each surviving crew member to see if his rating improves. Roll 1D separately for each. If the number rolled is higher than the current rating, the rating is increased by one. 
@@ -625,6 +614,17 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r21.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sunrise &lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r21.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Marking Time&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r21.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sunset</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r19.22 Serious Wounds&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If a crew member takes a wound that puts him out of action for one week or more, he is incapacitated and immediately ceases performing any crew actions. 
+Note incapacitated crewmen in the notes section of the After Action Report (AAR) 
+&lt;InlineUIContainer&gt;&lt;Button Content='r2.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The assistant driver may move through the tank to replace any one incapacitated crewmen. An incapacitated driver is moved to the assistant driver's position, and incapacitated men in the turret are placed on the turret floor.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+While occupying any other position except driver, the assistant driver's rating is halved (rounded down). This change takes one full round.</t>
   </si>
 </sst>
 </file>
@@ -999,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1134,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="117.55" customHeight="1" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="136.55000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1158,7 +1158,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="42.8" x14ac:dyDescent="0.25">
@@ -1214,7 +1214,7 @@
         <v>43</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="181.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1251,10 +1251,10 @@
     </row>
     <row r="31" spans="1:2" ht="142.65" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="156.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1334,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="78.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -1355,34 +1355,34 @@
     </row>
     <row r="44" spans="1:2" ht="199.7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="28.55" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Almost done with Prep phase
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DB5EFE7-0F8E-4C3F-ADBF-A02E2CFC4ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FCE637F-52D0-486D-94A3-5265EC1DDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -790,15 +790,6 @@
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c16Turret'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.45  Mark Loader Spot&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the loader is buttoned up or does not have a hatch, mark the sector he will be searching by placing the Loader Spot marker just outside the long range zone of a sector. If the commander is also buttoned up and does not have a vision cupola, place the Commander Spot marker similiarly for the sector hew will be searching. See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-            &lt;InlineUIContainer&gt;&lt;Image Name='c18LoaderSpot'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;           
-      &lt;InlineUIContainer&gt;&lt;Image Name='c19CommanderSpot'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>r4.46</t>
   </si>
   <si>
@@ -808,23 +799,6 @@
     <t>r17.1</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r17.0 Spotting&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Spotting is the attempt by your members to see and identify enemy units on the Battle Board. The placement of activated enemy units on the board does not mean that you see them. You know they are there perhaps because you have heard them or by radio reports. Until a crewman spots the unit, you do not see them and cannot shoot at it.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units on the Battle Board can be either:  1.) Unspotted,  2.) Spotted but not identified,  3.) Spotted and identified, &amp;amp;  4.) Hidden&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Spotting is attmpted during the Spotting Phase 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-of the Battle Round Sequence by referring to the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Spotting' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Procedure&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Restrictions &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Hidden Units &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Unidentified Units</t>
-  </si>
-  <si>
     <t>r17.11</t>
   </si>
   <si>
@@ -856,13 +830,6 @@
   </si>
   <si>
     <t>r17.25</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r17.12 Spotting Results&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the roll is equal to half or less than half of the crewman's rating (rounded down), he has also identified the unit. Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Apperance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table to detemine the specifc type of previously unidentified enemy tanks, SPs, and AT guns.</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r17.13 Spotting Modifiers&lt;/Bold&gt; 
@@ -877,15 +844,6 @@
 For each crewman attempting to spot a enemy unit, roll 1D. If the roll is less than or equal to the crewman's rating, he has spotted the unit. Mark the unit with a Spotted marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c32Spotted'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r17.14 Automatic Spotting Failure&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A spotting attempt roll of 9 or 10 before any modifications always means the unit is hidden from view in its current position andn spotting is impossible by any other crewman this round. Mark any hidden unit with a Hidden Marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You may not attempt to spot a hidden unit. A spotted unit cannot become hidden unless either it or your tank moves in following rounds.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Name='c31Hidden'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
   </si>
   <si>
     <t>&lt;Bold&gt;r17.15 Spotting Continuation&lt;/Bold&gt; 
@@ -904,13 +862,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Smoke Restrictions</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r17.21 Sector Restrictions&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The sectors in which each crewman may attempt to spot are noted on the Tank Card 
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Each crewman may attempt to spot every unit in the sector he can see. For example, the commander can spot into all sectors on an open hatch and thus may attempt to spot every enemy unit on the Battle Board.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r17.22 Crew Action Restrictions&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Performing certain crew actions may prevent a crewman from attempting to spot. Crew actions that allow spotting to continue have a spotting symbole on their marker.
@@ -992,13 +943,62 @@
  Table to determine what type of unit is actually present.</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;r17.21 Sector Restrictions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The sectors in which each crewman may attempt to spot are noted on the Tank Card 
+&lt;InlineUIContainer&gt;&lt;Button Content='r2.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Each crewman may attempt to spot every unit in the sector he can see. For example, the commander can spot into all sectors on an open hatch and thus may attempt to spot every enemy unit on the Battle Board.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r17.0 Spotting&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Spotting is the attempt by your members to see and identify enemy units on the Battle Board. The placement of activated enemy units on the board does not mean that you see them. You know they are there perhaps because you have heard them or by radio reports. Until a crewman spots the unit, you do not see them and cannot shoot at it.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units on the Battle Board can be either:  1.) Unspotted,  2.) Spotted but not identified,  3.) Spotted and identified, or 4.) Hidden.&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Spotting is attempted during the Spotting Phase 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+of the Battle Round Sequence by referring to the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Spotting' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Procedure&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Restrictions &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Hidden Units &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Unidentified Units</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r17.12 Spotting Results&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the roll is equal to half or less than half of the crewman's rating (rounded down), he has also identified the unit. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Appearance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to detemine the specifc type of previously unidentified enemy tanks, SPs, and AT guns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r17.14 Automatic Spotting Failure&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A spotting attempt roll of 9 or 10 before any modifications always means the unit is hidden from view in its current position and spotting is impossible by any other crewman this round. Mark any hidden unit with a Hidden Marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You may not attempt to spot a hidden unit. A spotted unit cannot become hidden unless either it or your tank moves in following rounds.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='c31Hidden'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r17.1 Spotting Procedure&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Roll&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Results &lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Modifiers &lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Automatic Spotting Failure &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Continuation</t>
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.15' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Continuation</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.45  Mark Loader Spot&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the loader is buttoned up or does not have a hatch, mark the sector he will be searching by placing the Loader Spot marker just outside the long range zone of a sector. If the commander is also buttoned up and does not have a vision cupola, place the Commander Spot marker similiarly for the sector hew will be searching. See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+                    &lt;InlineUIContainer&gt;&lt;Image Name='c18LoaderSpot'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;           
+      &lt;InlineUIContainer&gt;&lt;Image Name='c19CommanderSpot'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,7 +1383,7 @@
     <col min="2" max="2" width="216.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="300.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>49</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>54</v>
       </c>
@@ -1535,17 +1535,17 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="114.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>120</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>118</v>
@@ -1633,138 +1633,138 @@
     </row>
     <row r="32" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Refactor to use Stacks for displaying units on movement and battle board
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2512C94-0FDE-4726-B161-4761FACA786A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{1EA40052-200A-4EB9-AEF7-6AC711529BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
   <si>
     <t>r20.1</t>
   </si>
@@ -1115,13 +1115,6 @@
     <t>r22.2</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r22.0 Advancing Fire&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Advancing Fire represents blind HE and MG fire at places likely to be concealing unknown enemy units. It may take place both when you tank first enters a new map area and during Battle Rounds.
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Entering a New Area &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; During Battle Rounds&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r20.0 Campaign&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The campaign recreates actions of the 4th Armored Division from late July, 1944 through April, 1945. Each day the 4th Armored saw action,
 there is a chance your tank will fight; when the Division is refitting, you will be resting. Each day begins with a check of the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -1141,23 +1134,136 @@
     <t>r22.13</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;r22.11 Advancing Fire Ammo Use&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark off 1D/2 (round down) HE rounds and .30 caliber MG ammo boxes regardless of whether the battle occurs or not. Mark off on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r22.13 Advancing Fire Resolution&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing Fire is resolved in each Battle Board zone containing both an Advance Fire marker and enemy units during Battle Step 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.64' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each, roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table against each unit in the zone. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units kocked out are considered to be withdrawing and are not destroyed. No victory points are awarded. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Remove the Advancing Fire markers from the Battle Board after resolving.</t>
+  </si>
+  <si>
+    <t>r23.0</t>
+  </si>
+  <si>
+    <t>r23.1</t>
+  </si>
+  <si>
+    <t>r23.2</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.51 Mark Start Area&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Around the edge of the Movement Board, there are 10 areas number 1-10. Roll 1D to determine which of the ten is the start area for this scenario. Also, mark the area with a Start Area marker.
+Place the Task Force marker representing your friendly forces on that area.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                    &lt;InlineUIContainer&gt;&lt;Image Name='c33StartArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;           
+      &lt;InlineUIContainer&gt;&lt;Image Name='c35TaskForce'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r4.52 Mark Exit Area&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+On the &lt;InlineUIContainer&gt;&lt;Button Content='Exit Areas' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table, roll 1D and cross reference the number with the Start Area marker 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Mark the area with the Exit Area marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='c34ExitArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r4.54.2  Call for Artillery Support&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Call to hit an area adjacent to your task force. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if Artillery Support arrives 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+If successful, place an Artillery Support marker on the area. Three Artillery Support markers are allowed and can be placed in the same area. Continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.54.3  Call for Air Strike&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Call to hit an area adjacent to your task force. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if Air Strike arrives
+ &lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  If successful, place an Air Strike marker on the area. Two Air Strike markers are allowed and can be placed in the same area. Additionally, while waiting for air strike, a 15 minute operation can be chosen to happen in parallel. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>r23.11</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r23.1 Artillery Support Resolution&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Artillery support takes effect in a newly entered area immediately after any appearing enemy units are placed on the Battle Board. Resolve Arillery Support by rolling on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table against each enemy unit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units destroyed by artillery support are immediately removed, and their victory points ar recorded under friendly forces of the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll again against each surviving enemy unit for each additional support marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r23.1 Artillery Support&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Artillery support can be called for during the Movement Sequence 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+This operation takes 15 minutes. Mark off the time and rol 1D as shown on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Use Table to see if the support arrives. It arrives on 1-7 roll. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If successful, place an Artillery Support marker in the area where the artillery landed. If at any time during this day you enter the marked area (before reaching the exit area), the artillery support will attack all enemy units appearing. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Additional artillery support may be called for, but no more than three support markers may be on the Movement Board at one time. You may voluntarily pick up an Artillery Support marker if you decide to attempt to place it elsewhere.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r22.0 Advancing Fire&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing Fire represents blind HE and MG fire at places likely to be concealing unknown enemy units. It may take place both when you tank first enters a new map area and during Battle Rounds.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Entering a New Area &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; During Battle Rounds&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r22.1 Advancing Fire - Entering a New Area&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 When your tank force enters a new area on the Movement Board, you may have the task force conduct Advancing Fire. You make that choice during the Movement Sequence per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
 You may place a number of Advancing Fire markers on the Battle Board. If battle then occurs in the area, the Advancing Fire may remove enemy units appearing in the zones with the markers. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Your tank itself takes no sepcific action as the Advancing Fire is considered the effort of the entire task force including your tank. However, ammo is expended by your tank whether a battle occurs or not. If battle does occur, following steps occur:
+Your tank itself takes no specific action as the Advancing Fire is considered the effort of the entire task force including your tank. However, ammo is expended by your tank whether a battle occurs or not. If battle does occur, following steps occur:
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advancing Fire Ammo Use &lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advancing Fire Markers&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advancing Fire Resolution</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r22.11 Advancing Fire Ammo Use&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark off 1D/2 (round down) HE rounds and .30 caliber MG ammo boxes regardless of whether the battle occurs or not. Mark off on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+    <t>&lt;Bold&gt;r22.12 Advancing Fire Markers&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place up to six Advance Fire markers anywhere on the Battle Board except in Sectors 1, 2, 3, and the long range sectors 6-8. You may place more than one in a zone. For every 3 friendly tank losses (roudned up), omit one Advance Fire marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r23.0 Artillery Support and Air Strikes&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Artillery Support &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; AirStrikes&lt;LineBreak/&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r22.2 Advancing Fire - Entering a New Area&lt;/Bold&gt;
@@ -1165,7 +1271,10 @@
 You may fire your tank's MGs into zones containing no spotted units as a type of Advancing Fire. Order correct crew action (for example, Fire Bow MG) and place the Advancing Fire marker for the MG (Bow MG Advance Fire) into the zone you want to fire. Place the marker after any tank movement or facing changes. This type of fire can KO enemy units which move into the zone and reduce the danger of Panzerfaust attacks per the
 &lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attack Tables.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- During the Crew Action Phase, roll 2D:  (1-30 =  1 ammo box expected), (31-97 =  nothing), and (98-100 = MG malfunctions). 
+-- During the Crew Action Phase, roll 2D:  &lt;LineBreak/&gt;
+    1-30 =  1 ammo box expected&lt;LineBreak/&gt;
+    31-97 =  nothing&lt;LineBreak/&gt;
+    98-100 = MG malfunctions 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 -- Each enemy truck or infantry type that enters the zone may be immediately fired on by your MG according to the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -1175,118 +1284,20 @@
 -- Remove these Advancing Fire markers specific for your MGs at the beginning of the Orders Phase 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; of the next round
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c42FireBowMg'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r22.13 Advancing Fire Resolution&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Advancing Fire is resolved in each Battle Board zone containing both an Advance Fire marker and enemy units during Battle Step 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.64' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-For each, roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table against each unit in the zone. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units kocked out are considered to be withdrawing and are not destroyed. No victory points are awarded. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Remove the Advancing Fire markers from the Battle Board after resolving.</t>
-  </si>
-  <si>
-    <t>r23.0</t>
-  </si>
-  <si>
-    <t>r23.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r23.0 Artillery Support and Air Strikes&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Artillery Support &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; AirStrikes&lt;LineBreak/&gt;
-</t>
-  </si>
-  <si>
-    <t>r23.2</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r23.1 Artillery Support&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Artillery support can be called for during the Movement Sequence 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-This operation takes 15 minutes. Mark off the time and rol 1D as shown on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Use Table to see if the support arrives. It arrives on 1-7 roll. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If successful, place an Artillery Support marker in the area where the artillery landed. If at any time during this day you enter the marked area (before reaching the exit area), the artillery support will attack all enemy units appearing. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Additional artillery support may be called for, but no more than three support markers may be on the Movement Board at one time. You may voluntarily pick up an Artillery Support marker if you decide to attempt to place it elsewhere.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Artillery support takes effect in a newly entered area immediately after any appearing enemy units are placed on the Battle Board. Rsolve Arillery Support by rolling on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table against each enemy unit.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units destroyed by artillery support are immediately removed, and their victory points ar recorded under friendly forces of the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll again against each surviving enemy unit for each additional support marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c42FireBowMg'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r23.2 Air Strike&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Air Strikes function very similarly to artillery support
+Air Strikes function very similarly to artillery support 
 &lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; with a few exceptions. 
 They use more time (30 minutes). They are less likely to arrive (1D = 1-4). They are more effective against armor targets. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Also, air strikes may not be called for during overcast or falling snow weather. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-While the 30 minutes spent calling for air strike is passing, youuu may perform one additional 15 minute operation (such as call for arilltery support or chek an additional area for resistance.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c40AirSupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r22.12 Advancing Fire Markers&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Place up to six Advance Fire markers anywhere on the Battle Board except in Sectors 1, 2, 3, and the long range sectors 6-8. You may place more than one in a zone. For every 3 friendly tank losses (roudned up), omit one Advance Fire marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                                  &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.51 Mark Start Area&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Around the edge of the Movement Board, there are 10 areas number 1-10. Roll 1D to determine which of the ten is the start area for this scenario. Also, mark the area with a Start Area marker.
-Place the Task Force marker representing your friendly forces on that area.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                    &lt;InlineUIContainer&gt;&lt;Image Name='c33StartArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;           
-      &lt;InlineUIContainer&gt;&lt;Image Name='c35TaskForce'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r4.52 Mark Exit Area&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-On the &lt;InlineUIContainer&gt;&lt;Button Content='Exit Areas' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table, roll 1D and cross reference the number with the Start Area marker 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-Mark the area with the Exit Area marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Name='c34ExitArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r4.54.2  Call for Artillery Support&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Call to hit an area adjacent to your task force. Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if Artillery Support arrives 
-&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-If successful, place an Artillery Support marker on the area. Three Artillery Support markers are allowed and can be placed in the same area. Continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.54.3  Call for Air Strike&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Call to hit an area adjacent to your task force. Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if Air Strike arrives
- &lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  If successful, place an Air Strike marker on the area. Two Air Strike markers are allowed and can be placed in the same area. Additionally, while waiting for air strike, a 15 minute operation can be chosen to happen in parallel. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+While the 30 minutes spent calling for air strike is passing, you may perform one additional 15 minute operation (such as call for arilltery support or check an additional area for resistance).
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c40AirStrike'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -1659,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B202"/>
+  <dimension ref="A1:B203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1852,7 +1863,7 @@
         <v>145</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -1860,7 +1871,7 @@
         <v>146</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -1892,7 +1903,7 @@
         <v>150</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -1900,7 +1911,7 @@
         <v>151</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -2244,7 +2255,7 @@
         <v>75</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2375,12 +2386,12 @@
         <v>170</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>171</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -2388,72 +2399,80 @@
         <v>172</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>173</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="B96" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="4"/>
-    </row>
-    <row r="202" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+    </row>
+    <row r="203" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A130:B305">
-    <sortCondition ref="A130:A305"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A131:B306">
+    <sortCondition ref="A131:A306"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add rule seciton 12.0
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76CD8AB3-551D-46F7-ABEB-5A6244E23654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0D479F14-75EA-4985-A3D0-08921A6B2A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
   <si>
     <t>r20.1</t>
   </si>
@@ -564,19 +564,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Ammo Ready Rack</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r16.0 Ammunition (Ammo)&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Ammo is loaded into your tank at the beginning of each scenerio as part of morning briefing 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Each model and variant of the Sherman tank has a limit on its normal load and ammo, both for its man gun and MGs as shown on it Tank Card 
-.  
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.0a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Details&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Ammo Types&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Loading Ammo</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r16.0a Ammo Details&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 -- Both the 75 and 76L fired AP and HE rounds. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -1211,13 +1198,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advancing Fire Resolution</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r22.12 Advancing Fire Markers&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Place up to six Advance Fire markers anywhere on the Battle Board except in Sectors 1, 2, 3, and the long range sectors 6-8. You may place more than one in a zone. For every 3 friendly tank losses (roudned up), omit one Advance Fire marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r23.0 Artillery Support and Air Strikes&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Artillery Support &lt;LineBreak/&gt;
@@ -1771,6 +1751,253 @@
   </si>
   <si>
     <t>r4.65</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r22.12 Advancing Fire Markers&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place up to six Advance Fire markers anywhere on the Battle Board except in Sectors 1, 2, 3, and the long range sectors 6-8. You may place more than one in a zone. For every 3 friendly tank losses (rounded up), omit one Advance Fire marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c44AdvanceFire'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r12.0</t>
+  </si>
+  <si>
+    <t>r12.1</t>
+  </si>
+  <si>
+    <t>r12.11</t>
+  </si>
+  <si>
+    <t>r12.12</t>
+  </si>
+  <si>
+    <t>r12.13</t>
+  </si>
+  <si>
+    <t>r12.14</t>
+  </si>
+  <si>
+    <t>r12.15</t>
+  </si>
+  <si>
+    <t>r12.16</t>
+  </si>
+  <si>
+    <t>r12.17</t>
+  </si>
+  <si>
+    <t>r12.18</t>
+  </si>
+  <si>
+    <t>r12.2</t>
+  </si>
+  <si>
+    <t>r12.3</t>
+  </si>
+  <si>
+    <t>r12.31</t>
+  </si>
+  <si>
+    <t>r12.32</t>
+  </si>
+  <si>
+    <t>r12.33</t>
+  </si>
+  <si>
+    <t>r12.34</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.0 Enemy Units&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units of German armed forces engaged by the 4th Armored Division are represented in play by individual vehicles and small weapons teams. They are brought into play when battle is triggered by a roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+The number and type of enemy units appearing is determined by consulting the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Activation' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Description&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Activation&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Placement</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.2 Activation&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When battle is triggered on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Resistance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table, roll for the appearance of enemy units on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Activation' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table. The number of enemy units initially appearing depends on the level of resistance in the area:&lt;LineBreak/&gt;
+  2 = Light&lt;LineBreak/&gt;
+  3 = Medium&lt;LineBreak/&gt;
+  4 = Heavy
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each unit that will appear, roll once on the Activation Table under the column of the scenario type. This roll determines the type of unit that will be placed on the Battle Board.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.31 Sector&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The sector to place a new enemy unit is determined by a 1D roll as explained in 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.3 Placement&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Placing enemy units on the Battle Board consists of up to four steps to determine:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sector&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Range&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Vehicle Facing&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.34' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Target Terrain
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no limit on the number of enemy units that may be placed in the same sector, at the same range, and in the same terrain.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r16.0 Ammunition (Ammo)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ammo is loaded into your tank at the beginning of each scenerio as part of morning briefing 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Each model and variant of the Sherman tank has a limit on its normal load and ammo, both for its man gun and MGs as shown on it Tank Card .  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.0a' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Details&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Ammo Types&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Loading Ammo</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.11 Tanks or Panzerkampfwagen (Pz)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Panzer (armored) + kampf (fighting) + wagen (vehicle) = armored fighting vehicle (AFV). Tanks have turrets and appear in four types: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ -- Pz IV: medium tank&lt;LineBreak/&gt;
+ -- Pz V: Pather medium tank&lt;LineBreak/&gt;
+ -- Pz VIe: Tiger heavy tank&lt;LineBreak/&gt;
+ -- Pz VIb: King Tiger heavy tank
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c79PzIV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c80PzV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c81PzVIe'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c82PzVIb'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.13 Truck&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Any medium truck of the period
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c88Truck' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.14 Panzerspahwagen (PSW)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Armored scout car.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c89Psw232' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.16 Light Weapons (LW)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Light weapons units represent a source of infantry weapons fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c91Lw' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.17 Machine Gun (MG) Team&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Represents the fire of machine gun team.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c92MgTeam' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.18 Antitank (AT)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Pazerabwherkanone (Pak) = tank defense cannon. These represent an AT gun and its crew. AT Guns appear in three types: 50L (PaK38), 75L (PaK40), and 88LL (PaK43).
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+             &lt;InlineUIContainer&gt;&lt;Image Name='c93Pak38'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c94Pak40'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c95Pak43'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.12 Self Propelled Gun (SPG)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+SPGs have no turret and are designed as assault or anti-tnak guns. They appear in five types:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ -- STuG IIIG: Sturmgeschutz = assault - medium assault gun&lt;LineBreak/&gt;
+ -- Marder II: Marder = marten - medium assault gun&lt;LineBreak/&gt;
+ -- Marder III: medium assault gun&lt;LineBreak/&gt;
+ -- JgdPz IV: Jagdpanzer = armored hunter or tank destroyer - medium tank destroyer&lt;LineBreak/&gt;
+ -- JgdPz 38(t): Hetzer = troublemaker - medium tank destroyer
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+  &lt;InlineUIContainer&gt;&lt;Image Name='c83MarderII'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+  &lt;InlineUIContainer&gt;&lt;Image Name='c84MarderIII'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+  &lt;InlineUIContainer&gt;&lt;Image Name='c85STuGIIIg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+  &lt;InlineUIContainer&gt;&lt;Image Name='c86JgdPzIV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+  &lt;InlineUIContainer&gt;&lt;Image Name='c87JgdPz38t'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.15Schutzenpanzerwagen (SPW)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Armored infantry vehicle, i.e., armored personnel carrier.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c90Spw251' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.1 Description&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units appear in two major types: vehicles and infantry. 
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Vehicle types are:&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Tanks&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Self Propelled Guns (SPGs)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Trucks&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Panzerspahwagen (PSW)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.15' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Schutzenpanzerwagen (SPW)&lt;LineBreak/&gt;
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Infantry types are:&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.16' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Light Weapons (LW)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.17' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Muchaine Gun (MG) Team&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.18' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Antitank (AT) Gun
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank, SPG, and AT guns are printed in black on their front side and red on their back side. When these units first appear, place them red side up. They remain on their red side until they are identified by spotting per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                 &lt;InlineUIContainer&gt;&lt;Image Name='c76UnidentifiedAtg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c77UnidentifiedSpg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c78UnidentifiedTank'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.32 Range&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+To determine the range at which the enemy will be placed, roll 1D on Part I of the Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table. Range will depend on the unit type and the type of Movement Board area where the battle is taking place, as well as the die roll.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.33 Vehicle Facing&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D on Part II of the Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine the facing of the enemy vehicles. For front, side, or rear facing; position the front, side or rear of the vehcile counter, respectively toward your Sherman tank counter.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.34 Target Terrain&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D on Part III of the Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to determine the terrain occupied by the enemy unit. The table also indicates if the unit is hulled down or moving in the open. Mark units hall down, in woods, in a fortification, in a building, or moving in the open with the appropriate counter. Units in the open have no marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+       &lt;InlineUIContainer&gt;&lt;Image Name='c14HullDown'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+       &lt;InlineUIContainer&gt;&lt;Image Name='c97TerrainWoods'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+       &lt;InlineUIContainer&gt;&lt;Image Name='c98TerrainFort'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+       &lt;InlineUIContainer&gt;&lt;Image Name='c96TerrainBuilding'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+       &lt;InlineUIContainer&gt;&lt;Image Name='c13Moving'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r14.0</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r14.0 Friendly Action&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Friendly Action represents the firepower of the friendly forces accompanying your vehicle. Roll 2D on the Friendly Action Table for each enemy unit on the Battle Board. Friendly action will result in either no effect, destruction of the enemy unit, or the placement of smoke. Record the destruction of enemy units on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -2143,10 +2370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B230"/>
+  <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2232,7 +2459,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2256,7 +2483,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2264,367 +2491,367 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2632,7 +2859,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2651,581 +2878,717 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B80" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>34</v>
+        <v>110</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B115" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B113" s="3" t="s">
+    <row r="131" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B114" s="3" t="s">
+    <row r="132" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B132" s="3" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B116" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B124" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B126" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B128" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B137" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B133" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="4"/>
-    </row>
-    <row r="230" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="149" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="4"/>
+    </row>
+    <row r="247" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A158:B333">
-    <sortCondition ref="A158:A333"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A175:B350">
+    <sortCondition ref="A175:A350"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added rules for section 8
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0D479F14-75EA-4985-A3D0-08921A6B2A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A3B66FB-1320-42FA-9000-96D461AC08DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
   <si>
     <t>r20.1</t>
   </si>
@@ -608,16 +609,6 @@
   </si>
   <si>
     <t>r4.41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r3.0 Game Tables&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Tables can be viewed by selecting the &lt;Bold&gt;Help | Show Tables...&lt;/Bold&gt; menu.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;The game tables are used by rolling one or two ten-sided dice and reading the results generated by the table. 
-Throughout the game, the notation 1D  means roll one die and 2D means rolling two die. The notation 1D/2 means roll one die and dividing the number by half.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;When rolled together, the colored die is the tens digit and the white die is the ones digit. A roll of '00' represents 100. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;Many tables include additioinal factors that modify the randomly generated number of the dice roll. For example, when rolling on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table, 
-if the repairing crewman has a rating of 5, the roll modifier to repair is -5. </t>
   </si>
   <si>
     <t>r4.42</t>
@@ -1998,6 +1989,417 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Friendly Action represents the firepower of the friendly forces accompanying your vehicle. Roll 2D on the Friendly Action Table for each enemy unit on the Battle Board. Friendly action will result in either no effect, destruction of the enemy unit, or the placement of smoke. Record the destruction of enemy units on the After Action Report 
 &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>r8.0</t>
+  </si>
+  <si>
+    <t>r8.1</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.0 Crew Actions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Commander (C)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Gunner (G)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Loader (L)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Driver (D)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Assistant Driver (A)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Non-Specific Crew Actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r8.11 </t>
+  </si>
+  <si>
+    <t>r8.12</t>
+  </si>
+  <si>
+    <t>r8.2</t>
+  </si>
+  <si>
+    <t>r8.21</t>
+  </si>
+  <si>
+    <t>r8.22</t>
+  </si>
+  <si>
+    <t>r8.23</t>
+  </si>
+  <si>
+    <t>r8.24</t>
+  </si>
+  <si>
+    <t>r8.25</t>
+  </si>
+  <si>
+    <t>r8.3</t>
+  </si>
+  <si>
+    <t>r8.31</t>
+  </si>
+  <si>
+    <t>r8.32</t>
+  </si>
+  <si>
+    <t>r8.33</t>
+  </si>
+  <si>
+    <t>r8.34</t>
+  </si>
+  <si>
+    <t>r8.35</t>
+  </si>
+  <si>
+    <t>r8.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r8.4 </t>
+  </si>
+  <si>
+    <t>r8.41</t>
+  </si>
+  <si>
+    <t>r8.42</t>
+  </si>
+  <si>
+    <t>r8.43</t>
+  </si>
+  <si>
+    <t>r8.44</t>
+  </si>
+  <si>
+    <t>r8.45</t>
+  </si>
+  <si>
+    <t>r8.46</t>
+  </si>
+  <si>
+    <t>r8.5</t>
+  </si>
+  <si>
+    <t>r8.51</t>
+  </si>
+  <si>
+    <t>r8.52</t>
+  </si>
+  <si>
+    <t>r8.53</t>
+  </si>
+  <si>
+    <t>r8.6</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.6 Non-Specific Crew Actions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Throw Smoke Grenades&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.62' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire AA MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.63' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair AA MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.64' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Replace Periscope&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Sub MG</t>
+  </si>
+  <si>
+    <t>r8.61</t>
+  </si>
+  <si>
+    <t>r8.62</t>
+  </si>
+  <si>
+    <t>r8.63</t>
+  </si>
+  <si>
+    <t>r8.64</t>
+  </si>
+  <si>
+    <t>r8.65</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.1 Commander (C)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct Movement&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct Fire
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c07Commander'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.2 Gunner (G)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Main Gun&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Co-Axial MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rotate Turret&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rotate Turret/Fire Main Gun&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.25' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Main Gun
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c11Gunner'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.21 Fire Main Gun&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Subtract gunner&amp;apos;s rating from the To Hit roll for the main gun. Gunner may not spot. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c50GFIreMainGun'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.3 Loader (L)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Load&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Main Gun&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Co-Axial MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.34' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Mortar&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.35' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Change Gun Load&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.36' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Restock Ready Rack
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c09Loader'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.31 Load&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If no marker is placed in the loader&amp;apos;s box, he will automatically reload the main gun if it is fired. Subtract the loader&amp;apos;s rating from the To Hit roll for the main gun. May spot normally unless the main gun is being fired. If the main gun is being fired, the loader may not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c54LLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.35 Change Gun Load&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Change the ammo round in the main gun to any round still available. May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c59LChangeGunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.36 Restock Ready Rack&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Replace rounds in the ready rack from those still available. May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c60LRestockReadyRack'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.4 Driver (D)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Stop&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Forward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Forward to Hull Down&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.44' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Reverse&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Reverse to Hull Down&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Pivot Tank
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c08Driver'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.41 Stop&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If no action marker is placed in the driver&amp;apos;s box, he automatically stops the tank. Remove any previously placed Moving marker from the tank. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c61DStop'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.42 Forward&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank moves forward. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c62DForward'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.43 Forward to Hull Down&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank moves forward looking for a hull down position. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c63DForwardToHullDown'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.44 Reverse&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank moves backward. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c64DReverse'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.45 Reverse to Hull Down&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank moves backward looking for a hull down position. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c65DReverseToHullDown'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.5 Assistant Driver (A)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Bow MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.52' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Bow MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Pass Ammo
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c10Assistant'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.51 Fire Bow MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Subtract the assistant&amp;apos;s rating from To Kill roll for the bow MG. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c67AFireBowMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.53 Pass Ammo&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Assistant Driver passes ammo to speed reload time. Modify the To Hit roll by -10 when determining rate of fire per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+This action cannot be taken when reloading from ready rack 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. May not spot
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c69APassAmmo'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.64 Replace Periscope&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A crewman who has had his periscope knocked out replaces the damaged periscope.  May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c73ReplacePeriscope'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.22 Fire Co-Axial MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Subtract gunner&amp;apos;s rating from the To Kill roll for the co-axial MG. You may continue to spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c51GFireCoaxialMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.23 Rotate Turret&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Turn turret to face any sector. May spot only in the sector of the turret's front facing after rotation per per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                       &lt;InlineUIContainer&gt;&lt;Image Name='c52GRotateTurret'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.32 Repair Main Gun&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunctioning' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Table 
+to repair main gun. May not spot. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c55LRepairMainGun'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r3.0 Game Tables&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Tables can be viewed by selecting the &lt;Bold&gt;Help | Show Tables...&lt;/Bold&gt; menu.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;The game tables are used by rolling one or two ten-sided dice and reading the results generated by the table. 
+Throughout the game, the notation 1D  means roll one die and 2D means rolling two die. The notation 1D/2 means roll one die and dividing the number by half.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;When rolled together, the colored die is the tens digit and the white die is the ones digit. A roll of '00' represents 100. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;Many tables include additioinal factors that modify the randomly generated number of the dice roll. For example, when rolling on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Table, 
+if the repairing crewman has a rating of 5, the roll modifier to repair is -5. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.25 Repair Main Gun&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Subtract the gunner&amp;apos;s rating from roll to repair the main gun on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair 
+Table. Can only be used if the loader is also attempting to repair the main gun per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+You may not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c57GRepairMainGun'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.33 Repair Co-Axial MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunctioning' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Table 
+to repair malfunctioning co-axial MG. May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c55LRepairMainGun'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.34 Fire Mortar&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Firing the 2 inch smoke mortar places a smoke marker in close zone to the turret&amp;apos;s front. Also automatically reloads the mortar if smoke bombs are still available. May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c58LFireMortar'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.65 Fire Sub MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Commander (or loader in tanks other than those with a &amp;quot;A&amp;quot; turret) fires a .50 calibre submachine gun. The gun is fired as either Advancing Fire into an empty zone or 
+as direct fire against an enemy unit. Subtract rating from the To Kill roll. Crewman must fire from an open hatch. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c74FireSubMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.62 Fire AA MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Commander (or loader in tanks with a split loader hatch and AA MG mount) subtracts rating from the To Kill roll for the AA MG. Crewman must have an open hatch. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c71FireAaMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.63 Repair AA MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Commander (or loader in tanks with a split loader hatch and AA MG mount) rolls on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Table . He may not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c72RepairAaMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.61 Throw Smoke Grenades&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Either the commander or gunner may throw smoke grenades from their open hatch. Grenades must be available as shown on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContaine. Place a smoke marker on the tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c70ThrowSmokeGrenade'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.52 Repair Bow MG&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Table 
+to repair the malfunctioning bow MG. May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c68ARepairBowMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.46 Pivot Tank&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank may change facing to any sector. Pivoting tank loses hull down position. He may spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c66DPivotTank'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.24 Rotate Turret/Fire Main Gun&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Turn turret to face any sector and fire main gun with a penalty per 
+&lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table, i.e., +10 per sector rotated. 
+May not spot.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c53GRotateTurretFireMainGun'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.11 Direct Movement&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Direct the movement of the tank. This will reduce the chance of an accident per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Movement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+However, the commander have no effect on any fire. You may continue to spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c48CDirectMove'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.12 Direct Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Direct the fire of the main gun or any one machine gun. Subtract the commander&amp;apos;s crew rating from the To Hit roll on the
+&lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+for the main gun fire or the To Kill roll for the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. You may continue to spot per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c49CDirectFire'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2370,10 +2772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B247"/>
+  <dimension ref="A1:B281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2459,7 +2861,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>97</v>
+        <v>355</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2483,7 +2885,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2499,7 +2901,7 @@
         <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2507,351 +2909,351 @@
         <v>96</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2859,7 +3261,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2878,717 +3280,989 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>265</v>
+        <v>299</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>267</v>
+        <v>302</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>268</v>
+        <v>303</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>269</v>
+        <v>304</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>287</v>
+        <v>336</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>271</v>
+        <v>306</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>272</v>
+        <v>307</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>273</v>
+        <v>308</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>276</v>
+        <v>311</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>277</v>
+        <v>312</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>278</v>
+        <v>313</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>295</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>279</v>
+        <v>314</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>280</v>
+        <v>315</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>297</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>299</v>
+        <v>341</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>81</v>
+        <v>317</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>82</v>
+        <v>318</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>83</v>
+        <v>319</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>84</v>
+        <v>320</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>86</v>
+        <v>321</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>87</v>
+        <v>322</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>88</v>
+        <v>323</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>107</v>
+        <v>324</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>108</v>
+        <v>325</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>109</v>
+        <v>326</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>110</v>
+        <v>327</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>111</v>
+        <v>328</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>112</v>
+        <v>330</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>113</v>
+        <v>331</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>114</v>
+        <v>332</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>123</v>
+        <v>361</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+      <c r="B130" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
+    <row r="132" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+    <row r="133" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B133" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B99" s="2" t="s">
+    <row r="134" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+      <c r="B134" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B135" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B101" s="2" t="s">
+      <c r="B136" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+      <c r="B137" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+    </row>
+    <row r="138" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B138" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+    <row r="139" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="140" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
+    <row r="141" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+    <row r="142" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B142" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
+    <row r="143" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+    <row r="144" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
+    <row r="145" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
+    <row r="146" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B146" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
+    <row r="149" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B149" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B164" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B117" s="2" t="s">
+    <row r="165" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="B170" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B135" s="3" t="s">
+      <c r="B173" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B174" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B139" s="3" t="s">
+    <row r="175" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B177" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+    <row r="178" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B179" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B181" s="3" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B146" s="3" t="s">
+    <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B184" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B148" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B150" s="3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="4"/>
-    </row>
-    <row r="247" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202" s="4"/>
+    </row>
+    <row r="281" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A175:B350">
-    <sortCondition ref="A175:A350"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A209:B384">
+    <sortCondition ref="A209:A384"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Section 9 to rules
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A3B66FB-1320-42FA-9000-96D461AC08DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2D5F3FB1-F0AB-4B29-95CA-8E768A7DB1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="406">
   <si>
     <t>r20.1</t>
   </si>
@@ -1195,27 +1194,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; AirStrikes&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r22.2 Advancing Fire - Entering a New Area&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-You may fire your tank's MGs into zones containing no spotted units as a type of Advancing Fire. Order correct crew action (for example, Fire Bow MG) and place the Advancing Fire marker for the MG (Bow MG Advance Fire) into the zone you want to fire. Place the marker after any tank movement or facing changes. This type of fire can KO enemy units which move into the zone and reduce the danger of Panzerfaust attacks per the
-&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attack Tables.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- During the Crew Action Phase, roll 2D:  &lt;LineBreak/&gt;
-    1-30 =  1 ammo box expected&lt;LineBreak/&gt;
-    31-97 =  nothing&lt;LineBreak/&gt;
-    98-100 = MG malfunctions 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- Each enemy truck or infantry type that enters the zone may be immediately fired on by your MG according to the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-vs. Infantry Targets Table. Any kills are recorded as victory points on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
--- Remove these Advancing Fire markers specific for your MGs at the beginning of the Orders Phase 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; of the next round
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='c42FireBowMg'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r23.2 Air Strike&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Air Strikes function very similarly to artillery support 
@@ -1597,16 +1575,6 @@
 The driver and loader automatically perform the actions Stop and Load, respectively, unless ordered otherwise.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c59LChangeGunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r5.23 Gun Loads&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In the gun load section, place the Gun Load marker in the box of the ammo round loaded in the gun. Also markhere what round type you want to reload after firing (ammo reload marker), and whether you will draw reloads from the ready rack (ready rack ammo reload marker) per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                 &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c29AmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c30ReadyRackAmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r5.11 Battle Area&lt;/Bold&gt;
@@ -2400,6 +2368,303 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c49CDirectFire'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r9.0</t>
+  </si>
+  <si>
+    <t>r9.1</t>
+  </si>
+  <si>
+    <t>r9.2</t>
+  </si>
+  <si>
+    <t>r9.3</t>
+  </si>
+  <si>
+    <t>r9.31</t>
+  </si>
+  <si>
+    <t>r9.32</t>
+  </si>
+  <si>
+    <t>r9.33</t>
+  </si>
+  <si>
+    <t>r9.34</t>
+  </si>
+  <si>
+    <t>r9.4</t>
+  </si>
+  <si>
+    <t>r9.41</t>
+  </si>
+  <si>
+    <t>r9.42</t>
+  </si>
+  <si>
+    <t>r9.5</t>
+  </si>
+  <si>
+    <t>r9.51</t>
+  </si>
+  <si>
+    <t>r9.52</t>
+  </si>
+  <si>
+    <t>r9.53</t>
+  </si>
+  <si>
+    <t>r9.6</t>
+  </si>
+  <si>
+    <t>r9.35</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.2 Direct or Area Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Direct Fire represents aiming a shot at a specific target. Area Fire represents shooting into a general area. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+All AP and HVAP shots must use Direct Fire or they have no effect. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+WP and HCBI shots must use Area Fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+HE ammo can use either Direct or Area Fire.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.31 To Hit Table&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine whether the target fired on is hit by consulting the correct row on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The correct row will depend on the type of gun you have (75 or 76L), the type of target (infantry or vheicle), the type of ammo fired, and whether you are using Direct Fire or Area Fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At the top of the table are shown the basic To Hit numbers for each type of fire. You must roll the number shown or less on 2D (after modifications) to score a hit.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.3 Hitting the Target&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; To Hit Table&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; To Hit Modifiers&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Marking Target&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.34' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rate of Fire Roll&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.35' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Target Acquisition&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r5.23 Gun Loads&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In the gun load section, place the Gun Load marker in the box of the ammo round loaded in the gun. Also markhere what round type you want to reload after firing (ammo reload marker), and whether you will draw reloads from the ready rack (ready rack ammo reload marker) per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
++B93     &lt;InlineUIContainer&gt;&lt;Image Name='c30ReadyRackAmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.33 Marking Target&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If a hit is core with AP or HE ammo, mark the target with an appropriate Hit marker. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the target is hit with a smoke round, place a Smoke marker in the zone.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                 &lt;InlineUIContainer&gt;&lt;Image Name='c100ApHit'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c101HeHit'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c102SmokeHit'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.4 Rate of Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Achieving Rate of Fire allows for your crew to immediately fire another shot from the main gun. When a To Hit roll is made firing the main gun, the number rolled also deteremines whether the gun has acheived Rate of Fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the roll is low enough (30 or less for a 75mm gun and 20 or less for a 76L mm gun), you may immediately elect to fire again. You can continue to fire again until either the Rate of Fire roll is not acheived or the ammo runs out.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rate of Fire Modifiers&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Successive Rate of Fire</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.41 Rate of Fire Modifiers&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The 
+&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table details a number of modifiers that may affect the number needed to achieve the Rate of Fire. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+These modifiers affect only the Rate of Fire roll and have no effect on the To Hit dice roll.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.42 Successive Rate of Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Successive Rate of Fire shots must be fired at the original target even though you do not know the results of previous hits. You may not switch targets during a round.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.5 Killing the Target&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit against a target, consult one of the To Kill tables. The correct table is used to determine if the target is knocked out (KO&amp;apos;s).
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.51' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; HE versus Infantry Targets&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.52' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; AP vs Vehicles&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.53' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; HE versus Vehicles</t>
+  </si>
+  <si>
+    <t>r9.61</t>
+  </si>
+  <si>
+    <t>r9.62</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.0 Sherman Main Gun Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The American versions of the Sherman tank available for play are armed with one of two types of main gun: either a 75mm or 76mm gun. The &amp;quot;L&amp;quot; denotes improved long range capability. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Main gun is directed to fire by placing either a Fire Main Gun or Ratate and Fire marker in the gunner&amp;apos;s box on the Tank Card. The gun cannot be fired if it is not loaded or is malfunctioning. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Resolution of a shot from the main gun requires five steps: 1.) Selecting eligible target 2.) Selecting Direct Fire or Area Fire 3.) Hitting the target 4.) For vehicle targets only, determining where the target was hit, and 5.) Determining if the target is destroyed. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+However, you do not see the results of any hits until you have finished firing.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Selecting a Target&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct or Area Fire&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Hitting the Target&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rate of Fire&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Killing the Target&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Ammo Loads and Reloads</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.1 Selecting a Target&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only those enemy units that have been spotted per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; may be fired on. 
+The main gun may only fire at a target in the sector to the turret&amp;apos;s front. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+By ordering the gunner to rotate and fire, the turret may be swung up to any sector and still fire but at a penalty per 
+&lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The gun may be fired at targets at any range. The effectiveness of fire drops at longer ranges. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The main gun may be fired at only one unit per battle round, regardless of how many Rate of Fire shots are taken. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Infantry targets are LW, MG, and AT guns. All other enemy units are vehicles.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.32 To Hit Modifiers&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At the bottom of the table are shown various factors that may modify the number rolled upward or downward. Smoke and certain types of weather on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Weather' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table may half the basic To Hit number several times before any modifications.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.34 Rate of Fire Roll&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you achieve a Rate of Fire with your To Hit roll, you may immediately fire again per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+If your roll To Hit does not achieve a Rate of Fire, your firing is finished for this round.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.35 Target Acquisition&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+After your first shot at a target, place an &amp;quot;Acquired Target 1&amp;quot; marker on it. Place an &amp;quot;Acquired Target 2&amp;quot; marker on a target that already has one if you shoot a second time. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Acquired target modifiers to the To Hit dice rolls apply only to targets marked with the acquired markers. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only one target at a time may be acquired by your tank. Acquired markers are removed if your tank moves or pivots unless your crew has a gyrostablizer per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Additionally, the marker is removed if your turret rotates away from the target&amp;apos;s zone or if you fire at a different target.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                           &lt;InlineUIContainer&gt;&lt;Image Name='c103Acquired1'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c104Acquired2'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.52 AP vs Vehicles&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit against a target, consult one of the corresponding tables: 
+&lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (75)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
+&lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (76)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+All tables show a number for each type of enemy vehicle target for three different facings (front, side, and rear), three different ranges (close, medium, and long), and in some cases for both turrent or hull hits.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Where different numbers are shown for turret and hull hits, roll 1D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Hit Location Tank' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table to determine where the shell hits.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the number rolled is less than or equal to the number shown on the table, the target is KO&amp;apos;ed.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.51 HE versus Infantry Targets&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Both Area and Direct Fire versus infantry targets by 75 or 76L guns is resolved on the same 
+&lt;InlineUIContainer&gt;&lt;Button Content='To Kill Infantry' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At the top of the table are listed the base numbers which must be rolled To Kill the target. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+At the buttom of the table are listed factors which may modify the number rolled.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.53 HE versus Vehicles&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For each hit against a target, consult one of the corresponding tables: 
+&lt;InlineUIContainer&gt;&lt;Button Content='HE To Kill (75)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; or 
+&lt;InlineUIContainer&gt;&lt;Button Content='HE To Kill (76)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In general, HE is not an effective weapon against vehicles, but it can kill those with light armor and trucks. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+All tables show a number for each type of enemy vehicle target for three different facings (front, side, and rear), three different ranges (close, medium, and long), and in some cases for both turrent or hull hits.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Where different numbers are shown for turret and hull hits, roll 1D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Hit Location Tank' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table to determine where the shell hits.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.6 Ammo Loads and Reloads&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.61' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; First Ammo Load&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.62' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Ammo Reload</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.61 First Ammo Load&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the Prepare for Battle step of the Sequence of Play 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+, you have the opportunity to choose an ammo load for your main gun. When the battle round sequence begins, this is the type of ammo in your gun and what you will fire with your first shot. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you elect to leave your gun unloaded, you may not fire in the first battle round, but you may load the gun as you choose preparing for the second round. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you choose to use Advancing Fire when entering a new area, you must load your gun with HE. Mark the ammo load by placing the Gun Load marker in the correct ammo box on the Tank Card. Only those ammo types listed on the Tank Card can be loaded and fired from your gun. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.62 Ammo Reload&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+fo the Battle Round Sequence, you must mark what type of ammo you want reloaded if you are firing your main gun. If you acheive Rate of Fire 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+and wish to continue firing, your additional shots will all be the type of ammo selected as your reload.  
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During this step, also mark whether you want to draw ammo from your ready rack. Doing so increases your chance of achieving Rate of Fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ammo is marked off as used only after being fired. Loading ammo into the gun does not use it as it is possible to change gun loads. Place the Gun Reload marker (and Ready Rack Ammo Reload marker if desired) in the Gun Load section of the Tank Card.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you choose to use Advancing Fire 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+ when entering a new area, you must load your gun with HE. Mark the ammo load by placing the Gun Load marker in the correct ammo box on the Tank Card. Only those ammo types listed on the Tank Card can be loaded and fired from your gun. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c29AmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r22.2 Advancing Fire - Entering a New Area&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+You may fire your tank's MGs into zones containing no spotted units as a type of Advancing Fire. Order correct crew action (for example, Fire Bow MG) and place the Advancing Fire marker for the MG (Bow MG Advance Fire) into the zone you want to fire. Place the marker after any tank movement or facing changes. This type of fire can KO enemy units which move into the zone and reduce the danger of Panzerfaust attacks per the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attack Tables.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+-- During the Crew Action Phase, roll 2D:  &lt;LineBreak/&gt;
+    1-30 =  1 ammo box expected&lt;LineBreak/&gt;
+    31-97 =  nothing&lt;LineBreak/&gt;
+    98-100 = MG malfunctions 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+-- Each enemy truck or infantry type that enters the zone may be immediately fired on by your MG according to the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+vs. Infantry Targets Table. Any kills are recorded as victory points on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+-- Remove these Advancing Fire markers specific for your MGs at the beginning of the Orders Phase 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; of the next round
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c42FireBowMg'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -2772,10 +3037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B281"/>
+  <dimension ref="A1:B300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,7 +3126,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -2901,7 +3166,7 @@
         <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -2981,7 +3246,7 @@
         <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -3029,231 +3294,231 @@
         <v>150</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>238</v>
-      </c>
       <c r="B53" s="2" t="s">
-        <v>245</v>
+        <v>386</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3282,987 +3547,1139 @@
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>264</v>
+        <v>366</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>265</v>
+        <v>367</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>266</v>
+        <v>368</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>267</v>
+        <v>369</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>268</v>
+        <v>370</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>269</v>
+        <v>371</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>270</v>
+        <v>372</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>292</v>
+        <v>387</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>271</v>
+        <v>373</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>272</v>
+        <v>382</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>273</v>
+        <v>374</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>274</v>
+        <v>375</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>275</v>
+        <v>376</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>276</v>
+        <v>377</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>277</v>
+        <v>378</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>278</v>
+        <v>379</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>295</v>
+        <v>399</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>279</v>
+        <v>380</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>297</v>
+        <v>381</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>81</v>
+        <v>392</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>106</v>
+        <v>267</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>107</v>
+        <v>268</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>139</v>
+        <v>290</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>108</v>
+        <v>269</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>120</v>
+        <v>286</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>109</v>
+        <v>270</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>110</v>
+        <v>271</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>111</v>
+        <v>272</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>112</v>
+        <v>273</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>113</v>
+        <v>274</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>122</v>
+        <v>280</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
+    <row r="149" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+    <row r="150" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B150" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
+    <row r="151" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B151" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
+    <row r="152" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
+    <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
+    <row r="154" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B154" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
+    <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
+    <row r="156" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
+    <row r="157" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
+    <row r="158" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
+    <row r="159" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
+    <row r="160" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
+    <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B161" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
+    <row r="162" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
+    <row r="163" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
+    <row r="164" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B164" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
+    <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B165" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
+    <row r="166" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
+    <row r="167" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B167" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
+    <row r="168" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
+    <row r="169" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B169" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
+    <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B170" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
+    <row r="171" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B171" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
+    <row r="172" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B172" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
+    <row r="173" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B173" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
+    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B174" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
+    <row r="175" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B175" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
+    <row r="176" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B176" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
+    <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
+    <row r="178" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B178" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
+    <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B179" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
+    <row r="180" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B180" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
+    <row r="181" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B181" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
+    <row r="182" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B182" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
+    <row r="183" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B164" s="3" t="s">
+      <c r="B183" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
+    <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B165" s="3" t="s">
+      <c r="B184" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
+    <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B166" s="3" t="s">
+      <c r="B185" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
+    <row r="186" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="B186" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
+    <row r="187" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B187" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
+    <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B169" s="3" t="s">
+      <c r="B188" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A170" s="1" t="s">
+    <row r="189" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B170" s="3" t="s">
+      <c r="B189" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A171" s="1" t="s">
+    <row r="190" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B171" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
+      <c r="B190" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B172" s="3" t="s">
+      <c r="B191" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A173" s="1" t="s">
+    <row r="192" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B173" s="3" t="s">
+      <c r="B192" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B196" s="3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A174" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A175" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A176" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A177" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A178" s="1" t="s">
+    <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B178" s="3" t="s">
+      <c r="B198" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B200" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A179" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A180" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B180" s="3" t="s">
+    <row r="201" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B203" s="3" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A181" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B181" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A182" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B182" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B202" s="4"/>
-    </row>
-    <row r="281" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B221" s="4"/>
+    </row>
+    <row r="300" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A209:B384">
-    <sortCondition ref="A209:A384"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A228:B403">
+    <sortCondition ref="A228:A403"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished adding Section 11 to rules
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2D5F3FB1-F0AB-4B29-95CA-8E768A7DB1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2483724E-F741-4672-96B8-D6A1AC8AF80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="442">
   <si>
     <t>r20.1</t>
   </si>
@@ -331,15 +331,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sequence of Play
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Additional Rules can be viewed by selecting the &lt;Bold&gt;Help | Show Rules..."&lt;/Bold&gt; menu.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r2.12 Battle Board&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The battle board is an abstract display used to resolve engagements with enemy forces. Your tank is placed in the center of this display and the action of an engagement revolves 
-around it through the use of pieces representing enemy units and other informational markers. A detailed explanation is given in 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                 &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r19.11 Exploding Tank&lt;/Bold&gt; 
@@ -1371,13 +1362,6 @@
 -- WWII Victory Medal&lt;LineBreak/&gt;
 &lt;LineBreak/&gt;
 - Purple Hearts are awarded for each wound recieved in combat. The European Campaign Medal is automatically awarded for playing the game. The WWII Victory Medal is automatically awarded after May of 1945.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.91  Rating Improvements&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll for rating improvements for each surviving crew member. Roll 1D for each crew member. If the number rolled is higher than the crew member's current rating, his rating is improved by one. If the number is less than or equal to his current rating, there is no change. See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r7.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-for details about crew ratings.</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r4.92  Total Victory Points&lt;/Bold&gt;
@@ -2665,6 +2649,272 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; of the next round
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                         &lt;InlineUIContainer&gt;&lt;Image Name='c42FireBowMg'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r13.0</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.0 Enemy Action &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>r10.0</t>
+  </si>
+  <si>
+    <t>r11.0</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.0 Sherman Machine Guns (MGs)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Description&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Firing Machine Guns</t>
+  </si>
+  <si>
+    <t>r10.1</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.1 Description&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In addition to its main gun, the Sherman tank is armed with several machine guns (MGs). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .30 calibre bow MG is mounted in the front right hull and is fired by the assistant driver.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .30 calibre co-axial MG is mounted in the turret front along teh same axis as the main gun and is fired by the gunner.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .50 calibre anti-aircraft (AA) MG is fixed to a pintle mount (post) on top of the turret and is fired by the commander. In some configurations, it can be fired by the loader.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Several hand held submachine guns (sub MGs) are carried in the turret and may be fired from open hatches.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c51FireCoaxialMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>r10.2</t>
+  </si>
+  <si>
+    <t>r10.21</t>
+  </si>
+  <si>
+    <t>r10.22</t>
+  </si>
+  <si>
+    <t>r10.23</t>
+  </si>
+  <si>
+    <t>r10.24</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.21 Crew Actions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+MGs are directed to fire by placing a Crew Action marker on the operating crew member&amp;apos;s box on the Tank Card. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, if you want the co-axial MG to fire, place the Fire Co-Axial MG marker in the gunner&amp;apos;s box.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.23 MG Targets&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Machine guns are only effective against the following targets: LW, MG teams, trucks, and AT guns.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+They have no effect against other enemy units.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.2 Firing Machine Guns (MGs)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Description&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; MG Restrictions&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; MG Targets&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; MG Zones</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.22 MG Restrictions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Only those enemy units that have been spotted may be fired on. The co-axial MG may only fire at a target in the sector to the turret&amp;apos;s front. The bow MG may only fire into the sector to the tank&amp;apos;s front. The AA MG or a sub MG may be fired into any sector, but the firing crewman must operate it from an open hatch. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Any weapon may be fired at any range although the effectiveness of the MG fire drops at longer range. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When your tank is hulled down, the bow MG may not fire. Only one enemy unit may be fired at by each MG per battle round unless the MG is performing Advancing Fire per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.24' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>r11.1</t>
+  </si>
+  <si>
+    <t>r11.2</t>
+  </si>
+  <si>
+    <t>r11.3</t>
+  </si>
+  <si>
+    <t>r11.11</t>
+  </si>
+  <si>
+    <t>r11.12</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r2.12 Battle Board&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The battle board is an abstract display used to resolve engagements with enemy forces. Your tank is placed in the center of this display and the action of an engagement revolves 
+around it through the use of pieces representing enemy units and other informational markers. A detailed explanation is given in 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;B126
+                 &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.0 Sherman Movement&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Movement by your tank on the Battle Board is represented by you ordering one of the following crew actions: Forward, Forward to Hull Down, Reverse, or Reverse to Hull Down. However, due to the abstraction of the Battle Board system of sectors and zones radiating out from the hub your tank occupies, your tank never moves anywhere. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Instead, what actually happens is that enemy units shift their positions on the Battle Board relative to your tank&amp;apos;s position. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, assume your tank is facing a sector containing an enemy tank at long range. If you order &amp;quot;Forward&amp;quot;, the enemy unit tank changes from long range to the medium range zone and your tank remains where it is located in the center. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The four tank movement crew actions are resolved by refering to the two part 
+&lt;InlineUIContainer&gt;&lt;Button Content='Movement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table and rolling 2D. 
+The Part I of this table determines the effect of movement on your tank. The Part II determines the effect, if any, on the position and facing of enemy units.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Effect on your Tank&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Effect on Enemy Unit&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Leaving the Battle Area</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.11 Throwing a Track&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A tank with a thrown track may not move or pivot for the remainder of the battle. Your tank sits where it is until it is knocked out or until all enemy units withdraw or are eliminated.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the Battle Board is cleared of enemy units, the day of combat is finished for your tank. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The crew of a disabled tank may abandon the vehicle, but each man must roll once on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table while making his escape. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Go to Evening Debriefing 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c106ThrownTrack'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.12 Bogging Down&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A bogged down tank may not move or pivot until it freed itself. A bogged down tank attempts to free itself by ordering Reverse movement and rolling 2D on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Bogged Down' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Movement Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the result &amp;quot;Assistant Required&amp;quot; is rolled, the tank may not move or pivot or roll again on the table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When the battle ends, your tank is assumed to be freed with the help of friendly forces and play continues normally.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c105BoggedDown'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.24 MG Zones&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+MGs may also be fired into zones that contain no suitable MG targets. This is a type of Advancing Fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark the area with the correct Advancing Fire marker for that MG and roll for the gun malfunction and ammo use. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If enemy units move into the zone during the Enemy Action Phase per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+roll normally to see iif the MG fire KO&amp;apos;s them. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Advancing Fire in a zone will also reduce the chance and effectiveness of a Panzerfaust attack originating from that zone per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r11.1 Effect on your Tank&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ordering movement can result in no effect or one of the three possible states:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Throwing a Track&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Bogging Down&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Hulled Down&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Determine what occurs by rolling 2D on Part I of the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Movement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Find the number rolled under the movement action you ordered and read along the row of the number to the left to find the result. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The number rolled is modifed by the ratings of the driver and possible the commander, as well as weather conditions. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.91  Rating Improvements&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for rating improvements for each surviving crew member. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D for each crew member. If the number rolled is higher than the crew member's current rating, his rating is improved by one. If the number is less than or equal to his current rating, there is no change. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r7.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+for details about crew ratings.</t>
+  </si>
+  <si>
+    <t>r11.31</t>
+  </si>
+  <si>
+    <t>r11.32</t>
+  </si>
+  <si>
+    <t>r11.33</t>
+  </si>
+  <si>
+    <t>r11.34</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.31 Retreat&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A retreat occurs when your tank faces either Sector 1, 2, or 3 and moves forward, or faces one of the other three sectors and moves backward. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An advance occurs when your tank faces either Sector 4-5, 6-8, or 9-10 and moves forward, or faces one of the other three sectors and moves backwards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r11.2 Effect on Enemy Units&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The unmodified number rolled on the white die for the roll on Part I determines the effect of movement on the positioning of enemy units.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Find the number rolled along the left side of the table and read across to the column under the movement action ordered. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Depending on whether you were moving forward or reverse, enemy units may move towards you, away from you, remain in place and change facing, or remain unchanged. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Movement of enemy units on the Battle Board take place according to the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Move Diagram' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  If an enemy vehicle is required to change facing, roll on the Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table, Part II (Vehicle Facing), to see if the vehicle&amp;apos;s facing changes. It is possible the facing will not change. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.32 Enemy Moved Off Board&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you leave an engagement, place the enemy units that were still in play up to the moment of your leaving in the area on the Movement Board where the engagement took place. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you reenter that area again before reaching your exit area, another engagement is automatically triggered, and the remaining units are added to those units that are activated normally.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.33 Reentering Area&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you retreat from an engagement, your task force returns to the area which you last occupied. If you advance out of an engagement by moving forward, place your Task Force marker in any area adjacent to the one you left, except the area from which you entered it. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Leaving an engagement uses up the time that would have normally been expended to move into the new area.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.3 Leaving the Battle Board&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+It is possible for your tank and the accompanying friendly forces to leave the Battle Board before an engagement is finished. This event can be triggered by your tank moving either forward or backward. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Your task force is assumed to have left the Battle Board when movement by your tank causes all enemy units on the display to shift from from a long range zone off the board. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For example, assume the only enemy units in play are in the long range zone of Sector 6-8 (the sector your tank is facing) and you order reverse movement.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the effect of your movement is for the enemy units to move back off the board, your task force is considered to have instead retreated. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Retreat&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Moved Off Board&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Reentering Area&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.34' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advancing to New Area</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.34 Advancing to New Area&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you enter a new area not marked by a US Control marker, go back to step 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, Prepare for Battle, and complete 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; through 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.46' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Then skip to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Advancing Fire choice.</t>
   </si>
 </sst>
 </file>
@@ -3037,10 +3287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B300"/>
+  <dimension ref="A1:B318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,7 +3336,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3126,7 +3376,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3142,7 +3392,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -3150,7 +3400,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3158,367 +3408,367 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>192</v>
-      </c>
       <c r="B39" s="2" t="s">
-        <v>213</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3526,7 +3776,7 @@
         <v>28</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3534,7 +3784,7 @@
         <v>29</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -3542,1144 +3792,1288 @@
         <v>30</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>262</v>
+        <v>406</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>263</v>
+        <v>409</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>264</v>
+        <v>411</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>265</v>
+        <v>412</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>266</v>
+        <v>413</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>284</v>
+        <v>419</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>267</v>
+        <v>414</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>268</v>
+        <v>415</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>269</v>
+        <v>407</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>270</v>
+        <v>420</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>271</v>
+        <v>423</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>272</v>
+        <v>424</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>273</v>
+        <v>421</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>274</v>
+        <v>422</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>280</v>
+        <v>440</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>275</v>
+        <v>432</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>292</v>
+        <v>436</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>276</v>
+        <v>433</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>277</v>
+        <v>434</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>295</v>
+        <v>435</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>296</v>
+        <v>441</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B136" s="2" t="s">
+      <c r="B152" s="2" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>33</v>
+        <v>106</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>34</v>
+        <v>107</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A173" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B186" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B201" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B170" s="2" t="s">
+    <row r="202" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A179" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A183" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B183" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A184" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A185" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B185" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A186" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B186" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A187" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B187" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A188" s="1" t="s">
+      <c r="B207" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A209" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B188" s="3" t="s">
+      <c r="B210" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A211" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B211" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A189" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B189" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A190" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B190" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A191" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B191" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A192" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B192" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A193" s="1" t="s">
+    <row r="212" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B193" s="3" t="s">
+      <c r="B212" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A213" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B214" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A194" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B194" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A195" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A196" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B196" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A197" s="1" t="s">
+    <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A215" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B197" s="3" t="s">
+      <c r="B216" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A217" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B218" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A198" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B198" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A199" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B199" s="3" t="s">
+    <row r="219" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A219" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A221" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B221" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B200" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B201" s="3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A202" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A203" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B203" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B221" s="4"/>
-    </row>
-    <row r="300" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B239" s="4"/>
+    </row>
+    <row r="318" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A228:B403">
-    <sortCondition ref="A228:A403"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A246:B421">
+    <sortCondition ref="A246:A421"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trying to get weather rolls to work
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E63BBEF1-A036-46C2-A1B4-0BFC3A204568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C54573-70E8-4B88-9770-8835B6B5435E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
   <si>
     <t>r20.1</t>
   </si>
@@ -1663,22 +1663,6 @@
 Table per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r22.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and 
 &lt;InlineUIContainer&gt;&lt;Button Content='r23.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.65  Ambush Check&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D for possible Ambush and subtract one for rain, falling snow, or fog. If die roll is less than 7, consult appropriate 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, or 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Action Table for each enemy unit per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and 
-&lt;InlineUIContainer&gt;&lt;Button Content='r19.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
- Additionally, roll for random events on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Then go to 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Regardless of ambush status, continue with
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt; 
-to start the fight.</t>
   </si>
   <si>
     <t>r4.61</t>
@@ -2943,11 +2927,216 @@
     <t>r15.9</t>
   </si>
   <si>
-    <t>r15.10</t>
+    <t>r13.1</t>
+  </si>
+  <si>
+    <t>r13.11</t>
+  </si>
+  <si>
+    <t>r13.12</t>
+  </si>
+  <si>
+    <t>r13.13</t>
+  </si>
+  <si>
+    <t>r13.14</t>
+  </si>
+  <si>
+    <t>r13.3</t>
+  </si>
+  <si>
+    <t>r13.2</t>
+  </si>
+  <si>
+    <t>r13.4</t>
+  </si>
+  <si>
+    <t>r13.15</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.11 Move Forward &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A unit moving forward remains in the same sector, but moves one zone close to the hexagonal hub.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If it is already at close range, it jumps to close range in the sector on the other side of the hub direclty opposite the sector it now occupies.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.13 Move Right or Left &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Units moving to the right or left remain at the same range but move one zone clockwise or counterclockwise respectivley.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.14 Move Into US Control &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If an enemy unit moves into a sector marked US Control, remove the US Control marker.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.15 Moving Marker &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark moving enemy units with a Moving marker. Remove any Spotted, Hidden, or terrain markers. Immediately reroll for new facing and/or terrain on the Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c13Moving'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.0 Enemy Action &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the enemy action phase of the Battle Round Sequence, refer to the respective table: 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for each enemy unit on the Battle Board. Enemy units will either do nothing, move to another zone (or off the board), or fire their weapons.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Movement&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Infantry&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.1 Movement &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units move in four direcitons: &lt;LineBreak/&gt;
+F = Forward&lt;LineBreak/&gt;
+B = Backward&lt;LineBreak/&gt;
+L = Left&lt;LineBreak/&gt;
+R = Right
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Forward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Backward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Right or Left&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Into US Control &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Moving Marker</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.12 Move Backward &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A unit moving backward remains in the same sector, but moves one zone away from the hub. A unit already at long range in Sectors 4-5, 6-8, or 9-10 is removed from play.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A unit already at long range in Sectors 1, 2, or 3 is removed from the Battle Board and placed on the Movement Board in the area you moved out of to enter the current area. Remove the US Control marker from that area if present.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.4 Fire Versus Your Tank &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The enemy unit is trying to KO your tank. First roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Hit' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to see if the enemy shot hits your tank.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If it misses, continue resolving the action of the remaining enemy units. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the shot hits, roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Kill' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to see if the shot penetrates your tank. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;If the shot does not penetrate, continue to resolve enemy action. If it does penetrate, your tank is knocked out.</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r15.1 Time Passes&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Fifteen minutes of time has passed since the beginning of the battle. Mark off 15 minutes on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the passing of time moves the time past sunset, the battle continues as normal until resolved. Assume enough daylight remains to allow combat.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Once the battle is finished, the day ends.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.2 Friendly Artillery&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Friendly Artillery represents the fire of support guns. Resolve this fire by rolling on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+against each enemy unit on the Battle Board.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Note the special modifiers for artillery versus armored vehicles.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.4 Mines&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mines represent the danger of passing over buried mines when moving into enemy territory. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If your tank is not moving, this event is ignored. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If you are moving, refer to the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Minefield' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.5 Panzerfaust Attack&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+This event represents the random chance of an attack on your tank by a hand-held antitank rocket launcher. The German army of WW II was equipped with the Panzerchreck (a reusable launcher similar to the US bazooka) and the Panzerfaust ( a more commone disposable launcher).
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+These weapons fired a shaped charge something like a lump of putty that ignited on impact and would burn through armor. They send a jet of molten metal and burning gas into the tank. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Refer to the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Panzerfaust' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attack Table 
+to determine whether your tank is the object of this type of attack. If so, the table indicates whether the attack is succcessful.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c107Panzerfaust'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.6 Harassing Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+This event represents the random spraying of fire at your tank in the hopes of causing casualties to exposed crewmen. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+It was also possible for tis type of fire to cause collateral damage to your tank such as the damaging of periscopes, sights, adn the AA MG. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When this event is rolled, roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.8 Enemy Reinforcement&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When this event occurs, immediately activate one additional enemy unit for an Advance scenario and two additional for Battle/Counterattack scenarios.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the Battle Board 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+for the position of each new unit.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.3 Fire Versus Any Tank &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy SPG, tank and AT gun units may attempt to kill Sherman tanks of the forces friendly to you. Refer to the section of the &amp;quot;To Kill Sherman Tank&amp;quot; rows on the respective table:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, or &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The range for the enemy fire is determined by the range of the zone the unit occupies.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D. If the number rolled is less than or equal to the number shown on the table, one friendly tank is KO&amp;apos;ed. Record the loss of the tank on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.3 Enemy Artillery&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy Arillery represents the fire of guns in support of the enem units on the Battle Board and can result in the loss of friendly infantry squads. Also, it can damage your tank and wound exposed crew members. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D : &lt;LineBreak/&gt;
+1-6 = 1 squad lost &lt;LineBreak/&gt;
+7-9 = 2 squads lost &lt;LineBreak/&gt;
+10  = 3 squads lost &lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Also, roll on the &lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.7 Friendly Advance&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+This event represents the movement of friendly forces. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place one US Control marker in a sector of your choice that is empty of enemy units and adjacent to an already friendly sector.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ignore this event if no sector qualifies.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.9 Enemy Advance&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+This event represents the movement of enemy forces and the withdrawal of friendly forces.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Remove one US Control marker from the a Battle Board sector adjacent to an enemy unit but do not move the enemy unit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If two sectors are eligible, roll 1D:  &lt;LineBreak/&gt;
+1-5 = left hand sector  &lt;LineBreak/&gt;
+6-10 = right hand sector.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Ignore this event if no sector qualifies.</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r15.0 Random Events&lt;/Bold&gt; 
@@ -2963,145 +3152,115 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Advance&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.8' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Reinforcement&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r15.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Advance&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r15.10' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r15.2 Friendly Artillery&lt;/Bold&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r15.A' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Flanking Fire</t>
+  </si>
+  <si>
+    <t>r15.A</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.A Flanking Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+This event represents aggressive movement and fire from friendly forces. Roll against each enemy unit on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table with a die roll modifier of -10.</t>
+  </si>
+  <si>
+    <t>r4.7</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.2 Fire Versus Infantry &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy SPG, Tank, SPW, PSW, LW, and MG units may attempt to kill infantry squads of the forces friendly to you. Refer to the section of the &amp;quot;To Kill Infantry Squad&amp;quot; rows on the respective table:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
++B31&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The range for the enemy fire is determined by the range of the zone the unit occupies.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 2D. If the number rolled is less than or equal to the number shown on the table, one US infantry squad is KO&amp;apos;ed. Record the loss of the squad on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.65  Ambush Check&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D for possible Ambush and subtract one for rain, falling snow, or fog. If die roll is less than 7, consult appropriate table for each enemy unit:
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, or &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for enemy actions and 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for ambushes in Counterattack scenario. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
+Additionally, roll for random events on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Then go to 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Regardless of ambush status, continue with
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to start the fight.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.7  Battle Round Sequence&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Smoke Depletion Phase&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Spotting Phase&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.73' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Orders Phase&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Crew Actions Phase&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Enemy Actions Phase&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.76' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Friendly Action Phase&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Random Events Phase</t>
+  </si>
+  <si>
+    <t>r4.71</t>
+  </si>
+  <si>
+    <t>r4.72</t>
+  </si>
+  <si>
+    <t>r4.73</t>
+  </si>
+  <si>
+    <t>r4.74</t>
+  </si>
+  <si>
+    <t>r4.75</t>
+  </si>
+  <si>
+    <t>r4.76</t>
+  </si>
+  <si>
+    <t>r4.77</t>
+  </si>
+  <si>
+    <t>r4.8</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.71  Smoke Depletion Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.3 Enemy Artillery&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.72  Spotting Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.4 Mines&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.73  Orders Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.5 Panzerfaust Attack&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.74  Crew Actions Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.6 Harassing Fire&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.75  Enemy Actions Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.7 Friendly Advance&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.76  Friendly Action Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.8 Enemy Reinforcement&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.77   Random Events Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.9 Enemy Advance&lt;/Bold&gt; 
+    <t>&lt;Bold&gt;r4.8  When Your Tanks Is Target&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r15.10 Flanking Fire&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>r13.1</t>
-  </si>
-  <si>
-    <t>r13.11</t>
-  </si>
-  <si>
-    <t>r13.12</t>
-  </si>
-  <si>
-    <t>r13.13</t>
-  </si>
-  <si>
-    <t>r13.14</t>
-  </si>
-  <si>
-    <t>r13.3</t>
-  </si>
-  <si>
-    <t>r13.2</t>
-  </si>
-  <si>
-    <t>r13.4</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.3 Fire Versus Any Tank &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.4 Fire Versus Your Tank &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>r13.15</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.0 Enemy Action &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the enemy action phase of the Battle Round Sequence, refer to the respective table:
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll for each unit on the Battle Board. Enemy units will either do nothing, move to another zone (or off the board), move to another zone, or fire their weapons.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Movement&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Infantry&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.1 Movement &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units move n four direcitons: &lt;LineBreak/&gt;
-F = Forward&lt;LineBreak/&gt;
-B = Backward&lt;LineBreak/&gt;
-L = Left&lt;LineBreak/&gt;
-R = Right
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Forward&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Backward&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Right or Left&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Into US Control &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Moving Marker</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.11 Move Forward &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A unit moving forward remains in the same sector, but moves one zone close to the hexagonal hub.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If it is already at close range, it jumps to close range in the sector on the other side of the hub direclty opposite the sector it now occupies.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.12 Move Backward &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A unit moving backward remains in the same sector, but move sone zone away from the hub. A unit already at long range in Sectors 4-5, 6-8, or 9-10 is removed from play.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A unit alreayd at long range in Sectors 1, 2, or 3 is removed from the Battle Board and placed on the Movement Board in the area you moved out of to enter the current area. Remove the US Control marker from that area if present.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.13 Move Right or Left &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Units moving to the right or left remain at the same range but move one zone clockwise or counterclockwise respectivley.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.14 Move Into US Control &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If an enemy unit moves into a sector marked US Control, remove the US Control marker.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.15 Moving Marker &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark moving enemy units with a Moving marker. Remove any Spotted, Hidden, or terrain markers. Immediately reroll for new facing and/or terrain on the Battle Board 
-&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c13Moving'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r13.2 Fire Versus Infantry &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy SPG, Tank, SPW, PSW, LW, and MG units may attempt to kill infantry squads of the forces friendly to you. Refere to the section of the </t>
   </si>
 </sst>
 </file>
@@ -3474,10 +3633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B338"/>
+  <dimension ref="A1:B347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,7 +3682,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -3563,7 +3722,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -3744,7 +3903,7 @@
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>249</v>
@@ -3752,7 +3911,7 @@
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>250</v>
@@ -3760,7 +3919,7 @@
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>251</v>
@@ -3768,1659 +3927,1731 @@
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="48" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>228</v>
-      </c>
       <c r="B48" s="2" t="s">
-        <v>232</v>
+        <v>429</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>384</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+    <row r="68" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+    <row r="69" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="70" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
+    <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B73" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B64" s="2" t="s">
+      <c r="B74" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>364</v>
+        <v>320</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>365</v>
+        <v>321</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>381</v>
+        <v>345</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>367</v>
+        <v>323</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>368</v>
+        <v>325</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>369</v>
+        <v>326</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>370</v>
+        <v>327</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>371</v>
+        <v>328</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B120" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
+    <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="B113" s="2" t="s">
+    <row r="123" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+    <row r="124" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B124" s="2" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B116" s="2" t="s">
+    <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
+      <c r="B126" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="B117" s="2" t="s">
+    </row>
+    <row r="127" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+      <c r="B127" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B128" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
-        <v>431</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="B131" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B137" s="2" t="s">
         <v>438</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>265</v>
+        <v>430</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>283</v>
+        <v>434</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>266</v>
+        <v>431</v>
       </c>
       <c r="B139" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B143" s="2" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B142" s="2" t="s">
+    <row r="144" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>286</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B148" s="2" t="s">
+    <row r="158" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B149" s="2" t="s">
+      <c r="B168" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="B172" s="2" t="s">
         <v>474</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
-        <v>467</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
-        <v>473</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A165" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A172" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>82</v>
+        <v>444</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>83</v>
+        <v>445</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>85</v>
+        <v>446</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>86</v>
+        <v>447</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>92</v>
+        <v>475</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B186" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A178" s="5" t="s">
+    <row r="187" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B187" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A179" s="5" t="s">
+    <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B188" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
+    <row r="189" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B189" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A181" s="5" t="s">
+    <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B190" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A182" s="5" t="s">
+    <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B191" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A183" s="5" t="s">
+    <row r="192" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B192" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
+    <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B193" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A185" s="5" t="s">
+    <row r="194" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B194" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A186" s="5" t="s">
+    <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B195" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A187" s="5" t="s">
+    <row r="196" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B196" s="2" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A188" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A189" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A190" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B190" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A191" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A193" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A194" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>33</v>
+        <v>115</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>37</v>
+        <v>127</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>155</v>
+        <v>72</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A212" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A215" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="B215" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="5" t="s">
+    <row r="216" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B216" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A208" s="5" t="s">
+    <row r="217" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A217" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B217" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A209" s="5" t="s">
+    <row r="218" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A218" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="B218" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="5" t="s">
+    <row r="219" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B210" s="2" t="s">
+      <c r="B219" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="5" t="s">
+    <row r="220" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B211" s="2" t="s">
+      <c r="B220" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A212" s="5" t="s">
+    <row r="221" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B212" s="2" t="s">
+      <c r="B221" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="5" t="s">
+    <row r="222" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B213" s="2" t="s">
+      <c r="B222" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="5" t="s">
+    <row r="223" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B214" s="2" t="s">
+      <c r="B223" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A215" s="5" t="s">
+    <row r="224" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A224" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B224" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="5" t="s">
+    <row r="225" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B225" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A217" s="5" t="s">
+    <row r="226" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A226" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="B226" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A218" s="5" t="s">
+    <row r="227" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A227" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B227" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="5" t="s">
+    <row r="228" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="B228" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="5" t="s">
+    <row r="229" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B220" s="2" t="s">
+      <c r="B229" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A221" s="1" t="s">
+    <row r="230" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B221" s="3" t="s">
+      <c r="B230" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A222" s="1" t="s">
+    <row r="231" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A231" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B222" s="3" t="s">
+      <c r="B231" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A223" s="1" t="s">
+    <row r="232" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B223" s="3" t="s">
+      <c r="B232" s="3" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A224" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B224" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A225" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B225" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A226" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B226" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A227" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B227" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A228" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B228" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A229" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B229" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A230" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B230" s="3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A231" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B231" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A232" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B232" s="3" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A235" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A237" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A239" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A241" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B233" s="3" t="s">
+      <c r="B242" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A234" s="1" t="s">
+    <row r="243" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A243" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B234" s="3" t="s">
+      <c r="B243" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A235" s="1" t="s">
+    <row r="244" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B235" s="3" t="s">
+      <c r="B244" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A236" s="1" t="s">
+    <row r="245" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A245" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B236" s="3" t="s">
+      <c r="B245" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A237" s="1" t="s">
+    <row r="246" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B237" s="3" t="s">
+      <c r="B246" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A238" s="1" t="s">
+    <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A247" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B238" s="3" t="s">
+      <c r="B247" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A239" s="1" t="s">
+    <row r="248" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B239" s="3" t="s">
+      <c r="B248" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A240" s="1" t="s">
+    <row r="249" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B240" s="3" t="s">
+      <c r="B249" s="3" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A241" s="1" t="s">
+    <row r="250" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B241" s="3" t="s">
+      <c r="B250" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="259" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B259" s="4"/>
-    </row>
-    <row r="338" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B268" s="4"/>
+    </row>
+    <row r="347" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A266:B441">
-    <sortCondition ref="A266:A441"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A275:B450">
+    <sortCondition ref="A275:A450"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cleaened up Rules spreadsheet
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A3FAF72-A758-412F-9314-F50890F9272E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B14F6544-AA34-4AD6-9F92-B6537AF3BFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -391,14 +391,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r20.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Expected Enemy Resistance. </t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.12 Probability of Combat&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D. If the number rolled is less than or equal to the number shown on the scenario code, you go to action this day and begin the Sequence of Play 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the number rolled is higher than the code number, you miss combat this day. Mark the day off as completed on teh calender, and go on to the next day.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r20.4 Counterattack Scenario&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 A Counterattack scenario represents the Division on defense against an enemy counterattack. 
@@ -2579,21 +2571,6 @@
     <t>r10.1</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r10.1 Description&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In addition to its main gun, the Sherman tank is armed with several machine guns (MGs). 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The .30 calibre bow MG is mounted in the front right hull and is fired by the assistant driver.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The .30 calibre co-axial MG is mounted in the turret front along teh same axis as the main gun and is fired by the gunner.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The .50 calibre anti-aircraft (AA) MG is fixed to a pintle mount (post) on top of the turret and is fired by the commander. In some configurations, it can be fired by the loader.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Several hand held submachine guns (sub MGs) are carried in the turret and may be fired from open hatches.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c51FireCoaxialMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>r10.2</t>
   </si>
   <si>
@@ -3180,17 +3157,6 @@
     <t>r18.0</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.73  Orders Phase&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1. Hatch Segment: Open or close hatches by placing or removing Open Hatch marks on the Tank Card.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-2. Orders Segment: Mark crew battle actions by placing Crew Actions markers in teh crew boxes of the Tank Card per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Place only one marker per crewman.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-3. Ammo Reload Segment: Mark ammo reload if firing main gun by placing the Gun Reload marker in the box on the Tank Card for the ammo type you wish to reload per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Also mark the ammo is to be drawn from the ready rack by placing the Ready Rack Ammo Reload marker with the Gun Reload marker. Continue with &lt;InlineUIContainer&gt;&lt;Button Content='r4.74' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>r18.1</t>
   </si>
   <si>
@@ -3344,17 +3310,6 @@
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c70ThrowSmokeGrenade'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r18.21  Smoke Depletion Phase&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Smoke markers are printed in black on their front and gray on the back. When first placed, the black side is shown. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the Smoke Depletion Phase per 
-&lt;InlineUIContainer&gt;&lt;Image Name='r4.71'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; 
-of the Battle Round Sequence, one smoke marker is depleted in each zone containing Smoke markers. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Deplete smoke by either flipping one marker in each area to its gray side or by removing one marker already on its gray side.</t>
-  </si>
-  <si>
     <t>r18.3</t>
   </si>
   <si>
@@ -3457,6 +3412,26 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Crew Action Restrictions &lt;LineBreak/&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;r17.42 Unidentified Example&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+An unidentified tank is placed at medium range to your tanks's front. During the Spotting Phase, your gunner rolls sufficiently low to identify the vehicle. You immediately roll a 5 on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Appearance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
+resulting in the identification of the tank as a Pz IV. Replace the red Pz VIe counter with a black Pz IV counter.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Unidentified units are treated as the unit pictured for all purposes until identified. It is critical to identify counters as quickly as possible. Continue attempting to spot unidentified to spot unidentified units until they are identified.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r18.21  Smoke Depletion Phase&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Smoke markers are printed in black on their front and gray on the back. When first placed, the black side is shown. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the Smoke Depletion Phase per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+of the Battle Round Sequence, one smoke marker is depleted in each zone containing Smoke markers. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Deplete smoke by either flipping one marker in each area to its gray side or by removing one marker already on its gray side.</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r17.41 Unidentified Tanks&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 When an enemy tank, SPG, or AT gun unit is activated and first placed on the Battle Board, they are placed with their red side up. This indicates they are unidentified. 
@@ -3466,20 +3441,45 @@
 All unidentified units are:&lt;LineBreak/&gt;
 -- Tanks -&gt; Pz VIe&lt;LineBreak/&gt;
 -- SP Vehicles -&gt; STuG IIIg&lt;LineBreak/&gt;
--- AT guns -&gt; Pak 43 (88LL)
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When one of these is successfully identified, consult the 
+-- AT guns -&gt; Pak 43 (88LL) 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When one of these is successfully identified, consult the
 &lt;InlineUIContainer&gt;&lt;Button Content='Enemy Appearance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
- Table to determine what type of unit is actually present.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r17.42 Unidentified Example&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-An unidentified tank is placed at medium range to your tanks's front. During the Spotting Phase, your gunner rolls sufficiently low to identify the vehicle. You immediately roll a 5 on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Appearance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  
-resulting in the identification of the tank as a Pz IV. Replace the red Pz VIe counter with a black Pz IV counter.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Unidentified units are treated as the unit pictured for all purposes until identified. It is critical to identify counters as quickly as possible. Continue attempting to spot unidentified to spot unidentified units until they are identified.</t>
+Table to determine what type of unit is actually present.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.1 Description&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In addition to its main gun, the Sherman tank is armed with several machine guns (MGs). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .30 calibre bow MG is mounted in the front right hull and is fired by the assistant driver.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .30 calibre co-axial MG is mounted in the turret front along the same axis as the main gun and is fired by the gunner.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .50 calibre anti-aircraft (AA) MG is fixed to a pintle mount (post) on top of the turret and is fired by the commander. In some configurations, it can be fired by the loader.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Several hand held submachine guns (sub MGs) are carried in the turret and may be fired from open hatches.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c51FireCoaxialMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r20.12 Probability of Combat&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D. If the number rolled is less than or equal to the number shown on the scenario code, you go to action this day and begin the Sequence of Play 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the number rolled is higher than the code number, you miss combat this day. Mark the day off as completed on the calender, and go on to the next day.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.73  Orders Phase&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1. Hatch Segment: Open or close hatches by placing or removing Open Hatch marks on the Tank Card.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2. Orders Segment: Mark crew battle actions by placing Crew Actions markers in the crew boxes of the Tank Card per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Place only one marker per crewman.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+3. Ammo Reload Segment: Mark ammo reload if firing main gun by placing the Gun Reload marker in the box on the Tank Card for the ammo type you wish to reload per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Also, mark the ammo is to be drawn from the ready rack by placing the Ready Rack Ammo Reload marker with the Gun Reload marker. Continue with &lt;InlineUIContainer&gt;&lt;Button Content='r4.74' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -3854,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3901,7 +3901,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -3941,7 +3941,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -3957,7 +3957,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -3965,7 +3965,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -3973,439 +3973,439 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>491</v>
+        <v>529</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -4413,7 +4413,7 @@
         <v>28</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4421,7 +4421,7 @@
         <v>29</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -4429,1183 +4429,1183 @@
         <v>30</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>401</v>
+        <v>527</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>514</v>
+        <v>525</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
+        <v>512</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5613,7 +5613,7 @@
         <v>31</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -5621,7 +5621,7 @@
         <v>32</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5677,7 +5677,7 @@
         <v>41</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.3">
@@ -5693,7 +5693,7 @@
         <v>43</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5701,7 +5701,7 @@
         <v>44</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5714,10 +5714,10 @@
     </row>
     <row r="232" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -5741,7 +5741,7 @@
         <v>11</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>66</v>
+        <v>528</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -5773,7 +5773,7 @@
         <v>4</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="240" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -5781,7 +5781,7 @@
         <v>5</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -5789,7 +5789,7 @@
         <v>6</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -5797,7 +5797,7 @@
         <v>7</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5818,170 +5818,170 @@
     </row>
     <row r="245" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B257" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="283" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Created last two tables
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57BFA92B-AD84-43C1-81CA-32392AC0D948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F55FC27E-1176-42E6-86AB-AC3AEE612A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -827,14 +827,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.54.4  Attempt Resupply&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if resupply occurs. If successful, you may relead your tank with ammo. Continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.5  Movement Sequence&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The Movement Sequence is performed on the Movement Board using the following steps:
@@ -1043,27 +1035,6 @@
 Mark the area with the Exit Area marker.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c34ExitArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r4.54.2  Call for Artillery Support&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Call to hit an area adjacent to your task force. Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if Artillery Support arrives 
-&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-If successful, place an Artillery Support marker on the area. Three Artillery Support markers are allowed and can be placed in the same area. Continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.54.3  Call for Air Strike&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Call to hit an area adjacent to your task force. Consult the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-to see if Air Strike arrives
- &lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  If successful, place an Air Strike marker on the area. Two Air Strike markers are allowed and can be placed in the same area. Additionally, while waiting for air strike, a 15 minute operation can be chosen to happen in parallel. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Continue with 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
     <t>r23.11</t>
@@ -3647,6 +3618,37 @@
 If the colored die is 1-3, mark off 1 unit of fuel. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 A tank with no fuel may not perform the above movement actions, nor may the tank pivot.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.54.3  Call for Air Strike&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Call to hit an area adjacent to your task force. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if Air Strike arrives per
+ &lt;InlineUIContainer&gt;&lt;Button Content='r23.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Roll 1D with roll less than 5. If successful, place an Air Strike marker on the area. Two Air Strike markers are allowed and can be placed in the same area. Additionally, while waiting for air strike, a 15 minute operation can be chosen to happen in parallel. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r4.54.2  Call for Artillery Support&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Call to hit an area adjacent to your task force. Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to see if Artillery Support arrives per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.  Roll 1D with a roll less than 8. 
+If successful, place an Artillery Support marker on the area. Three Artillery Support markers are allowed and can be placed in the same area. Continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.54.4  Attempt Resupply&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table to see if resupply occurs (Roll 1D less than 8). If successful, you may reload your tank with ammo per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+and fuel per &lt;InlineUIContainer&gt;&lt;Button Content='r29.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -4021,8 +4023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A273" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B277" sqref="B277"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4068,7 +4070,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -4108,7 +4110,7 @@
         <v>50</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -4132,7 +4134,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
@@ -4148,7 +4150,7 @@
         <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -4156,7 +4158,7 @@
         <v>93</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -4204,7 +4206,7 @@
         <v>134</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -4212,7 +4214,7 @@
         <v>135</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -4220,7 +4222,7 @@
         <v>136</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -4228,7 +4230,7 @@
         <v>137</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -4236,7 +4238,7 @@
         <v>138</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -4252,7 +4254,7 @@
         <v>140</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>173</v>
+        <v>552</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -4260,15 +4262,15 @@
         <v>141</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>142</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>145</v>
+        <v>553</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
@@ -4276,303 +4278,303 @@
         <v>143</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -4580,7 +4582,7 @@
         <v>28</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -4601,866 +4603,866 @@
     </row>
     <row r="72" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -5468,7 +5470,7 @@
         <v>78</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -5500,7 +5502,7 @@
         <v>83</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -5548,7 +5550,7 @@
         <v>106</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -5636,7 +5638,7 @@
         <v>125</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -5644,7 +5646,7 @@
         <v>127</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -5652,127 +5654,127 @@
         <v>128</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5788,7 +5790,7 @@
         <v>32</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5844,7 +5846,7 @@
         <v>41</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.3">
@@ -5860,7 +5862,7 @@
         <v>43</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
@@ -5868,7 +5870,7 @@
         <v>44</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5884,7 +5886,7 @@
         <v>72</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
@@ -5908,7 +5910,7 @@
         <v>11</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
@@ -5988,7 +5990,7 @@
         <v>73</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="246" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -5996,7 +5998,7 @@
         <v>75</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="247" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
@@ -6004,7 +6006,7 @@
         <v>76</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
@@ -6012,239 +6014,239 @@
         <v>77</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B265" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B275" s="3" t="s">
         <v>548</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B276" s="3" t="s">
         <v>549</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Set up when skipping Movement Phase
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F55FC27E-1176-42E6-86AB-AC3AEE612A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{487752E2-7F77-4357-A03E-8EF3E2DFEEE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -3039,24 +3039,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.65  Ambush Check&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll 1D for possible Ambush and subtract one for rain, falling snow, or fog. If die roll is less than 7, consult appropriate table for each enemy unit:
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table, or &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Action Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-See 
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for enemy actions and 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for ambushes in Counterattack scenario. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt; 
-Additionally, roll for random events on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. Then go to 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Regardless of ambush status, continue with
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to start the fight.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.7  Battle Round Sequence&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Smoke Depletion Phase&lt;LineBreak/&gt;
@@ -3649,6 +3631,26 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 and fuel per &lt;InlineUIContainer&gt;&lt;Button Content='r29.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Continue with 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.65  Ambush Check&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll 1D for possible Ambush and subtract one for rain, falling snow, or fog. If roll is greater than 6, no ambush occurs.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If die roll is less than 7, ambush occurs. consult appropriate table for each enemy unit on the appropriate Action Table: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for enemy actions and 
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for ambushes in Counterattack scenario. 
+Additionally, roll for random events on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Regardless of ambush status, continue with 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to start the fight.</t>
   </si>
 </sst>
 </file>
@@ -4023,17 +4025,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="216.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="216.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>47</v>
       </c>
@@ -4041,7 +4043,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>48</v>
       </c>
@@ -4049,7 +4051,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -4057,7 +4059,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -4065,7 +4067,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
@@ -4073,7 +4075,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
@@ -4081,7 +4083,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
@@ -4089,7 +4091,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>51</v>
       </c>
@@ -4097,7 +4099,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -4105,7 +4107,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
@@ -4113,7 +4115,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
@@ -4137,7 +4139,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -4145,7 +4147,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>92</v>
       </c>
@@ -4153,7 +4155,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>93</v>
       </c>
@@ -4161,7 +4163,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>94</v>
       </c>
@@ -4169,7 +4171,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>95</v>
       </c>
@@ -4177,7 +4179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>96</v>
       </c>
@@ -4185,7 +4187,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>97</v>
       </c>
@@ -4193,7 +4195,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>102</v>
       </c>
@@ -4201,7 +4203,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>134</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>135</v>
       </c>
@@ -4217,7 +4219,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>136</v>
       </c>
@@ -4225,7 +4227,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>137</v>
       </c>
@@ -4233,7 +4235,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>138</v>
       </c>
@@ -4241,7 +4243,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>139</v>
       </c>
@@ -4249,31 +4251,31 @@
         <v>144</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>140</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>141</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>142</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>143</v>
       </c>
@@ -4281,7 +4283,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>237</v>
       </c>
@@ -4289,7 +4291,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>243</v>
       </c>
@@ -4297,7 +4299,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>244</v>
       </c>
@@ -4305,7 +4307,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>245</v>
       </c>
@@ -4313,7 +4315,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>246</v>
       </c>
@@ -4321,87 +4323,87 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>247</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>467</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="B39" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="B40" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>472</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="B41" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="B42" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
         <v>476</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>180</v>
       </c>
@@ -4409,7 +4411,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>181</v>
       </c>
@@ -4417,7 +4419,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>182</v>
       </c>
@@ -4425,7 +4427,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>183</v>
       </c>
@@ -4433,7 +4435,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>184</v>
       </c>
@@ -4441,7 +4443,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>185</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>213</v>
       </c>
@@ -4457,7 +4459,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>215</v>
       </c>
@@ -4465,7 +4467,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>216</v>
       </c>
@@ -4473,7 +4475,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>217</v>
       </c>
@@ -4481,7 +4483,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>218</v>
       </c>
@@ -4489,7 +4491,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>219</v>
       </c>
@@ -4497,7 +4499,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>220</v>
       </c>
@@ -4505,7 +4507,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>223</v>
       </c>
@@ -4513,7 +4515,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>224</v>
       </c>
@@ -4521,15 +4523,15 @@
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>225</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>226</v>
       </c>
@@ -4537,7 +4539,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>228</v>
       </c>
@@ -4545,7 +4547,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>205</v>
       </c>
@@ -4553,7 +4555,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>207</v>
       </c>
@@ -4561,7 +4563,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>208</v>
       </c>
@@ -4569,7 +4571,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>209</v>
       </c>
@@ -4577,7 +4579,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>28</v>
       </c>
@@ -4585,7 +4587,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>29</v>
       </c>
@@ -4593,7 +4595,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>30</v>
       </c>
@@ -4601,7 +4603,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>284</v>
       </c>
@@ -4609,7 +4611,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>285</v>
       </c>
@@ -4617,7 +4619,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>287</v>
       </c>
@@ -4625,7 +4627,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>288</v>
       </c>
@@ -4633,7 +4635,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>289</v>
       </c>
@@ -4641,7 +4643,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>290</v>
       </c>
@@ -4649,7 +4651,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>291</v>
       </c>
@@ -4657,7 +4659,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>292</v>
       </c>
@@ -4665,7 +4667,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>293</v>
       </c>
@@ -4673,7 +4675,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>294</v>
       </c>
@@ -4681,7 +4683,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>295</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>296</v>
       </c>
@@ -4697,7 +4699,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>297</v>
       </c>
@@ -4705,7 +4707,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>298</v>
       </c>
@@ -4713,7 +4715,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>299</v>
       </c>
@@ -4721,7 +4723,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>300</v>
       </c>
@@ -4729,7 +4731,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>301</v>
       </c>
@@ -4737,7 +4739,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>302</v>
       </c>
@@ -4745,7 +4747,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>303</v>
       </c>
@@ -4753,7 +4755,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>304</v>
       </c>
@@ -4761,7 +4763,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>305</v>
       </c>
@@ -4769,7 +4771,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>306</v>
       </c>
@@ -4777,7 +4779,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>307</v>
       </c>
@@ -4785,7 +4787,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>308</v>
       </c>
@@ -4793,7 +4795,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>309</v>
       </c>
@@ -4801,7 +4803,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>310</v>
       </c>
@@ -4809,7 +4811,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>311</v>
       </c>
@@ -4817,7 +4819,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>312</v>
       </c>
@@ -4825,7 +4827,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>313</v>
       </c>
@@ -4833,15 +4835,15 @@
         <v>314</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>315</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>316</v>
       </c>
@@ -4849,7 +4851,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>317</v>
       </c>
@@ -4857,7 +4859,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>318</v>
       </c>
@@ -4865,7 +4867,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>319</v>
       </c>
@@ -4873,7 +4875,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>352</v>
       </c>
@@ -4881,7 +4883,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>353</v>
       </c>
@@ -4889,7 +4891,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>354</v>
       </c>
@@ -4897,7 +4899,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>355</v>
       </c>
@@ -4905,7 +4907,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>356</v>
       </c>
@@ -4913,7 +4915,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>357</v>
       </c>
@@ -4921,7 +4923,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>358</v>
       </c>
@@ -4929,7 +4931,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>359</v>
       </c>
@@ -4937,7 +4939,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>368</v>
       </c>
@@ -4945,7 +4947,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>360</v>
       </c>
@@ -4953,7 +4955,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>361</v>
       </c>
@@ -4961,7 +4963,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>362</v>
       </c>
@@ -4969,7 +4971,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>363</v>
       </c>
@@ -4977,7 +4979,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>364</v>
       </c>
@@ -4985,7 +4987,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>365</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>366</v>
       </c>
@@ -5001,7 +5003,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>367</v>
       </c>
@@ -5009,7 +5011,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>377</v>
       </c>
@@ -5017,7 +5019,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>378</v>
       </c>
@@ -5025,7 +5027,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>392</v>
       </c>
@@ -5033,15 +5035,15 @@
         <v>394</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>395</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>396</v>
       </c>
@@ -5049,7 +5051,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>397</v>
       </c>
@@ -5057,7 +5059,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>398</v>
       </c>
@@ -5065,7 +5067,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>399</v>
       </c>
@@ -5073,7 +5075,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>400</v>
       </c>
@@ -5081,7 +5083,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>393</v>
       </c>
@@ -5089,7 +5091,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>405</v>
       </c>
@@ -5097,7 +5099,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>408</v>
       </c>
@@ -5105,7 +5107,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>409</v>
       </c>
@@ -5113,7 +5115,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>406</v>
       </c>
@@ -5121,7 +5123,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>407</v>
       </c>
@@ -5129,7 +5131,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>417</v>
       </c>
@@ -5137,7 +5139,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>418</v>
       </c>
@@ -5145,7 +5147,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>419</v>
       </c>
@@ -5153,7 +5155,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>420</v>
       </c>
@@ -5161,7 +5163,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>249</v>
       </c>
@@ -5169,7 +5171,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>250</v>
       </c>
@@ -5177,7 +5179,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>251</v>
       </c>
@@ -5185,7 +5187,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>252</v>
       </c>
@@ -5193,7 +5195,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>253</v>
       </c>
@@ -5201,7 +5203,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>254</v>
       </c>
@@ -5209,7 +5211,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>255</v>
       </c>
@@ -5217,7 +5219,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>256</v>
       </c>
@@ -5225,7 +5227,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>257</v>
       </c>
@@ -5233,7 +5235,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>258</v>
       </c>
@@ -5241,7 +5243,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>259</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>260</v>
       </c>
@@ -5257,7 +5259,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>261</v>
       </c>
@@ -5265,7 +5267,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>262</v>
       </c>
@@ -5273,7 +5275,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>263</v>
       </c>
@@ -5281,7 +5283,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>264</v>
       </c>
@@ -5289,7 +5291,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>391</v>
       </c>
@@ -5297,7 +5299,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>437</v>
       </c>
@@ -5305,7 +5307,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>438</v>
       </c>
@@ -5313,7 +5315,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>439</v>
       </c>
@@ -5321,7 +5323,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>440</v>
       </c>
@@ -5329,7 +5331,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>441</v>
       </c>
@@ -5337,7 +5339,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>445</v>
       </c>
@@ -5345,7 +5347,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>443</v>
       </c>
@@ -5353,7 +5355,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>442</v>
       </c>
@@ -5361,7 +5363,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>444</v>
       </c>
@@ -5369,7 +5371,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>282</v>
       </c>
@@ -5377,7 +5379,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>427</v>
       </c>
@@ -5385,7 +5387,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>428</v>
       </c>
@@ -5393,7 +5395,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>429</v>
       </c>
@@ -5401,7 +5403,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>430</v>
       </c>
@@ -5409,7 +5411,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>431</v>
       </c>
@@ -5417,7 +5419,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>432</v>
       </c>
@@ -5425,7 +5427,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>433</v>
       </c>
@@ -5433,7 +5435,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>434</v>
       </c>
@@ -5441,7 +5443,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>435</v>
       </c>
@@ -5449,7 +5451,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>436</v>
       </c>
@@ -5457,7 +5459,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>465</v>
       </c>
@@ -5465,7 +5467,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>78</v>
       </c>
@@ -5473,7 +5475,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>79</v>
       </c>
@@ -5481,7 +5483,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>80</v>
       </c>
@@ -5489,7 +5491,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>81</v>
       </c>
@@ -5497,7 +5499,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>83</v>
       </c>
@@ -5505,7 +5507,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>84</v>
       </c>
@@ -5513,7 +5515,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>85</v>
       </c>
@@ -5521,7 +5523,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>103</v>
       </c>
@@ -5529,7 +5531,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>104</v>
       </c>
@@ -5537,7 +5539,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>105</v>
       </c>
@@ -5545,15 +5547,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>107</v>
       </c>
@@ -5561,7 +5563,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>108</v>
       </c>
@@ -5569,7 +5571,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>109</v>
       </c>
@@ -5577,7 +5579,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>110</v>
       </c>
@@ -5585,7 +5587,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>111</v>
       </c>
@@ -5593,7 +5595,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>112</v>
       </c>
@@ -5601,7 +5603,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>113</v>
       </c>
@@ -5609,7 +5611,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>114</v>
       </c>
@@ -5617,7 +5619,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>115</v>
       </c>
@@ -5625,7 +5627,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>124</v>
       </c>
@@ -5633,151 +5635,151 @@
         <v>126</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B203" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A206" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A212" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A204" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A205" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A206" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A207" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A208" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A209" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A210" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A211" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A212" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="B212" s="2" t="s">
+    <row r="214" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="B214" s="2" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A213" s="5" t="s">
-        <v>501</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A214" s="5" t="s">
+    <row r="215" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A215" s="5" t="s">
         <v>502</v>
       </c>
-      <c r="B214" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A215" s="5" t="s">
+      <c r="B215" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="B215" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A217" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B217" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A218" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A217" s="5" t="s">
-        <v>508</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A218" s="5" t="s">
-        <v>509</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
         <v>31</v>
       </c>
@@ -5785,15 +5787,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
         <v>33</v>
       </c>
@@ -5801,7 +5803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
         <v>34</v>
       </c>
@@ -5809,7 +5811,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
         <v>35</v>
       </c>
@@ -5817,7 +5819,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
         <v>36</v>
       </c>
@@ -5825,7 +5827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
         <v>37</v>
       </c>
@@ -5833,7 +5835,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
         <v>40</v>
       </c>
@@ -5841,7 +5843,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>41</v>
       </c>
@@ -5849,7 +5851,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>39</v>
       </c>
@@ -5857,7 +5859,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>43</v>
       </c>
@@ -5865,7 +5867,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>44</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>45</v>
       </c>
@@ -5881,7 +5883,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>72</v>
       </c>
@@ -5889,7 +5891,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>0</v>
       </c>
@@ -5897,7 +5899,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>1</v>
       </c>
@@ -5905,15 +5907,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>12</v>
       </c>
@@ -5921,7 +5923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>2</v>
       </c>
@@ -5929,7 +5931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>3</v>
       </c>
@@ -5937,7 +5939,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>4</v>
       </c>
@@ -5945,7 +5947,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>5</v>
       </c>
@@ -5953,7 +5955,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>6</v>
       </c>
@@ -5961,7 +5963,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
         <v>7</v>
       </c>
@@ -5969,7 +5971,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
         <v>8</v>
       </c>
@@ -5977,7 +5979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
         <v>9</v>
       </c>
@@ -5985,7 +5987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>73</v>
       </c>
@@ -5993,7 +5995,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>75</v>
       </c>
@@ -6001,7 +6003,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>76</v>
       </c>
@@ -6009,7 +6011,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>77</v>
       </c>
@@ -6017,7 +6019,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>158</v>
       </c>
@@ -6025,7 +6027,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>159</v>
       </c>
@@ -6033,7 +6035,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>162</v>
       </c>
@@ -6041,7 +6043,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>163</v>
       </c>
@@ -6049,7 +6051,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>164</v>
       </c>
@@ -6057,7 +6059,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="288" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>160</v>
       </c>
@@ -6065,7 +6067,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>167</v>
       </c>
@@ -6073,7 +6075,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>168</v>
       </c>
@@ -6081,7 +6083,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>172</v>
       </c>
@@ -6089,39 +6091,39 @@
         <v>173</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B258" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A259" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="B259" s="3" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A260" s="1" t="s">
-        <v>539</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A261" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>188</v>
       </c>
@@ -6129,7 +6131,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>189</v>
       </c>
@@ -6137,7 +6139,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>190</v>
       </c>
@@ -6145,7 +6147,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>191</v>
       </c>
@@ -6153,7 +6155,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="266" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>195</v>
       </c>
@@ -6161,7 +6163,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>196</v>
       </c>
@@ -6169,7 +6171,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>197</v>
       </c>
@@ -6177,82 +6179,82 @@
         <v>201</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="B269" s="3" t="s">
+      <c r="B270" s="3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B273" s="3" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="270" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A270" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A271" s="1" t="s">
-        <v>528</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A272" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A273" s="1" t="s">
+    <row r="274" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B273" s="3" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A274" s="1" t="s">
+      <c r="B274" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="B274" s="3" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="B275" s="3" t="s">
+      <c r="B276" s="3" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A276" s="1" t="s">
+    <row r="277" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="B276" s="3" t="s">
+      <c r="B277" s="3" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A277" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B286" s="4"/>
     </row>
-    <row r="365" ht="154.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="365" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A293:B468">
     <sortCondition ref="A293:A468"/>

</xml_diff>

<commit_message>
Setting up Enemy Action Move and Fire
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{80D5D6A0-9E2B-4C91-89C3-27D3B898D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9C894194-A9AD-48E5-84DD-B6C7A679AAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -1490,12 +1490,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.65' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Ambush Check</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.61  Placement of Advancing Fire&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Place Advancing Fire markes per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.62  Activation of Enemy Units&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Consult the 
@@ -2821,21 +2815,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r13.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r13.1 Movement &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units move in four direcitons: &lt;LineBreak/&gt;
-F = Forward&lt;LineBreak/&gt;
-B = Backward&lt;LineBreak/&gt;
-L = Left&lt;LineBreak/&gt;
-R = Right
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Forward&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Backward&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Right or Left&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Into US Control &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Moving Marker</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r13.12 Move Backward &lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 A unit moving backward remains in the same sector, but moves one zone away from the hub. A unit already at long range in Sectors 4-5, 6-8, or 9-10 is removed from play.
@@ -3044,10 +3023,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.75  Enemy Actions Phase&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.76  Friendly Action Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
@@ -3599,14 +3574,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.54' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r20.44 Counterattack - Clear Battle Board&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If battle (or even your Ambush) clears the board of enemy units, return to Time Check &lt;InlineUIContainer&gt;&lt;Button Content='r4.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
-to determine how many hours pass before a battle becomes possible again. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Mark off the hours that pass, and go to Prepare for Battle &lt;InlineUIContainer&gt;&lt;Button Content='r20.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r20.0 Campaign&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;The campaign recreates actions of the 4th Armored Division from late July, 1944 through April, 1945. Each day the 4th Armored saw action,
 there is a chance your tank will fight; when the Division is refitting, you will be resting. Each day begins with a check of the Combat &lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
@@ -3636,6 +3603,12 @@
 If you retreat from the Battle Board, go to &lt;InlineUIContainer&gt;&lt;Button Content='r20.45' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
+    <t>&lt;Bold&gt;r4.61  Placement of Advancing Fire&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Place Advancing Fire markers per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r22.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
     <t>&lt;Bold&gt;r4.65  Ambush Check&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Roll 1D for possible Ambush and subtract one for rain, falling snow, or fog. If roll is greater than 6, no ambush occurs.
@@ -3651,10 +3624,55 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 If this is a Counterattack scenario, skip the enemy actions and follow 
-&lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for how ambushes are affected.
+&lt;InlineUIContainer&gt;&lt;Button Content='r20.43' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for how ambushes are implemented.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Regardless of ambush status, continue with 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to start the fight.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.1 Movement &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units move in four directions: &lt;LineBreak/&gt;
+F = Forward&lt;LineBreak/&gt;
+B = Backward&lt;LineBreak/&gt;
+L = Left&lt;LineBreak/&gt;
+R = Right
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Forward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Backward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Right or Left&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Into US Control &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Moving Marker</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.75  Enemy Actions Phase&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll on the respective table for each enemy unit on the Battle Board:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) &lt;InlineUIContainer&gt;&lt;Button Content='r13.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Roll for each moving enemy unit on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Placement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table (vehicle units only) for new facing and/or terrain. Place Moving marker on units that move.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2.) &lt;InlineUIContainer&gt;&lt;Button Content='r13.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; For attacks not directed at your tank, roll on the 
+respective Enemy Combat Fire Table. Record friendly casualties on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+3.) For attacks directed at your tank, go to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.8' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+4.) Continue with Friendly Action Phase per &lt;InlineUIContainer&gt;&lt;Button Content='r4.76' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r20.44 Counterattack - Clear Battle Board&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If battle (or even your Ambush) clears the board of enemy units, return to Time Check &lt;InlineUIContainer&gt;&lt;Button Content='r4.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+to determine how many hours pass before a battle becomes possible again. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Mark off the hours that pass, and go to Prepare for Battle &lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
 </sst>
 </file>
@@ -4029,8 +4047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B242" sqref="B242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4076,7 +4094,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4116,7 +4134,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4260,7 +4278,7 @@
         <v>138</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4268,7 +4286,7 @@
         <v>139</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4276,7 +4294,7 @@
         <v>140</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4297,114 +4315,114 @@
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>236</v>
+        <v>549</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>476</v>
+        <v>552</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4420,7 +4438,7 @@
         <v>178</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4532,7 +4550,7 @@
         <v>222</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4609,866 +4627,866 @@
     </row>
     <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>448</v>
+        <v>551</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B168" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5476,7 +5494,7 @@
         <v>76</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5556,7 +5574,7 @@
         <v>104</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5644,7 +5662,7 @@
         <v>123</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -5652,7 +5670,7 @@
         <v>125</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5660,127 +5678,127 @@
         <v>126</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>503</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5796,7 +5814,7 @@
         <v>31</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5892,7 +5910,7 @@
         <v>71</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5916,7 +5934,7 @@
         <v>11</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5972,7 +5990,7 @@
         <v>7</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5980,7 +5998,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6052,7 +6070,7 @@
         <v>160</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6068,7 +6086,7 @@
         <v>158</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6100,31 +6118,31 @@
         <v>166</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6185,74 +6203,74 @@
     </row>
     <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B275" s="3" t="s">
         <v>541</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B276" s="3" t="s">
         <v>542</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B277" s="3" t="s">
         <v>543</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started on Random Events
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7CA541-09C1-47F0-A8C3-B988132B34EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{71E7128A-5C8D-48E8-A288-2CA612B8DA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3232,14 +3232,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.72' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r5.23 Gun Loads&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In the gun load section, place the Gun Load marker in the box of the ammo round loaded in the gun. Also markhere what round type you want to reload after firing (ammo reload marker), and whether you will draw reloads from the ready rack (ready rack ammo reload marker) per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Name='c30ReadyRackAmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.72  Spotting Phase&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Determine what your crew can see by consulting the 
@@ -3674,6 +3666,16 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r18.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Smoke Depletion Phase&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r18.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Smoke Multiplier Markers&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r18.23' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Smoke In Rain</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r5.23 Gun Loads&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In the gun load section, place the Gun Load marker in the box of the ammo round loaded in the gun. Also mark here what round type you want to reload after firing (ammo reload marker), and whether you will draw reloads from the ready rack (ready rack ammo reload marker) per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+           &lt;InlineUIContainer&gt;&lt;Image Name='c17GunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+      &lt;InlineUIContainer&gt;&lt;Image Name='c29AmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+      &lt;InlineUIContainer&gt;&lt;Image Name='c30ReadyRackAmmoReload'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4048,8 +4050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A210" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B64" sqref="B63:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4279,7 +4281,7 @@
         <v>138</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4287,7 +4289,7 @@
         <v>139</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4295,7 +4297,7 @@
         <v>140</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4319,7 +4321,7 @@
         <v>239</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4351,7 +4353,7 @@
         <v>243</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4375,7 +4377,7 @@
         <v>466</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4383,7 +4385,7 @@
         <v>467</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4399,7 +4401,7 @@
         <v>469</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4546,12 +4548,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>222</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>507</v>
+        <v>553</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5063,7 +5065,7 @@
         <v>391</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5327,7 +5329,7 @@
         <v>433</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5575,7 +5577,7 @@
         <v>104</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5663,7 +5665,7 @@
         <v>123</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -5671,7 +5673,7 @@
         <v>125</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5679,7 +5681,7 @@
         <v>126</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -5751,7 +5753,7 @@
         <v>493</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5759,7 +5761,7 @@
         <v>494</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5767,7 +5769,7 @@
         <v>495</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5911,7 +5913,7 @@
         <v>71</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5935,7 +5937,7 @@
         <v>11</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5991,7 +5993,7 @@
         <v>7</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5999,7 +6001,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6119,31 +6121,31 @@
         <v>166</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6204,74 +6206,74 @@
     </row>
     <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B274" s="3" t="s">
         <v>522</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Trying to figure out problem with smoke depletion
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9FA2007-67E9-43AC-9BC2-ECD6D6F797E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FE0C082-B12C-4E50-ADB6-759B5E7433B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -996,32 +996,6 @@
     <t>r23.11</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r23.1 Artillery Support Resolution&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Artillery support takes effect in a newly entered area immediately after any appearing enemy units are placed on the Battle Board. Resolve Arillery Support by rolling on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table against each enemy unit.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units destroyed by artillery support are immediately removed, and their victory points ar recorded under friendly forces of the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll again against each surviving enemy unit for each additional support marker.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r23.1 Artillery Support&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Artillery support can be called for during the Movement Sequence 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-This operation takes 15 minutes. Mark off the time and rol 1D as shown on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Use Table to see if the support arrives. It arrives on 1-7 roll. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If successful, place an Artillery Support marker in the area where the artillery landed. If at any time during this day you enter the marked area (before reaching the exit area), the artillery support will attack all enemy units appearing. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Additional artillery support may be called for, but no more than three support markers may be on the Movement Board at one time. You may voluntarily pick up an Artillery Support marker if you decide to attempt to place it elsewhere.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r22.0 Advancing Fire&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Advancing Fire represents blind HE and MG fire at places likely to be concealing unknown enemy units. It may take place both when you tank first enters a new map area and during Battle Rounds.
@@ -3682,6 +3656,37 @@
 If either event occurs, remove the Hidden marker. You may attempt to spot this unit during the next Spotting Phase.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c31Hidden'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r23.1 Artillery Support Resolution&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Artillery support takes effect in a newly entered area immediately after any appearing enemy units are placed on the Battle Board. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Resolve Arillery Support by rolling on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table against each enemy unit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units destroyed by artillery support are immediately removed, and their victory points ar recorded under friendly forces of the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Roll again against each surviving enemy unit for each additional support marker.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r23.1 Artillery Support&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Artillery support can be called for during the Movement Sequence 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+This operation takes 15 minutes. Mark off the time and roll 1D as shown on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Time' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Use Table to see if the support arrives. It arrives on 1-7 roll. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If successful, place an Artillery Support marker in the area where the artillery landed. If at any time during this day you enter the marked area (before reaching the exit area), the artillery support will attack all enemy units appearing. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Additional artillery support may be called for, but no more than three support markers may be on the Movement Board at one time. You may voluntarily pick up an Artillery Support marker if you decide to attempt to place it elsewhere. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Resolution is performed per  
+&lt;InlineUIContainer&gt;&lt;Button Content='r23.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                        &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4056,8 +4061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B365"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B198" sqref="B198"/>
+    <sheetView tabSelected="1" topLeftCell="A254" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4103,7 +4108,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4143,7 +4148,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4183,7 +4188,7 @@
         <v>90</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4263,7 +4268,7 @@
         <v>134</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
@@ -4287,7 +4292,7 @@
         <v>137</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4295,7 +4300,7 @@
         <v>138</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4303,7 +4308,7 @@
         <v>139</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4311,303 +4316,303 @@
         <v>140</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4636,866 +4641,866 @@
     </row>
     <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B125" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5503,7 +5508,7 @@
         <v>76</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5583,7 +5588,7 @@
         <v>104</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5663,7 +5668,7 @@
         <v>122</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5671,7 +5676,7 @@
         <v>123</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -5679,7 +5684,7 @@
         <v>124</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5687,127 +5692,127 @@
         <v>125</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5823,7 +5828,7 @@
         <v>31</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5919,7 +5924,7 @@
         <v>71</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5943,7 +5948,7 @@
         <v>11</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5999,7 +6004,7 @@
         <v>7</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6007,7 +6012,7 @@
         <v>8</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6055,7 +6060,7 @@
         <v>155</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6063,7 +6068,7 @@
         <v>156</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6079,7 +6084,7 @@
         <v>159</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6095,7 +6100,7 @@
         <v>157</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6103,23 +6108,23 @@
         <v>163</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>164</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>168</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>169</v>
+        <v>552</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6127,159 +6132,159 @@
         <v>165</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B261" s="3" t="s">
         <v>526</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B267" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B270" s="3" t="s">
         <v>513</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
working the order phase
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FE0C082-B12C-4E50-ADB6-759B5E7433B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66547465-A8B7-4578-BF32-9110156293E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="560">
   <si>
     <t>r20.1</t>
   </si>
@@ -2987,18 +2987,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.76  Friendly Action Phase&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.77   Random Events Phase&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r4.8  When Your Tanks Is Target&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>r18.0</t>
   </si>
   <si>
@@ -3687,6 +3675,108 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r23.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                         &lt;InlineUIContainer&gt;&lt;Image Name='c39ArtillerySupport'  Height='80' Width='80'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.76  Friendly Action Phase&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Friendly Action' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+once against each enemy unit on the Battle Board. Remove any knocked out units and record victory points on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. Place any Smoke markers generated due to dice roll.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2.) After all Friendly Action is resolved, go to the Random Events Phase 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.77' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.77   Random Events Phase&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) Roll once on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Random Events' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table based on the appropriate scenario.
+ And resolve the event.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2.) If the Battle Board is now empty of enemy units, the battle for the area is over. Mark the area on the Movement Board with a US Control makrer. Record Victory Points on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for capture territory. Return to the Prepare for Battle Step, i.e., 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+3.) If the battle does not end, return to the Smoke Depletion Phase, i.e., 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.71' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>r4.81</t>
+  </si>
+  <si>
+    <t>r4.82</t>
+  </si>
+  <si>
+    <t>r4.81.4</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.81  Attacks from Enemy Tanks, SPG, and AT Guns&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Hit' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to determine if your tank is hit. If the shot misses, continue resolving Enemy Actions per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. If it hits, go to step 2.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Hit Location' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to determine where your tank is hit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+3.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Kill' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to determine if the shell penetrates your tank. If no penetration, continue resolving Enemy Actions per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+If shell penetrates, go to step &lt;InlineUIContainer&gt;&lt;Button Content='r4.81.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.8  When Your Tanks Is Target&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.81' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attacks from Enemy Tanks, SPG, and AT Guns&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.82' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attacks from LW, MG, PSW, and SPW Units&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.81.4  Your Tank is Knocked Out&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+a.) Roll for explosion on the Tank 
+&lt;InlineUIContainer&gt;&lt;Button Content='Explosion' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. 
+If the tank exploses, the entire crew is killed. Go to Evening Debriefing
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.95' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+b.) Roll for crew casualties on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+c.) Surviving crewman roll for escape on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Bail Out' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+d.) Roll for crew rescues on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. See 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+e.) Roll on the  
+&lt;InlineUIContainer&gt;&lt;Button Content='Brew Up' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table to 
+see if the tank burns. If it burns, all crewmen still inside are killed. If it does not burn, all crewmen are automatically rescued with no chance of wounds.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+f.) Record crew casualties and how the tank was destroyed in the notes ection of the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+g.) The engagement ends with destruction of your tank. Go to the Evening Debriefing phase per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.82  Attacks from LW, MG, PSW, and SPW Units&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) If there is no effect, go back to 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; and continue resolving Enemy Actions.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2.) If your tank is hit, note any damage on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+Roll for possible hit crewmen on the 
+After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r19.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Continue resolving Enemy Actions.</t>
   </si>
 </sst>
 </file>
@@ -4059,10 +4149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B365"/>
+  <dimension ref="A1:B368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A254" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B254" sqref="B254"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4292,7 +4382,7 @@
         <v>137</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4300,7 +4390,7 @@
         <v>138</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4308,7 +4398,7 @@
         <v>139</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4332,7 +4422,7 @@
         <v>236</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4364,7 +4454,7 @@
         <v>240</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4380,7 +4470,7 @@
         <v>462</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4388,7 +4478,7 @@
         <v>463</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4396,7 +4486,7 @@
         <v>464</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -4412,1888 +4502,1912 @@
         <v>466</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>467</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>468</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>469</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>555</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
+    <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B54" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
+    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+    <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B58" s="2" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B62" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="64" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="69" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+    <row r="72" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="73" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+    <row r="74" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B74" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B75" s="2" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B76" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+    <row r="78" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B79" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
+    <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B81" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B82" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+    <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B86" s="2" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B87" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B88" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="92" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>320</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B100" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+    <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B101" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+    <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B102" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+    <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B103" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+    <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+      <c r="B104" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+    <row r="107" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+    <row r="108" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="109" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
+    <row r="110" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+    <row r="111" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
+    <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B112" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
+    <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
+    <row r="114" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
         <v>350</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
+    <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
+    <row r="116" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
         <v>352</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
+    <row r="117" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B117" s="2" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
+    <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
         <v>353</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
+    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
+    <row r="120" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B120" s="2" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
+    <row r="121" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
         <v>356</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
+    <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B122" s="2" t="s">
         <v>378</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A121" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A122" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
+    <row r="129" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
+      <c r="B129" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
+    <row r="131" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
+    <row r="132" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B132" s="2" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
+    <row r="133" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
         <v>392</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B133" s="2" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+    <row r="134" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B134" s="2" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
+    <row r="135" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B135" s="2" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
+    <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B136" s="2" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
+    <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
+    <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B142" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A140" s="5" t="s">
+    <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
         <v>412</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B143" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
+    <row r="144" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
+    <row r="145" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
+    <row r="146" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
+    <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B147" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
+    <row r="148" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B153" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
+    <row r="154" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B154" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
+    <row r="155" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B155" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A153" s="5" t="s">
+    <row r="156" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B156" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
+    <row r="157" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
+    <row r="158" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
+    <row r="159" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
+    <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B160" s="2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
+    <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B161" s="2" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
+    <row r="162" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
         <v>430</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
+      <c r="B162" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
+    <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B164" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
+    <row r="165" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
         <v>433</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B165" s="2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A163" s="5" t="s">
+    <row r="166" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B166" s="2" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
+    <row r="167" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
         <v>438</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B167" s="2" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A165" s="5" t="s">
+    <row r="168" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B168" s="2" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
+    <row r="169" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
         <v>435</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B169" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
+    <row r="170" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
         <v>437</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B170" s="2" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
+    <row r="171" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B171" s="2" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
+    <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B172" s="2" t="s">
         <v>456</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A172" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
         <v>424</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B176" s="2" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
+    <row r="177" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
         <v>425</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
+    <row r="178" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B178" s="2" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A176" s="5" t="s">
+    <row r="179" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
         <v>427</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B179" s="2" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
+    <row r="180" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B180" s="2" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A178" s="5" t="s">
+    <row r="181" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
         <v>429</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B181" s="2" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A179" s="5" t="s">
+    <row r="182" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B182" s="2" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
+    <row r="183" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B183" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A181" s="5" t="s">
+    <row r="184" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B184" s="2" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A182" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A183" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A187" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B188" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A186" s="5" t="s">
+    <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B189" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A187" s="5" t="s">
+    <row r="190" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B190" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A188" s="5" t="s">
+    <row r="191" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B191" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A189" s="5" t="s">
+    <row r="192" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B192" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A190" s="5" t="s">
+    <row r="193" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A191" s="5" t="s">
+      <c r="B193" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B194" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
+    <row r="195" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B195" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A193" s="5" t="s">
+    <row r="196" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B196" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A194" s="5" t="s">
+    <row r="197" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B197" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A195" s="5" t="s">
+    <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A198" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B198" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
+    <row r="199" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A199" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B199" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A197" s="5" t="s">
+    <row r="200" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A200" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="B200" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A198" s="5" t="s">
+    <row r="201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A201" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B201" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A199" s="5" t="s">
+    <row r="202" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B202" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A200" s="5" t="s">
+    <row r="203" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B200" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A201" s="5" t="s">
+      <c r="B203" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A202" s="5" t="s">
+      <c r="B204" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A203" s="5" t="s">
+      <c r="B205" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A206" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B203" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A204" s="5" t="s">
+      <c r="B206" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A205" s="5" t="s">
+      <c r="B209" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
         <v>475</v>
       </c>
-      <c r="B205" s="2" t="s">
+      <c r="B210" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="206" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A206" s="5" t="s">
+      <c r="B211" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A212" s="5" t="s">
         <v>477</v>
       </c>
-      <c r="B206" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A207" s="5" t="s">
+      <c r="B212" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
         <v>478</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B213" s="2" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A208" s="5" t="s">
+    <row r="214" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
         <v>479</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B214" s="2" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A209" s="5" t="s">
-        <v>480</v>
-      </c>
-      <c r="B209" s="2" t="s">
+    <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A215" s="5" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A210" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="B210" s="2" t="s">
+      <c r="B215" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A216" s="5" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A211" s="5" t="s">
-        <v>482</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A212" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A213" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A214" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A215" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A216" s="5" t="s">
-        <v>497</v>
-      </c>
       <c r="B216" s="2" t="s">
-        <v>500</v>
+        <v>543</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A218" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A219" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>495</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A218" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="5" t="s">
+    </row>
+    <row r="222" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="B222" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A220" s="5" t="s">
+    <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B220" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A221" s="5" t="s">
+      <c r="B223" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A224" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B221" s="2" t="s">
+      <c r="B224" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="5" t="s">
+    <row r="225" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B222" s="2" t="s">
+      <c r="B225" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A223" s="5" t="s">
+    <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A226" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B223" s="2" t="s">
+      <c r="B226" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="5" t="s">
+    <row r="227" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="B227" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A225" s="5" t="s">
+    <row r="228" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A228" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B225" s="2" t="s">
+      <c r="B228" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A226" s="5" t="s">
+    <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A229" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B226" s="2" t="s">
+      <c r="B229" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A227" s="5" t="s">
+    <row r="230" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A230" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B227" s="2" t="s">
+      <c r="B230" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="5" t="s">
+    <row r="231" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B228" s="2" t="s">
+      <c r="B231" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A229" s="5" t="s">
+    <row r="232" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A232" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="B232" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230" s="5" t="s">
+    <row r="233" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A233" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B230" s="2" t="s">
+      <c r="B233" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="5" t="s">
+    <row r="234" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B234" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A232" s="5" t="s">
+    <row r="235" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A235" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B232" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A233" s="5" t="s">
+      <c r="B235" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A236" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B233" s="2" t="s">
+      <c r="B236" s="2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A236" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A239" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="B240" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="5" t="s">
+    <row r="241" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="B241" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A239" s="5" t="s">
+    <row r="242" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A242" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B242" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="5" t="s">
+    <row r="243" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="B243" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A241" s="5" t="s">
+    <row r="244" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B244" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A242" s="5" t="s">
+    <row r="245" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A245" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B242" s="2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="5" t="s">
+      <c r="B245" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B243" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="5" t="s">
+      <c r="B246" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B247" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A245" s="1" t="s">
+    <row r="248" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B245" s="3" t="s">
+      <c r="B248" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A246" s="1" t="s">
+    <row r="249" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A249" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B246" s="3" t="s">
+      <c r="B249" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A247" s="1" t="s">
+    <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B247" s="3" t="s">
+      <c r="B250" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
+    <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A251" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B248" s="3" t="s">
+      <c r="B251" s="3" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B249" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B250" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>241</v>
+        <v>169</v>
       </c>
     </row>
     <row r="253" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B253" s="3" t="s">
+      <c r="B256" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
+    <row r="257" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B254" s="3" t="s">
+      <c r="B257" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
+    <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B255" s="3" t="s">
+      <c r="B258" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
+    <row r="259" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B256" s="3" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
+      <c r="B259" s="3" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B257" s="3" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+      <c r="B260" s="3" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B258" s="3" t="s">
+      <c r="B261" s="3" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="B259" s="3" t="s">
+    <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="B264" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="B260" s="3" t="s">
+      <c r="B279" s="3" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A266" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A267" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A268" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B268" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
-        <v>514</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A273" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A274" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A275" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A276" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A277" s="1" t="s">
+      <c r="B280" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="B277" s="3" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B286" s="4"/>
-    </row>
-    <row r="365" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B289" s="4"/>
+    </row>
+    <row r="368" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A293:B468">
-    <sortCondition ref="A293:A468"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A296:B471">
+    <sortCondition ref="A296:A471"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish rules for fight sequence
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66547465-A8B7-4578-BF32-9110156293E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{702B8CB3-66AE-4173-A9D9-4BC1A2382666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="570">
   <si>
     <t>r20.1</t>
   </si>
@@ -523,15 +524,6 @@
 -- Extra main gun and MG ammo could be stuffed into the tank if desired, but at the cost of increased crew discomfort and danger. See 
 &lt;InlineUIContainer&gt;&lt;Button Content='Brew Up' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  and Tank 
 &lt;InlineUIContainer&gt;&lt;Button Content='Explosion' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tables.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r16.23 Ammo Ready Rack&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-On the Tank Card, mark the number and types of rounds loaded into your ready rack with the Rounds Left markers. Reloading from the ready rack during battle increases the chance of achieving 
-&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-additional attacks. Each Sherman variant has a ready rack that cannot be exceeded.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-             &lt;InlineUIContainer&gt;&lt;Image Name='ReadyRack'  Height='270' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r16.22  Extra Ammo &lt;/Bold&gt; 
@@ -2238,16 +2230,6 @@
      &lt;InlineUIContainer&gt;&lt;Image Name='c102SmokeHit'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r9.4 Rate of Fire&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Achieving Rate of Fire allows for your crew to immediately fire another shot from the main gun. When a To Hit roll is made firing the main gun, the number rolled also deteremines whether the gun has acheived Rate of Fire.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the roll is low enough (30 or less for a 75mm gun and 20 or less for a 76L mm gun), you may immediately elect to fire again. You can continue to fire again until either the Rate of Fire roll is not acheived or the ammo runs out.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rate of Fire Modifiers&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r9.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Successive Rate of Fire</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r9.41 Rate of Fire Modifiers&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The 
@@ -2983,10 +2965,6 @@
     <t>r4.8</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.74  Crew Actions Phase&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
-  </si>
-  <si>
     <t>r18.0</t>
   </si>
   <si>
@@ -3712,24 +3690,6 @@
     <t>r4.81.4</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.81  Attacks from Enemy Tanks, SPG, and AT Guns&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-1.) Roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Hit' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
-to determine if your tank is hit. If the shot misses, continue resolving Enemy Actions per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. If it hits, go to step 2.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-2.) Roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Hit Location' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
-to determine where your tank is hit.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-3.) Roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Kill' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
-to determine if the shell penetrates your tank. If no penetration, continue resolving Enemy Actions per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-If shell penetrates, go to step &lt;InlineUIContainer&gt;&lt;Button Content='r4.81.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.8  When Your Tanks Is Target&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.81' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Attacks from Enemy Tanks, SPG, and AT Guns&lt;LineBreak/&gt;
@@ -3777,6 +3737,127 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r19.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Continue resolving Enemy Actions.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.81  Attacks from Enemy Tanks, SPG, and AT Guns&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+1.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Hit' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to determine if your tank is hit. If the shot misses, continue resolving Enemy Actions per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. If it hits, go to step 2.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+2.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Hit Location Tank' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to determine where your tank is hit.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+3.) Roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy AP To Kill' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+to determine if the shell penetrates your tank. If no penetration, continue resolving Enemy Actions per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+If shell penetrates, go to step &lt;InlineUIContainer&gt;&lt;Button Content='r4.81.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>r4.74.1</t>
+  </si>
+  <si>
+    <t>r4.74.2</t>
+  </si>
+  <si>
+    <t>r4.74.3</t>
+  </si>
+  <si>
+    <t>r4.74.4</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.74.1  Crew Actions Phase - Tank Movement&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Resolve on 
+&lt;InlineUIContainer&gt;&lt;Button Content='Movement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank movement may require the shifting of enemy units on the Battle Board.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.74  Crew Actions Phase&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tank Movement&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tank Main Gun Fire&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tank MG Fire&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.74.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Miscellaenous Actions&lt;LineBreak/&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+After all crew actions are resolved, go to the Enemy Action Phase, step 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.75' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r9.4 Rate of Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Achieving Rate of Fire allows for your crew to immediately fire another shot from the main gun. When a To Hit roll is made firing the main gun, the number rolled also deteremines whether the gun has acheived Rate of Fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the roll is low enough (30 or less for a 75mm gun and 20 or less for a 76L mm gun), you may immediately elect to fire again. You can continue to fire again until either the Rate of Fire roll is not acheived or the ammo runs out.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Rate of Fire Modifiers&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Successive Rate of Fire</t>
+  </si>
+  <si>
+    <t>r16.3</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r16.3 Machine Gun (MG) Ammo (OPTIONAL)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+All rules dealing with MG ammunition should be considered optional and be followed only by choice. For most players, the additional problems posed by the consideration of MG ammo are not worth the record keeping involved. Continue to check for MG malfunctions, but otherwise assume there is sufficient MG ammo on hand for all firing.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r16.23 Ammo Ready Rack&lt;/Bold&gt; B5
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+On the Tank Card, mark the number and types of rounds loaded into your ready rack with the Rounds Left markers. Reloading from the ready rack during battle increases the chance of achieving 
+&lt;InlineUIContainer&gt;&lt;Button Content='Rate of Fire' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+additional attacks. Each Sherman variant has a ready rack that cannot be exceeded.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+             &lt;InlineUIContainer&gt;&lt;Image Name='ReadyRack'  Height='270' Width='350'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.74.3  Crew Actions Phase - Tank MG Fire&lt;/Bold&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r10.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+a.) Mark any Advancing Fire and consult the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Sherman MG' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+for ammo use and gun malfunctions.&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+b.) Conduct fire against spotted targets on the  same table. Mark off ammo used per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r16.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+c.) Remove knocked out enemy units from the board and record the victory points for their destruction on the After Action Report.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r4.74.4  Crew Actions Phase - Miscellaenous Actions&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+a.) Replace periscopes: Mark off a periscope replacement on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for each replacement. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+b.) Attempt to repair guns that have malfunctioned by consulting the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+c.) Fire 2" smoke mortar. Place Smoke marker in target zone and mark off one smoke bomb from the After Action Report per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+d.) Throw smoke grenade. Place smoke marker on your tank and mark off one smoke grenade from the After Action Report per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.74.2  Crew Actions Phase - Tank Main Gun Fire&lt;/Bold&gt;  
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+a.) Mark off ammo on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.&lt;LineBreak/&gt;
+b.) Consult the correct 
+&lt;InlineUIContainer&gt;&lt;Button Content='To Hit Target' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table for gun to determine if target is hit. Mark a hit by placing either an HE or AP hit marker on the target.&lt;LineBreak/&gt;
+c.) If the Rate of Fire is possible per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r9.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+gun may be fired again and again. Mark off ammo for each shot and mark any hits.
+&lt;LineBreak/&gt;
+d.) After all possible shots are fired, roll for each hit roll on the correct To Kill Table:&lt;LineBreak/&gt;
+   -- &lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (75)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+   -- &lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (76L)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+   -- &lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (76LL)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+   -- &lt;InlineUIContainer&gt;&lt;Button Content='HE To Kill (75)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+   -- &lt;InlineUIContainer&gt;&lt;Button Content='HE To Kill (76)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
+e.) Remove knocked out enemy units from the board and record the victory points for their destruction on the After Action Report.</t>
   </si>
 </sst>
 </file>
@@ -4149,10 +4230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
-  <dimension ref="A1:B368"/>
+  <dimension ref="A1:B373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4198,7 +4279,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4238,7 +4319,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4262,7 +4343,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4270,2144 +4351,2184 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>559</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>560</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="B47" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="B48" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="B49" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>553</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="B53" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>554</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>181</v>
+        <v>407</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="B62" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="B63" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B67" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
+    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B68" s="2" t="s">
+    </row>
+    <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+      <c r="B73" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B74" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="76" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="B76" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B77" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B80" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B76" s="2" t="s">
+      <c r="B81" s="2" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B84" s="2" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
-        <v>288</v>
-      </c>
       <c r="B85" s="2" t="s">
-        <v>316</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>317</v>
+        <v>330</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+      <c r="B92" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B93" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+      <c r="B94" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B95" s="2" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+    <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B96" s="2" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B103" s="2" t="s">
+    </row>
+    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+      <c r="B108" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+      <c r="B109" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>347</v>
-      </c>
       <c r="B111" s="2" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>348</v>
+        <v>311</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A116" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A117" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A118" s="5" t="s">
-        <v>353</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A119" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A120" s="5" t="s">
-        <v>355</v>
-      </c>
       <c r="B120" s="2" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B127" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A123" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A124" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="B124" s="2" t="s">
+    <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B130" s="2" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A125" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B125" s="2" t="s">
+    <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B131" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A126" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A127" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A128" s="5" t="s">
+    <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A132" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B128" s="2" t="s">
+    </row>
+    <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A129" s="5" t="s">
+      <c r="B134" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A130" s="5" t="s">
+      <c r="B135" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A131" s="5" t="s">
+      <c r="B136" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
         <v>390</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A132" s="5" t="s">
+      <c r="B137" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
         <v>391</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A133" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A134" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A135" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A136" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A137" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B137" s="2" t="s">
+      <c r="B138" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A138" s="5" t="s">
+    <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B139" s="2" t="s">
         <v>402</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A141" s="5" t="s">
+      <c r="B142" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A142" s="5" t="s">
+      <c r="B147" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A143" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="B143" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A144" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A145" s="5" t="s">
+    <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="330" x14ac:dyDescent="0.25">
-      <c r="A146" s="5" t="s">
+      <c r="B150" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A147" s="5" t="s">
+      <c r="B151" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="B147" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="225" x14ac:dyDescent="0.25">
-      <c r="A148" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A149" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A150" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A151" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A152" s="5" t="s">
-        <v>249</v>
-      </c>
       <c r="B152" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B158" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A154" s="5" t="s">
+    <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="B154" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A155" s="5" t="s">
+      <c r="B159" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B160" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="B161" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A156" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A157" s="5" t="s">
+    <row r="162" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="B157" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A158" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A159" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A160" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A161" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A162" s="5" t="s">
-        <v>430</v>
-      </c>
       <c r="B162" s="2" t="s">
-        <v>539</v>
+        <v>271</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B169" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A164" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="B164" s="2" t="s">
+    <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A173" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A165" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>434</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A167" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A168" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A169" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="B169" s="2" t="s">
+    <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A170" s="5" t="s">
-        <v>437</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A171" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A172" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="B172" s="2" t="s">
+    <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>456</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A173" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A174" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A175" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A176" s="5" t="s">
-        <v>424</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A177" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A178" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A179" s="5" t="s">
-        <v>427</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A180" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A181" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A182" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A183" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A184" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A185" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A186" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A188" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A189" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A190" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A191" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A188" s="5" t="s">
+      <c r="B191" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A192" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A189" s="5" t="s">
+      <c r="B192" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A193" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A190" s="5" t="s">
+      <c r="B193" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A194" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A195" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A196" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A191" s="5" t="s">
+      <c r="B196" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A197" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A192" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A193" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A194" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B194" s="2" t="s">
+      <c r="B197" s="2" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A195" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A196" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A197" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A202" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A203" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A204" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A205" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A206" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A207" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="B207" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A202" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B202" s="2" t="s">
+    <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="203" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A203" s="5" t="s">
+      <c r="B208" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B203" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A204" s="5" t="s">
+      <c r="B209" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B204" s="2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A205" s="5" t="s">
+      <c r="B210" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A206" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A207" s="5" t="s">
+      <c r="B211" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A212" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
         <v>471</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B214" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A215" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A216" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A217" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A218" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A219" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A224" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A208" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A209" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A210" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A211" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A212" s="5" t="s">
-        <v>477</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A213" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A214" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A215" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A216" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A217" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A218" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A219" s="5" t="s">
-        <v>494</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A220" s="5" t="s">
-        <v>495</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>499</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A221" s="5" t="s">
+      <c r="B225" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A223" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A224" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>34</v>
+        <v>493</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>62</v>
+        <v>478</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A231" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A233" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A234" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="B234" s="2" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A230" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A232" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B232" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A233" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A237" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A238" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A240" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B235" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A236" s="5" t="s">
+      <c r="B240" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B236" s="2" t="s">
+      <c r="B241" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="5" t="s">
+    <row r="242" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B237" s="2" t="s">
+      <c r="B242" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="5" t="s">
+    <row r="243" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B238" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A239" s="5" t="s">
+      <c r="B243" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B244" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="5" t="s">
+    <row r="245" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B240" s="2" t="s">
+      <c r="B245" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="5" t="s">
+    <row r="246" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B241" s="2" t="s">
+      <c r="B246" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="210" x14ac:dyDescent="0.25">
-      <c r="A242" s="5" t="s">
+    <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A247" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B242" s="2" t="s">
+      <c r="B247" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="5" t="s">
+    <row r="248" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B243" s="2" t="s">
+      <c r="B248" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A244" s="5" t="s">
+    <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A249" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B244" s="2" t="s">
+      <c r="B249" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="255" x14ac:dyDescent="0.25">
-      <c r="A245" s="5" t="s">
+    <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A250" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B245" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="5" t="s">
+      <c r="B250" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B246" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="5" t="s">
+      <c r="B251" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B247" s="2" t="s">
+      <c r="B252" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A248" s="1" t="s">
+    <row r="253" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A253" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B248" s="3" t="s">
+      <c r="B253" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B254" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A249" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B249" s="3" t="s">
+    <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A255" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B255" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A250" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B250" s="3" t="s">
+    <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B256" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A251" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B251" s="3" t="s">
+    <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="252" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A252" s="1" t="s">
+      <c r="B257" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B252" s="3" t="s">
+      <c r="B258" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A253" s="1" t="s">
+    <row r="259" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B253" s="3" t="s">
+      <c r="B262" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A254" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A255" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A256" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B256" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" ht="300" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+    <row r="264" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B258" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A259" s="1" t="s">
+      <c r="B264" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B259" s="3" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A260" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A261" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A262" s="1" t="s">
+      <c r="B266" s="3" t="s">
         <v>519</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B264" s="3" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A265" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A266" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>184</v>
+        <v>516</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B271" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B268" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A269" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B269" s="3" t="s">
+    </row>
+    <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B272" s="3" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A270" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B273" s="3" t="s">
+      <c r="B280" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="274" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A274" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A275" s="1" t="s">
+      <c r="B282" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="B275" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A276" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A277" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A278" s="1" t="s">
+    </row>
+    <row r="283" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B283" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="B278" s="3" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A279" s="1" t="s">
+    </row>
+    <row r="284" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B284" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="B279" s="3" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A280" s="1" t="s">
+    </row>
+    <row r="285" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B285" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="B280" s="3" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="289" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B289" s="4"/>
-    </row>
-    <row r="368" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B294" s="4"/>
+    </row>
+    <row r="373" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A296:B471">
-    <sortCondition ref="A296:A471"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A301:B476">
+    <sortCondition ref="A301:A476"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding rules for firefly
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{702B8CB3-66AE-4173-A9D9-4BC1A2382666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2009_{8919D7A6-C2E9-41D4-AB10-BC5CA632ACAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="580">
   <si>
     <t>r20.1</t>
   </si>
@@ -3858,6 +3858,60 @@
    -- &lt;InlineUIContainer&gt;&lt;Button Content='HE To Kill (75)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
    -- &lt;InlineUIContainer&gt;&lt;Button Content='HE To Kill (76)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;&lt;LineBreak/&gt;
 e.) Remove knocked out enemy units from the board and record the victory points for their destruction on the After Action Report.</t>
+  </si>
+  <si>
+    <t>r30.0</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r30.0 British Firefly Variant&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Sherman Firefly was a British variant of the Sherman tank notable become of its gun, the British 17 pounder (a 76LL). The gun fired a 17 pound shell at a very high velocity, and was capable of penetrating all but the thickest German armor. Although this gun was offered to the US, for various reasons, it was never was used by US troops.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+For historical interest and comparison, a Tank Card (#18) and an 
+&lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (76LL)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table have been included for one of the Firefly models. This allows you to experience commanding one of the best Sherman variants, even though it was never used by the 4th Armored Division.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When employing the Firefly variant, make the following adjustments to the normal rules at the noted step in the Sequence of Play:&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r30.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Firefly Crew&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r30.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Firefly Terrain&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r30.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Firefly To Hit&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r30.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; German Tactics against Firefly</t>
+  </si>
+  <si>
+    <t>r30.1</t>
+  </si>
+  <si>
+    <t>r30.2</t>
+  </si>
+  <si>
+    <t>r30.3</t>
+  </si>
+  <si>
+    <t>r30.4</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r30.4 German Tactics against Firefly&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r30.1 Firefly Crew&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Firefly crew consists of only four men as the assistant driver is eliminated to accommodate the extra large rounds of ammo for the 76LL gun. There is no Bow MG.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r30.2 Firefly Terrain&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The Firefly tank begins all engagements stopped/hulled down to provide cover fire. Mark the tank with the Hull down marker.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r30.3 Firefly To Hit&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Use the 
+&lt;InlineUIContainer&gt;&lt;Button Content='AP To Hit (76LL)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+when firing the 76LL gun. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Use the 
+&lt;InlineUIContainer&gt;&lt;Button Content='AP To Kill (76LL)' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table 
+when firing the 76LL gun. </t>
   </si>
 </sst>
 </file>
@@ -4232,8 +4286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B373"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A284" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B289" sqref="B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6522,7 +6576,47 @@
         <v>528</v>
       </c>
     </row>
-    <row r="294" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="B290" s="3" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B294" s="4"/>
     </row>
     <row r="373" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Display enemy units moved to Move Board
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D87718F0-10A1-498C-A333-9A8351B80761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0660221-50F1-40A9-AE2E-507F17DD6016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -2745,21 +2745,6 @@
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c13Moving'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r13.0 Enemy Action &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the enemy action phase of the Battle Round Sequence, refer to the respective table: 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or 
-&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Roll for each enemy unit on the Battle Board. Enemy units will either do nothing, move to another zone (or off the board), or fire their weapons.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Movement&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Infantry&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r13.12 Move Backward &lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 A unit moving backward remains in the same sector, but moves one zone away from the hub. A unit already at long range in Sectors 4-5, 6-8, or 9-10 is removed from play.
@@ -3491,21 +3476,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Regardless of ambush status, continue with 
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.7' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; to start the fight.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r13.1 Movement &lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units move in four directions: &lt;LineBreak/&gt;
-F = Forward&lt;LineBreak/&gt;
-B = Backward&lt;LineBreak/&gt;
-L = Left&lt;LineBreak/&gt;
-R = Right
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Forward&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Backward&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Right or Left&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Into US Control &lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Moving Marker</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r4.75  Enemy Actions Phase&lt;/Bold&gt;
@@ -4030,6 +4000,36 @@
 When rolling for non-Ambush Enemy Action; enemy tanks, SPGs, and AT guns fir at your tank on rolls 91-100 in addition to other rolls.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 This represents the German tactic of trying to knock out Firefly tanks as soon as they were identified.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.0 Enemy Action &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the enemy action phase of the Battle Round Sequence, refer to the respective table: 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Advance' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Battle' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, or 
+&lt;InlineUIContainer&gt;&lt;Button Content='Enemy Counterattack' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Roll for each enemy unit on the Battle Board. Enemy units will either do nothing, move to another zone (or off the board), or fire their weapons.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Movement&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Infantry&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Any Tank&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Versus Your Tank</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r13.1 Movement &lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units move in four directions: &lt;LineBreak/&gt;
+F = Forward&lt;LineBreak/&gt;
+B = Backward&lt;LineBreak/&gt;
+L = Left&lt;LineBreak/&gt;
+R = Right
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Forward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Backward&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Right or Left&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Move Into US Control &lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r13.15' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Moving Marker</t>
   </si>
 </sst>
 </file>
@@ -4404,8 +4404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A262" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B167" sqref="B167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4635,7 +4635,7 @@
         <v>136</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4643,7 +4643,7 @@
         <v>137</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4651,7 +4651,7 @@
         <v>138</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4675,7 +4675,7 @@
         <v>235</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4707,135 +4707,135 @@
         <v>239</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>550</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4963,7 +4963,7 @@
         <v>218</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5275,7 +5275,7 @@
         <v>307</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5387,7 +5387,7 @@
         <v>352</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5475,7 +5475,7 @@
         <v>386</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5731,7 +5731,7 @@
         <v>382</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>441</v>
+        <v>598</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5739,7 +5739,7 @@
         <v>428</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>536</v>
+        <v>599</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5755,7 +5755,7 @@
         <v>430</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5787,7 +5787,7 @@
         <v>434</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5795,7 +5795,7 @@
         <v>433</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5803,7 +5803,7 @@
         <v>435</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5819,7 +5819,7 @@
         <v>418</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5827,7 +5827,7 @@
         <v>419</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5835,7 +5835,7 @@
         <v>420</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5843,7 +5843,7 @@
         <v>421</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5851,7 +5851,7 @@
         <v>422</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5859,7 +5859,7 @@
         <v>423</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5867,7 +5867,7 @@
         <v>424</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5875,7 +5875,7 @@
         <v>425</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5883,7 +5883,7 @@
         <v>426</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5891,15 +5891,15 @@
         <v>427</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5955,15 +5955,15 @@
         <v>83</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -5995,7 +5995,7 @@
         <v>103</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6075,7 +6075,7 @@
         <v>121</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6083,7 +6083,7 @@
         <v>122</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6091,7 +6091,7 @@
         <v>123</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6099,127 +6099,127 @@
         <v>124</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
+        <v>468</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>469</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6235,7 +6235,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6331,7 +6331,7 @@
         <v>71</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6355,7 +6355,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6411,7 +6411,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6419,7 +6419,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6523,7 +6523,7 @@
         <v>163</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6531,7 +6531,7 @@
         <v>167</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6539,31 +6539,31 @@
         <v>164</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6624,194 +6624,194 @@
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B282" s="3" t="s">
         <v>510</v>
-      </c>
-      <c r="B282" s="3" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="300" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B300" s="3" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
close to finishing ReadXml()
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DAB1277B-DCF5-4D60-8164-232973742C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ACF4C0-F88A-49D5-8D89-CE69E7AB23F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
@@ -298,24 +298,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r1.0 Introduction&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;Bold&gt;PATTON'S BEST&lt;/Bold&gt; recreates the World War II campaing in nothern Europe through the eyes of a tank commander in George Patton's most famous unit, the 4th Armored Division. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Patton's Best is designed as a solitaire game, with you acting as the commander of a Sherman tank. As the commander, you control the actions of your crew, and through them,
- fight and maneuver your tank. The actions of the enemy tanks and troops, as well as friendly forces  on your side, are randomly generated by various game aides and tables. 
-Each scenario consists of a single engagement or a day  of movement and battle. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-However, the game realizes its full interest when played as a campaign which allows you to take part in every historical battle of the 4th Armored Division. 
-You and your crew can witness and participate in the great drives across Europe, the battles for the Siegfried Line, the relief of Bastogne, and the crossing of the Rhine. Further details here:
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r2.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Game Equipment&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r3.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Game Tables&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sequence of Play
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Additional Rules can be viewed by selecting the &lt;Bold&gt;Help | Show Rules..."&lt;/Bold&gt; menu.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r19.11 Exploding Tank&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;First determine if the tank explodes by consulting the Tank 
 &lt;InlineUIContainer&gt;&lt;Button Content='Explosion' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table. All crewmen of an exploding tank are killed</t>
@@ -4021,6 +4003,24 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; .
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c49CDirectMainGunFire'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r1.0 Introduction&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;Bold&gt;PATTON'S BEST&lt;/Bold&gt; recreates the World War II campaign in nothern Europe through the eyes of a tank commander in George Patton's most famous unit, the 4th Armored Division. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Patton's Best is designed as a solitaire game, with you acting as the commander of a Sherman tank. As the commander, you control the actions of your crew, and through them,
+ fight and maneuver your tank. The actions of the enemy tanks and troops, as well as friendly forces  on your side, are randomly generated by various game aides and tables. 
+Each scenario consists of a single engagement or a day  of movement and battle. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+However, the game realizes its full interest when played as a campaign which allows you to take part in every historical battle of the 4th Armored Division. 
+You and your crew can witness and participate in the great drives across Europe, the battles for the Siegfried Line, the relief of Bastogne, and the crossing of the Rhine. Further details here:
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r2.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Game Equipment&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r3.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Game Tables&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sequence of Play
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Additional Rules can be viewed by selecting the &lt;Bold&gt;Help | Show Rules..."&lt;/Bold&gt; menu.</t>
   </si>
 </sst>
 </file>
@@ -4395,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,7 +4410,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4482,7 +4482,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4498,7 +4498,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4506,7 +4506,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -4514,495 +4514,495 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5010,7 +5010,7 @@
         <v>27</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5018,7 +5018,7 @@
         <v>28</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5026,1191 +5026,1191 @@
         <v>29</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="196" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="204" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="205" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6218,7 +6218,7 @@
         <v>30</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="228" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -6226,7 +6226,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6234,7 +6234,7 @@
         <v>32</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="230" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
@@ -6242,7 +6242,7 @@
         <v>33</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="231" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6250,7 +6250,7 @@
         <v>34</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
@@ -6266,7 +6266,7 @@
         <v>36</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="234" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6282,7 +6282,7 @@
         <v>40</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
@@ -6290,7 +6290,7 @@
         <v>38</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="237" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6298,7 +6298,7 @@
         <v>42</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="238" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6306,7 +6306,7 @@
         <v>43</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="239" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
@@ -6319,10 +6319,10 @@
     </row>
     <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6330,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="242" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
@@ -6346,7 +6346,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6378,7 +6378,7 @@
         <v>4</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="248" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -6386,7 +6386,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6394,7 +6394,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6402,7 +6402,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6410,7 +6410,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6423,378 +6423,378 @@
     </row>
     <row r="253" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="254" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="258" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="259" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="262" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="264" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="271" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="273" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="275" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="276" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>558</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
making progress on Loading Game
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ACF4C0-F88A-49D5-8D89-CE69E7AB23F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16130893-0820-40F5-A2C9-5066AC9E3A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -1315,21 +1315,6 @@
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c15OpenHatch'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r5.22 Action Boxes&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Adjacent to the overhead view of the tank, each crew position has a labeled action box:&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- C = Commander&lt;LineBreak/&gt;
- G = Gunner&lt;LineBreak/&gt;
- L = Loader&lt;LineBreak/&gt;
- D = Driver&lt;LineBreak/&gt;
- A = Assistant Criver&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-To order a crewman to perform an action, place the desired Action marker in the crewman&amp;apos;s box per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-The driver and loader automatically perform the actions Stop and Load, respectively, unless ordered otherwise.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Name='c59LChangeGunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r5.11 Battle Area&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 The Battle Area is a distorted circle centered on a hexagonal hub. The counter representing your Sherman tank is placed in this hub and remains there throughout play, changing only the direction it is facing. 
@@ -2436,15 +2421,6 @@
   </si>
   <si>
     <t>r11.12</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r2.12 Battle Board&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The battle board is an abstract display used to resolve engagements with enemy forces. Your tank is placed in the center of this display and the action of an engagement revolves 
-around it through the use of pieces representing enemy units and other informational markers. A detailed explanation is given in 
-&lt;InlineUIContainer&gt;&lt;Button Content='r5.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;B126
-                 &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r11.0 Sherman Movement&lt;/Bold&gt; 
@@ -4011,7 +3987,7 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Patton's Best is designed as a solitaire game, with you acting as the commander of a Sherman tank. As the commander, you control the actions of your crew, and through them,
  fight and maneuver your tank. The actions of the enemy tanks and troops, as well as friendly forces  on your side, are randomly generated by various game aides and tables. 
-Each scenario consists of a single engagement or a day  of movement and battle. 
+Each scenario consists of a single engagement or a day of movement and battle. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 However, the game realizes its full interest when played as a campaign which allows you to take part in every historical battle of the 4th Armored Division. 
 You and your crew can witness and participate in the great drives across Europe, the battles for the Siegfried Line, the relief of Bastogne, and the crossing of the Rhine. Further details here:
@@ -4021,6 +3997,30 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Sequence of Play
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Additional Rules can be viewed by selecting the &lt;Bold&gt;Help | Show Rules..."&lt;/Bold&gt; menu.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r2.12 Battle Board&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The battle board is an abstract display used to resolve engagements with enemy forces. Your tank is placed in the center of this display and the action of an engagement revolves 
+around it through the use of pieces representing enemy units and other informational markers. A detailed explanation is given in 
+&lt;InlineUIContainer&gt;&lt;Button Content='r5.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                &lt;InlineUIContainer&gt;&lt;Image Name='MapBattle'  Height='400' Width='400'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r5.22 Action Boxes&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Adjacent to the overhead view of the tank, each crew position has a labeled action box:&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ C = Commander&lt;LineBreak/&gt;
+ G = Gunner&lt;LineBreak/&gt;
+ L = Loader&lt;LineBreak/&gt;
+ D = Driver&lt;LineBreak/&gt;
+ A = Assistant Driver&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+To order a crewman to perform an action, place the desired Action marker in the crewman&amp;apos;s box per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+The driver and loader automatically perform the actions Stop and Load, respectively, unless ordered otherwise.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='c59LChangeGunLoad'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4395,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,7 +4410,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>396</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4482,7 +4482,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
         <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4655,178 +4655,178 @@
     </row>
     <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4842,7 +4842,7 @@
         <v>170</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4898,7 +4898,7 @@
         <v>205</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4922,7 +4922,7 @@
         <v>208</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4930,7 +4930,7 @@
         <v>209</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -4946,7 +4946,7 @@
         <v>213</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>220</v>
+        <v>597</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4954,7 +4954,7 @@
         <v>214</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4962,7 +4962,7 @@
         <v>215</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4970,7 +4970,7 @@
         <v>217</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5031,866 +5031,866 @@
     </row>
     <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="330" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5898,7 +5898,7 @@
         <v>72</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5946,15 +5946,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -5986,7 +5986,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6066,7 +6066,7 @@
         <v>117</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6074,7 +6074,7 @@
         <v>118</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6082,7 +6082,7 @@
         <v>119</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6090,127 +6090,127 @@
         <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>487</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6226,7 +6226,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6322,7 +6322,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6346,7 +6346,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6386,7 +6386,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6394,7 +6394,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6402,7 +6402,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6410,7 +6410,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6482,7 +6482,7 @@
         <v>154</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6498,7 +6498,7 @@
         <v>152</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6514,7 +6514,7 @@
         <v>159</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6522,7 +6522,7 @@
         <v>163</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6530,31 +6530,31 @@
         <v>160</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>507</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6615,186 +6615,186 @@
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B278" s="3" t="s">
         <v>499</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changes to support alerts
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15280A8B-BAF7-42FE-B11D-B4B126E1A5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3031562D-03BE-4081-9163-124F1CEBC554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -1542,13 +1542,6 @@
      &lt;InlineUIContainer&gt;&lt;Image Name='c82PzVIb'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r12.13 Truck&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Any medium truck of the period
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c88Truck' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r12.14 Panzerspahwagen (PSW)&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Armored scout car.
@@ -1601,30 +1594,6 @@
 Armored infantry vehicle, i.e., armored personnel carrier.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c90Spw251' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r12.1 Description&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Enemy units appear in two major types: vehicles and infantry. 
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Vehicle types are:&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Tanks&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Self Propelled Guns (SPGs)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Trucks&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Panzerspahwagen (PSW)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.15' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Schutzenpanzerwagen (SPW)&lt;LineBreak/&gt;
- &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Infantry types are:&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.16' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Light Weapons (LW)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.17' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Muchaine Gun (MG) Team&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r12.18' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Antitank (AT) Gun
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Tank, SPG, and AT guns are printed in black on their front side and red on their back side. When these units first appear, place them red side up. They remain on their red side until they are identified by spotting per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                 &lt;InlineUIContainer&gt;&lt;Image Name='c76UnidentifiedAtg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c77UnidentifiedSpg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c78UnidentifiedTank'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r12.32 Range&lt;/Bold&gt; 
@@ -3081,21 +3050,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Unidentified Tanks&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.42' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Crew Action Restrictions &lt;LineBreak/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r10.1 Description&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In addition to its main gun, the Sherman tank is armed with several machine guns (MGs). 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The .30 calibre bow MG is mounted in the front right hull and is fired by the assistant driver.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The .30 calibre co-axial MG is mounted in the turret front along the same axis as the main gun and is fired by the gunner.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The .50 calibre anti-aircraft (AA) MG is fixed to a pintle mount (post) on top of the turret and is fired by the commander. In some configurations, it can be fired by the loader.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Several hand held submachine guns (sub MGs) are carried in the turret and may be fired from open hatches.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c51FireCoaxialMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r20.12 Probability of Combat&lt;/Bold&gt;
@@ -4021,6 +3975,52 @@
 Consult the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Ammo' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
 Table for the amount of each type is available.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.1 Description&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Enemy units appear in two major types: vehicles and infantry. 
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Vehicle types are:&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Tanks&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Self Propelled Guns (SPGs)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.13' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Trucks&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.14' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Panzerspahwagen (PSW)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.15' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Schutzenpanzerwagen (SPW)&lt;LineBreak/&gt;
+ &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Infantry types are:&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.16' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Light Weapons (LW)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.17' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Machine Gun (MG) Team&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r12.18' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Antitank (AT) Gun
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tank, SPG, and AT guns are printed in black on their front side and red on their back side. When these units first appear, place them red side up. They remain on their red side until they are identified by spotting per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                 &lt;InlineUIContainer&gt;&lt;Image Name='c76UnidentifiedAtg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c77UnidentifiedSpg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c78UnidentifiedTank'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r10.1 Description&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In addition to its main gun, the Sherman tank is armed with several machine guns (MGs). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .30 calibre bow MG is mounted in the front right hull and is fired by the assistant driver.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .30 calibre co-axial MG is mounted in the turret front along the same axis as the main gun and is fired by the gunner.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The .50 calibre anti-aircraft (AA) MG is fixed to a pintle mount (post) on top of the turret and is fired by the commander. In some configurations, it can be fired by the loader.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Several hand held submachine guns (sub MGs) are carried in the turret and may be fired from open hatches.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c51GFireCoaxialMg'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.13 Truck&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Any medium truck of the period. Trucks require TO HIT roll for main gun but can also be targeted with MG fire.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c88Truck' Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4395,8 +4395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B191" sqref="B191"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,7 +4410,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4482,7 +4482,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
         <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4642,7 +4642,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4666,7 +4666,7 @@
         <v>229</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4698,135 +4698,135 @@
         <v>233</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4842,7 +4842,7 @@
         <v>169</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4946,7 +4946,7 @@
         <v>212</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4954,7 +4954,7 @@
         <v>213</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5031,562 +5031,562 @@
     </row>
     <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B132" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>492</v>
+        <v>596</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5602,7 +5602,7 @@
         <v>236</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>264</v>
+        <v>595</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5618,7 +5618,7 @@
         <v>238</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5626,7 +5626,7 @@
         <v>239</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>257</v>
+        <v>597</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5634,7 +5634,7 @@
         <v>240</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5642,7 +5642,7 @@
         <v>241</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5650,7 +5650,7 @@
         <v>242</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5658,7 +5658,7 @@
         <v>243</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5666,7 +5666,7 @@
         <v>244</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5698,7 +5698,7 @@
         <v>248</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5706,7 +5706,7 @@
         <v>249</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5714,183 +5714,183 @@
         <v>250</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5930,7 +5930,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5946,15 +5946,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -5986,7 +5986,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6066,7 +6066,7 @@
         <v>117</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6074,7 +6074,7 @@
         <v>118</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6082,7 +6082,7 @@
         <v>119</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6090,127 +6090,127 @@
         <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6226,7 +6226,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6322,7 +6322,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6346,7 +6346,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6386,7 +6386,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6394,7 +6394,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6402,7 +6402,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6410,7 +6410,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6498,7 +6498,7 @@
         <v>151</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6514,7 +6514,7 @@
         <v>158</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6522,7 +6522,7 @@
         <v>162</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6530,31 +6530,31 @@
         <v>159</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6615,186 +6615,186 @@
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B292" s="3" t="s">
         <v>509</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B293" s="3" t="s">
         <v>510</v>
-      </c>
-      <c r="B293" s="3" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B294" s="3" t="s">
         <v>511</v>
-      </c>
-      <c r="B294" s="3" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix  counterattack movement roll thread ending. added fixes to rules for fuel opion. Begin adding fuel option to option dialog.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9203FFFC-EB05-4906-862F-47A494472487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67A492B8-1C4D-4425-AC71-F37F9F1A0A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3175,27 +3175,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r29.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Battle Board Fuel Use</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r29.1 Movement Board Fuel Use&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Moving from one area to another on the Movement Board consumes 2 fuel units. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Successfully completing an ammo resupply operations refills the tank with fuel.  Put the fuel supply back to 25 units. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If your tank is out of fuel, assume the entire task force is out or low, and no movement on the Movement Board is possible until a successful ammo (and fuel) resupply occurs per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r29.2 Battle Board Fuel Use&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-While on the Battle Board, fuel is consumed during movement. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When the driver performs the actions Forward, Forward to Hull Down, Reversion, and Reverse to Hull Down, the number rolled on the color die determines if fuel is consumed.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the colored die is 1-3, mark off 1 unit of fuel. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A tank with no fuel may not perform the above movement actions, nor may the tank pivot.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.54.3  Call for Air Strike&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Call to hit an area adjacent to your task force. Consult the 
@@ -4021,6 +4000,27 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                            &lt;InlineUIContainer&gt;&lt;Image Name='c103Acquired1_0'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
      &lt;InlineUIContainer&gt;&lt;Image Name='c104Acquired2_0'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r29.1 Movement Board Fuel Use&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Moving from one area to another on the Movement Board consumes 2 fuel units. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Successfully completing an ammo resupply operations refills the tank with fuel.  Put the fuel supply back to 35 units. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If your tank is out of fuel, assume the entire task force is out or low, and no movement on the Movement Board is possible until a successful ammo (and fuel) resupply occurs per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.54.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r29.2 Battle Board Fuel Use&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+While on the Battle Board, fuel is consumed during movement. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When the driver performs the actions Forward, Forward to Hull Down, Reverse, and Reverse to Hull Down, the number rolled on the color die determines if fuel is consumed.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the colored die is 1-3, mark off 1 unit of fuel. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A tank with no fuel may not perform the above movement actions, nor may the tank pivot.</t>
   </si>
 </sst>
 </file>
@@ -4395,25 +4395,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="B292" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B293" sqref="B293"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="216.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="216.109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -4437,23 +4437,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>51</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
@@ -4485,7 +4485,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -4533,7 +4533,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>90</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>95</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>126</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>127</v>
       </c>
@@ -4589,7 +4589,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>128</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>129</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>130</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>131</v>
       </c>
@@ -4621,31 +4621,31 @@
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>135</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>224</v>
       </c>
@@ -4661,15 +4661,15 @@
         <v>225</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>229</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>230</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>231</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>232</v>
       </c>
@@ -4693,15 +4693,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>233</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>445</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>448</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>449</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>450</v>
       </c>
@@ -4733,103 +4733,103 @@
         <v>490</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>451</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>537</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="B45" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>538</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>539</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="165" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>540</v>
-      </c>
       <c r="B46" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>453</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>454</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>455</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>168</v>
       </c>
@@ -4837,7 +4837,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>169</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>170</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>171</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>172</v>
       </c>
@@ -4869,7 +4869,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>173</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>201</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>203</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>204</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>205</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>206</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>207</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>208</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>211</v>
       </c>
@@ -4941,23 +4941,23 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>212</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>213</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>214</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>216</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>193</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>195</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>196</v>
       </c>
@@ -4997,7 +4997,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>197</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>27</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>28</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>29</v>
       </c>
@@ -5029,7 +5029,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
         <v>268</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
         <v>269</v>
       </c>
@@ -5045,7 +5045,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
         <v>271</v>
       </c>
@@ -5053,15 +5053,15 @@
         <v>334</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>272</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>273</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>274</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>275</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A86" s="5" t="s">
         <v>276</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A87" s="5" t="s">
         <v>277</v>
       </c>
@@ -5101,7 +5101,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
         <v>278</v>
       </c>
@@ -5109,7 +5109,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
         <v>279</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>280</v>
       </c>
@@ -5125,7 +5125,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>281</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>282</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>283</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
         <v>284</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
         <v>285</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
         <v>286</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A97" s="5" t="s">
         <v>287</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>288</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>289</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="s">
         <v>290</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>291</v>
       </c>
@@ -5213,7 +5213,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
         <v>292</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
         <v>293</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="s">
         <v>294</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="s">
         <v>295</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="s">
         <v>296</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="s">
         <v>297</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="s">
         <v>299</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="s">
         <v>300</v>
       </c>
@@ -5277,7 +5277,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A110" s="5" t="s">
         <v>301</v>
       </c>
@@ -5285,7 +5285,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A111" s="5" t="s">
         <v>302</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
         <v>303</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
         <v>335</v>
       </c>
@@ -5309,7 +5309,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="s">
         <v>336</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
         <v>337</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
         <v>338</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A117" s="5" t="s">
         <v>339</v>
       </c>
@@ -5341,7 +5341,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
         <v>340</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
         <v>341</v>
       </c>
@@ -5357,7 +5357,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
         <v>342</v>
       </c>
@@ -5365,23 +5365,23 @@
         <v>364</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A121" s="5" t="s">
         <v>351</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A122" s="5" t="s">
         <v>343</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
         <v>344</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" s="5" t="s">
         <v>345</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>346</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
         <v>347</v>
       </c>
@@ -5413,7 +5413,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
         <v>348</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A128" s="5" t="s">
         <v>349</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
         <v>350</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
         <v>359</v>
       </c>
@@ -5445,7 +5445,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
         <v>360</v>
       </c>
@@ -5453,7 +5453,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
         <v>373</v>
       </c>
@@ -5461,15 +5461,15 @@
         <v>375</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A133" s="5" t="s">
         <v>376</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
         <v>377</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>378</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="s">
         <v>379</v>
       </c>
@@ -5493,7 +5493,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A137" s="5" t="s">
         <v>380</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
         <v>381</v>
       </c>
@@ -5509,7 +5509,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A139" s="5" t="s">
         <v>374</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A140" s="5" t="s">
         <v>386</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A141" s="5" t="s">
         <v>389</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A142" s="5" t="s">
         <v>390</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="5" t="s">
         <v>387</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A144" s="5" t="s">
         <v>388</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A145" s="5" t="s">
         <v>397</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A146" s="5" t="s">
         <v>398</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A147" s="5" t="s">
         <v>399</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
         <v>400</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
         <v>235</v>
       </c>
@@ -5597,15 +5597,15 @@
         <v>251</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
         <v>236</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A151" s="5" t="s">
         <v>237</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
         <v>238</v>
       </c>
@@ -5621,15 +5621,15 @@
         <v>261</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
         <v>239</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
         <v>240</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
         <v>241</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
         <v>242</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
         <v>243</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
         <v>244</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
         <v>245</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
         <v>246</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
         <v>247</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
         <v>248</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
         <v>249</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
         <v>250</v>
       </c>
@@ -5717,23 +5717,23 @@
         <v>265</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
         <v>372</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
         <v>417</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
         <v>418</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
         <v>419</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
         <v>420</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
         <v>421</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
         <v>425</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
         <v>423</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
         <v>422</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
         <v>424</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
         <v>266</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
         <v>407</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A177" s="5" t="s">
         <v>408</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A178" s="5" t="s">
         <v>409</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A179" s="5" t="s">
         <v>410</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A180" s="5" t="s">
         <v>411</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A181" s="5" t="s">
         <v>412</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A182" s="5" t="s">
         <v>413</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A183" s="5" t="s">
         <v>414</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A184" s="5" t="s">
         <v>415</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A185" s="5" t="s">
         <v>416</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A186" s="5" t="s">
         <v>443</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>72</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>73</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>74</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>75</v>
       </c>
@@ -5925,15 +5925,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>78</v>
       </c>
@@ -5941,23 +5941,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>96</v>
       </c>
@@ -5965,7 +5965,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>97</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>98</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>99</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>100</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>101</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>102</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>103</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>104</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>105</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>106</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>107</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>108</v>
       </c>
@@ -6061,15 +6061,15 @@
         <v>116</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>118</v>
       </c>
@@ -6077,23 +6077,23 @@
         <v>488</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
         <v>456</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A213" s="5" t="s">
         <v>457</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A214" s="5" t="s">
         <v>459</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A215" s="5" t="s">
         <v>460</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A216" s="5" t="s">
         <v>461</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A217" s="5" t="s">
         <v>462</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A218" s="5" t="s">
         <v>463</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A219" s="5" t="s">
         <v>464</v>
       </c>
@@ -6157,31 +6157,31 @@
         <v>471</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A220" s="5" t="s">
         <v>472</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A221" s="5" t="s">
         <v>473</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A222" s="5" t="s">
         <v>474</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A223" s="5" t="s">
         <v>475</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
         <v>479</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A225" s="5" t="s">
         <v>480</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A226" s="5" t="s">
         <v>481</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>30</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>31</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>32</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>33</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>34</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>35</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>36</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>39</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>40</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>38</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>42</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>43</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>44</v>
       </c>
@@ -6317,15 +6317,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>0</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>1</v>
       </c>
@@ -6341,7 +6341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>11</v>
       </c>
@@ -6349,7 +6349,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>12</v>
       </c>
@@ -6357,7 +6357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>2</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>3</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>4</v>
       </c>
@@ -6381,39 +6381,39 @@
         <v>63</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>9</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>68</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>69</v>
       </c>
@@ -6437,7 +6437,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>70</v>
       </c>
@@ -6445,7 +6445,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>71</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>149</v>
       </c>
@@ -6461,7 +6461,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>150</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>152</v>
       </c>
@@ -6477,7 +6477,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>153</v>
       </c>
@@ -6485,7 +6485,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>154</v>
       </c>
@@ -6493,7 +6493,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>151</v>
       </c>
@@ -6501,7 +6501,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>157</v>
       </c>
@@ -6509,23 +6509,23 @@
         <v>165</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>162</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>159</v>
       </c>
@@ -6533,7 +6533,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>498</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>499</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>500</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>176</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="271" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>177</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>178</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>179</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>183</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>184</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>185</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>491</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>492</v>
       </c>
@@ -6629,111 +6629,111 @@
         <v>494</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>493</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>495</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>496</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A283" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A284" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="B282" s="3" t="s">
+      <c r="B284" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A285" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A286" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A287" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A288" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A289" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B289" s="3" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
-      <c r="A283" s="1" t="s">
-        <v>560</v>
-      </c>
-      <c r="B283" s="3" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A284" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="B284" s="3" t="s">
+    <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A290" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B290" s="3" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A285" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="B285" s="3" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A286" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="B286" s="3" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A287" s="1" t="s">
-        <v>564</v>
-      </c>
-      <c r="B287" s="3" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A288" s="1" t="s">
-        <v>565</v>
-      </c>
-      <c r="B288" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A289" s="1" t="s">
+    <row r="291" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A291" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="B289" s="3" t="s">
+      <c r="B291" s="3" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A290" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="B290" s="3" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A291" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>505</v>
       </c>
@@ -6741,66 +6741,66 @@
         <v>508</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>506</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>507</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A296" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="B295" s="3" t="s">
+      <c r="B296" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A297" s="1" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A296" s="1" t="s">
+      <c r="B297" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A298" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="B296" s="3" t="s">
+      <c r="B298" s="3" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A297" s="1" t="s">
+    <row r="299" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A299" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="B297" s="3" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A298" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="B298" s="3" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A299" s="1" t="s">
-        <v>555</v>
-      </c>
       <c r="B299" s="3" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B303" s="4"/>
     </row>
-    <row r="382" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="154.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A310:B485">
     <sortCondition ref="A310:A485"/>

</xml_diff>

<commit_message>
finish testing bail out mechanics
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5A643CD-E3DE-4DA0-9EFB-E95F1BD5FF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{35F54294-1DB9-4C86-9905-286995807F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3556,19 +3556,6 @@
 c.) Remove knocked out enemy units from the board and record the victory points for their destruction on the After Action Report.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;r4.74.4  Crew Actions Phase - Miscellaenous Actions&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-a.) Replace periscopes: Mark off a periscope replacement on the After Action Report 
-&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for each replacement. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-b.) Attempt to repair guns that have malfunctioned by consulting the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-c.) Fire 2" smoke mortar. Place Smoke marker in target zone and mark off one smoke bomb from the After Action Report per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
-d.) Throw smoke grenade. Place smoke marker on your tank and mark off one smoke grenade from the After Action Report per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r4.74.2  Crew Actions Phase - Tank Main Gun Fire&lt;/Bold&gt;  
 &lt;InlineUIContainer&gt;&lt;Button Content='r9.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
@@ -4019,6 +4006,22 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c106ThrownTrack'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r4.74.4  Crew Actions Phase - Miscellaenous Actions&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+a.) Replace periscopes: Mark off a periscope replacement on the After Action Report 
+&lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; for each replacement. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+b.) Attempt to repair guns that have malfunctioned by consulting the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Gun Malfunction' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+c.) Fire 2" smoke mortar. Place Smoke marker in target zone and mark off one smoke bomb from the After Action Report per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. &lt;LineBreak/&gt;&lt;LineBreak/&gt;
+d.) Throw smoke grenade. Place smoke marker on your tank and mark off one smoke grenade from the After Action Report per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r18.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Note: If tank is disabled due to thrown track or stuck in bog, Commander may elect to bail out of tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
   </si>
 </sst>
 </file>
@@ -4393,8 +4396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4408,7 +4411,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -4440,7 +4443,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -4448,7 +4451,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -4752,7 +4755,7 @@
         <v>535</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -4763,12 +4766,12 @@
         <v>544</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5" t="s">
         <v>537</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>545</v>
+        <v>597</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="288" x14ac:dyDescent="0.55000000000000004">
@@ -4944,7 +4947,7 @@
         <v>212</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -5056,7 +5059,7 @@
         <v>272</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -5368,7 +5371,7 @@
         <v>351</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -5464,7 +5467,7 @@
         <v>376</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -5528,7 +5531,7 @@
         <v>389</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -5600,7 +5603,7 @@
         <v>236</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
@@ -5624,7 +5627,7 @@
         <v>239</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -5720,7 +5723,7 @@
         <v>372</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
@@ -5728,7 +5731,7 @@
         <v>416</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -5928,7 +5931,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -6384,7 +6387,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -6392,7 +6395,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
@@ -6408,7 +6411,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -6632,7 +6635,7 @@
         <v>492</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -6640,7 +6643,7 @@
         <v>494</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -6648,87 +6651,87 @@
         <v>495</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
@@ -6744,7 +6747,7 @@
         <v>505</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -6752,47 +6755,47 @@
         <v>506</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>547</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
made sure Rules.txt created
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35F54294-1DB9-4C86-9905-286995807F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0458C8A9-74BC-48D9-8051-B7BC7578B544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -1152,17 +1152,6 @@
     <t>r6.0</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r6.0 How to Win&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In order to win an engagement or scenario, both you and your tank must survive. If you are killed or wounded sufficently to miss combat for any time, or if you tank is knocked out, you lose. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If both you and your tank survive, winning depends on your score of victory points. Vicotry in the campaign game is a special case.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Victory Points&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Victory&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r6.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Campaign Game Victory</t>
-  </si>
-  <si>
     <t>r6.1</t>
   </si>
   <si>
@@ -1638,16 +1627,6 @@
     <t>r8.1</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r8.0 Crew Actions&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Commander (C)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Gunner (G)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Loader (L)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Driver (D)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Assistant Driver (A)&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Non-Specific Crew Actions</t>
-  </si>
-  <si>
     <t xml:space="preserve">r8.11 </t>
   </si>
   <si>
@@ -1753,14 +1732,6 @@
     <t>r8.65</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r8.1 Commander (C)&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct Movement&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct Fire
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c07Commander'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r8.2 Gunner (G)&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r8.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Main Gun&lt;LineBreak/&gt;
@@ -1777,18 +1748,6 @@
 Subtract gunner&amp;apos;s rating from the To Hit roll for the main gun. Gunner may not spot. 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c50GFIreMainGun'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r8.3 Loader (L)&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Load&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Main Gun&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Co-Axial MG&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.34' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Mortar&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.35' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Change Gun Load&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r8.36' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Restock Ready Rack
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c09Loader'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
     <t>&lt;Bold&gt;r8.31 Load&lt;/Bold&gt; 
@@ -4022,6 +3981,56 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Note: If tank is disabled due to thrown track or stuck in bog, Commander may elect to bail out of tank per 
 &lt;InlineUIContainer&gt;&lt;Button Content='r11.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r8.0 Crew Actions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Commander (C)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Gunner (G)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Loader (L)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.4' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Driver (D)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.5' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Assistant Driver (A)&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.6' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Non-Specific Crew Actions
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Note: If tank is disabled due to thrown track or stuck in bog, Commander may elect to bail out of tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r8.1 Commander (C)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct Movement&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.12' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Direct Fire
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c07Commander'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Note: If tank is disabled due to thrown track or stuck in bog, Commander may elect to bail out of tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r11.11' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r8.3 Loader (L)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Load&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.32' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Main Gun&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.33' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Repair Co-Axial MG&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.34' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Fire Mortar&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.35' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Change Gun Load&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.36' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Restock Ready Rack
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c09Loader'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Note: The Load action allows loader to perform spotting unless the main gun is fired per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r8.31' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r6.0 How to Win&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In order to win an engagement or scenario, both you and your tank must survive. If you are killed or wounded sufficently to miss combat for any time, or if you tank is knocked out, you lose. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If both you and your tank survive, winning depends on your score of victory points. Victory in the campaign game is a special case.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Victory Points&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Victory&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r6.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Campaign Game Victory</t>
   </si>
 </sst>
 </file>
@@ -4396,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="B71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4411,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -4443,7 +4452,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -4451,7 +4460,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -4483,7 +4492,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -4523,7 +4532,7 @@
         <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -4627,7 +4636,7 @@
         <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -4635,7 +4644,7 @@
         <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -4643,7 +4652,7 @@
         <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
@@ -4656,178 +4665,178 @@
     </row>
     <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="5" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="5" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="259.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="5" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="5" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="5" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="288" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="5" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="5" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="5" t="s">
+        <v>524</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>528</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -4843,7 +4852,7 @@
         <v>169</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -4880,98 +4889,98 @@
     </row>
     <row r="60" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -4979,31 +4988,31 @@
         <v>193</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>194</v>
+        <v>597</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -5030,868 +5039,868 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="5" t="s">
-        <v>269</v>
-      </c>
       <c r="B80" s="2" t="s">
-        <v>304</v>
+        <v>595</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>307</v>
+        <v>596</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="5" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="5" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="5" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="5" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B135" s="2" t="s">
         <v>378</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="5" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="5" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="5" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="5" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="5" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="5" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="5" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B145" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="5" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="5" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="5" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="316.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="5" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="5" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="5" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B171" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="5" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="5" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="5" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="5" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="5" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -5899,7 +5908,7 @@
         <v>72</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="188" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -5931,7 +5940,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -5947,15 +5956,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" s="5" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
@@ -5987,7 +5996,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -6067,7 +6076,7 @@
         <v>117</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -6075,7 +6084,7 @@
         <v>118</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
@@ -6083,7 +6092,7 @@
         <v>119</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -6091,127 +6100,127 @@
         <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
       <c r="A212" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A213" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A214" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A215" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A216" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A217" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A218" s="5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A219" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A220" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A221" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A222" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A223" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A224" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>479</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -6227,7 +6236,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -6323,7 +6332,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -6347,7 +6356,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
@@ -6387,7 +6396,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
@@ -6395,7 +6404,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
@@ -6403,7 +6412,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -6411,7 +6420,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -6483,7 +6492,7 @@
         <v>153</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="261" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
@@ -6499,7 +6508,7 @@
         <v>151</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -6515,7 +6524,7 @@
         <v>158</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -6523,7 +6532,7 @@
         <v>162</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -6531,31 +6540,31 @@
         <v>159</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A267" s="1" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A268" s="1" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A269" s="1" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -6616,186 +6625,186 @@
     </row>
     <row r="277" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A277" s="1" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A278" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A279" s="1" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A280" s="1" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A281" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A282" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="A283" s="1" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A284" s="1" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A285" s="1" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A286" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A287" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A288" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A289" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A290" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A291" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A292" s="1" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A293" s="1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A294" s="1" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A295" s="1" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A296" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B296" s="3" t="s">
         <v>548</v>
-      </c>
-      <c r="B296" s="3" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A297" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B297" s="3" t="s">
         <v>549</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A298" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B298" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="B298" s="3" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A299" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Lots of fixes. Fix missed gun shot on end of ROF stream. Fix GameStats. FIx win/lose display at end of game.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA9249D5-9F81-42B9-8D13-22BED1F5363C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3553269A-ECCA-48CF-864C-D5B2DDCE7DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -906,15 +906,6 @@
     <t>r23.2</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r4.51 Mark Start Area&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Around the edge of the Movement Board, there are 10 areas number 1-10. Roll 1D to determine which of the ten is the start area for this scenario. Also, mark the area with a Start Area marker.
-Place the Task Force marker representing your friendly forces on that area.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                    &lt;InlineUIContainer&gt;&lt;Image Name='c33StartArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;           
-      &lt;InlineUIContainer&gt;&lt;Image Name='c35TaskForce'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;r4.52 Mark Exit Area&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 On the &lt;InlineUIContainer&gt;&lt;Button Content='Exit Areas' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
@@ -4031,6 +4022,15 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r29.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Movement Board Fuel Use&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r29.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Battle Board Fuel Use</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r4.51 Mark Start Area&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Around the edge of the Movement Board, there are 10 areas number 1-10. Roll 1D to determine which of the ten is the start area for this scenario. Also, mark the area with a Start Area marker. 
+Place the Task Force marker representing your friendly forces on that area.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                    &lt;InlineUIContainer&gt;&lt;Image Name='c33StartArea'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;           
+      &lt;InlineUIContainer&gt;&lt;Image Name='c35TaskForce'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4405,25 +4405,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B292" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B294" sqref="B294"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.68359375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="216.1015625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="216.109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -4447,23 +4447,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>51</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -4487,15 +4487,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -4527,15 +4527,15 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>90</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>95</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>126</v>
       </c>
@@ -4591,31 +4591,31 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>128</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>129</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>130</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>131</v>
       </c>
@@ -4631,391 +4631,391 @@
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>132</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>134</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.55000000000000004">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>135</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B37" s="2" t="s">
+    <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="288" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="5" t="s">
-        <v>440</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="259.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="5" t="s">
-        <v>532</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="288" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>447</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="5" t="s">
+      <c r="B48" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="5" t="s">
-        <v>450</v>
-      </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="5" t="s">
+    <row r="53" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>522</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="374.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B58" s="2" t="s">
+    <row r="60" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="5" t="s">
+      <c r="B72" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="5" t="s">
+      <c r="B73" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>27</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>28</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
         <v>29</v>
       </c>
@@ -5039,879 +5039,879 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B80" s="2" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B81" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A84" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A86" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A81" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B81" s="2" t="s">
+    <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A90" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A94" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A96" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A98" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A100" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A101" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A102" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A103" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A104" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A105" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A106" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A107" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A109" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A110" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A112" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A113" s="5" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="5" t="s">
+      <c r="B113" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="5" t="s">
+    <row r="115" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A116" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A117" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="B116" s="2" t="s">
+    <row r="119" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="B118" s="2" t="s">
+    <row r="120" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A120" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B119" s="2" t="s">
+    <row r="121" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A121" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A122" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A123" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="B120" s="2" t="s">
+    <row r="124" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A124" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A127" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="B125" s="2" t="s">
+    <row r="128" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A128" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A130" s="5" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A126" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="B129" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="5" t="s">
+    <row r="131" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A131" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="5" t="s">
-        <v>356</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A132" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A133" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A134" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A135" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A137" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A138" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A139" s="5" t="s">
         <v>369</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B133" s="2" t="s">
+      <c r="B139" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A141" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A142" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A145" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A146" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A147" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A148" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A149" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="A150" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A151" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+      <c r="A152" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A153" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B153" s="2" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A135" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A138" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A139" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A141" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A142" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A143" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B144" s="2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="B148" s="2" t="s">
+    <row r="154" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A154" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A155" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A156" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A157" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A158" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A159" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A160" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A162" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A164" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A166" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A167" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A168" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A169" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A170" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A171" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A172" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A173" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A174" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A175" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A176" s="5" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A149" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="316.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A150" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A151" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="216" x14ac:dyDescent="0.55000000000000004">
-      <c r="A152" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A153" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A154" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A155" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A156" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A157" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A158" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A159" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A160" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A161" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A162" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A163" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A164" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A165" s="5" t="s">
-        <v>368</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A167" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A169" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A170" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A171" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A172" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A173" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="B173" s="2" t="s">
+      <c r="B176" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A177" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A178" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A179" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A174" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A175" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A176" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="B176" s="2" t="s">
+    <row r="180" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A180" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A181" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A182" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A183" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A184" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A185" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A186" s="5" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A177" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A178" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A179" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A180" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A182" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A183" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A184" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A185" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A186" s="5" t="s">
+      <c r="B186" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="187" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A187" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A188" s="5" t="s">
         <v>73</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A189" s="5" t="s">
         <v>74</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>75</v>
       </c>
@@ -5935,15 +5935,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A191" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A192" s="5" t="s">
         <v>78</v>
       </c>
@@ -5951,23 +5951,23 @@
         <v>83</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A193" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A194" s="5" t="s">
+        <v>535</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="195" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A195" s="5" t="s">
         <v>96</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A196" s="5" t="s">
         <v>97</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A197" s="5" t="s">
         <v>98</v>
       </c>
@@ -5991,15 +5991,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A198" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A199" s="5" t="s">
         <v>100</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A200" s="5" t="s">
         <v>101</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A201" s="5" t="s">
         <v>102</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A202" s="5" t="s">
         <v>103</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A203" s="5" t="s">
         <v>104</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A204" s="5" t="s">
         <v>105</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A205" s="5" t="s">
         <v>106</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A206" s="5" t="s">
         <v>107</v>
       </c>
@@ -6063,7 +6063,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A207" s="5" t="s">
         <v>108</v>
       </c>
@@ -6071,159 +6071,159 @@
         <v>116</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A208" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A209" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A210" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A211" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.55000000000000004">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A212" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A213" s="5" t="s">
         <v>451</v>
       </c>
-      <c r="B212" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A213" s="5" t="s">
+      <c r="B213" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B213" s="2" t="s">
+    </row>
+    <row r="214" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A214" s="5" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A214" s="5" t="s">
+      <c r="B214" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A215" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="B214" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A215" s="5" t="s">
+      <c r="B215" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A216" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B216" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A216" s="5" t="s">
+    <row r="217" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A217" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B217" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A217" s="5" t="s">
+    <row r="218" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A218" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="B218" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A218" s="5" t="s">
+    <row r="219" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A219" s="5" t="s">
         <v>458</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B219" s="2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A219" s="5" t="s">
-        <v>459</v>
-      </c>
-      <c r="B219" s="2" t="s">
+    <row r="220" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A220" s="5" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A220" s="5" t="s">
+      <c r="B220" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A221" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B220" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A221" s="5" t="s">
+      <c r="B221" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A222" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A222" s="5" t="s">
+      <c r="B222" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A223" s="5" t="s">
         <v>469</v>
       </c>
-      <c r="B222" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A223" s="5" t="s">
+      <c r="B223" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B223" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="224" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A224" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A225" s="5" t="s">
         <v>474</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="B225" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A226" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A225" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A226" s="5" t="s">
-        <v>476</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="5" t="s">
         <v>30</v>
       </c>
@@ -6231,15 +6231,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A228" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A229" s="5" t="s">
         <v>32</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="78.45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:2" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="5" t="s">
         <v>33</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A231" s="5" t="s">
         <v>34</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="5" t="s">
         <v>35</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A233" s="5" t="s">
         <v>36</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>39</v>
       </c>
@@ -6287,7 +6287,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A235" s="5" t="s">
         <v>40</v>
       </c>
@@ -6295,7 +6295,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="5" t="s">
         <v>38</v>
       </c>
@@ -6303,7 +6303,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A237" s="5" t="s">
         <v>42</v>
       </c>
@@ -6311,7 +6311,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A238" s="5" t="s">
         <v>43</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="5" t="s">
         <v>44</v>
       </c>
@@ -6327,15 +6327,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A240" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A241" s="5" t="s">
         <v>0</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="5" t="s">
         <v>1</v>
       </c>
@@ -6351,15 +6351,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A244" s="5" t="s">
         <v>12</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="5" t="s">
         <v>2</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="75.45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:2" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="5" t="s">
         <v>3</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A247" s="5" t="s">
         <v>4</v>
       </c>
@@ -6391,39 +6391,39 @@
         <v>63</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A249" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A250" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="5" t="s">
         <v>9</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>68</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>69</v>
       </c>
@@ -6447,7 +6447,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>70</v>
       </c>
@@ -6455,7 +6455,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>71</v>
       </c>
@@ -6463,23 +6463,23 @@
         <v>148</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>149</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>150</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>152</v>
       </c>
@@ -6487,15 +6487,15 @@
         <v>155</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>154</v>
       </c>
@@ -6503,314 +6503,314 @@
         <v>156</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="288" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:2" ht="288" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>151</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>157</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="230.4" x14ac:dyDescent="0.55000000000000004">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>158</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B266" s="3" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A267" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A268" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A269" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A267" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A268" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="B268" s="3" t="s">
+    <row r="270" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A270" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A271" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A272" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A273" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A274" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A275" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A276" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A277" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A278" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A279" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A280" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B280" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A281" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A282" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A283" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A284" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A285" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A286" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A287" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A288" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A289" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A290" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="B290" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A291" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B291" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A292" s="1" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A269" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A270" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A271" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="187.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A272" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A273" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A274" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A275" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A276" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" ht="158.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A277" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A278" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A279" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B279" s="3" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A280" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" ht="100.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A281" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" ht="244.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A282" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="B282" s="3" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" ht="144" x14ac:dyDescent="0.55000000000000004">
-      <c r="A283" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="B283" s="3" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A284" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="B284" s="3" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A285" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="B285" s="3" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A286" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="B286" s="3" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A287" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="B287" s="3" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A288" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B288" s="3" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A289" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="B289" s="3" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A290" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="B290" s="3" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A291" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="B291" s="3" t="s">
+      <c r="B292" s="3" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A293" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A294" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B294" s="3" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A295" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A296" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A297" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A298" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B298" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A299" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A292" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="115.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A293" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="B293" s="3" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A294" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="B294" s="3" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" ht="201.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A295" s="1" t="s">
-        <v>541</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A296" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="B296" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A297" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" ht="129.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A298" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B298" s="3" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A299" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="B299" s="3" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B303" s="4"/>
     </row>
-    <row r="382" ht="154.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="382" ht="154.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A310:B485">
     <sortCondition ref="A310:A485"/>

</xml_diff>

<commit_message>
Remove acq if a spotted unit moves and loses it spot state.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{858F6ECF-0AEA-443F-B140-D52A876FED68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CBCAD56-9BC8-4FB2-8A33-581BFCE8B31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -626,11 +626,6 @@
 Crewmen with closed hatches (other than the gunner) that have broken periscopes may not spot. The gunner may spot if either his sight or periscope is unbroken.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r17.24 Weather Restrictions&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During falling snow and fog weather, spotting is only possible at close range.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r17.25 Smoke Restrictions&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Spotting rolls are +1 for each Smoke marker on your tank, in the zone with the unit you are attempting to spot, or in any zones between.</t>
@@ -3277,16 +3272,6 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Hidden units are addressed by 
 &lt;InlineUIContainer&gt;&lt;Button Content='r17.3' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;Bold&gt;r17.3 Hidden Units&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Hidden enemy units cannot be spotted, cannot be fired on, and cannot fire at you. This changes when your tank moves or the hidden unit moves during the Eney Action Phase 
-&lt;InlineUIContainer&gt;&lt;Button Content='r17.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If either event occurs, remove the Hidden marker. You may attempt to spot this unit during the next Spotting Phase.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                     &lt;InlineUIContainer&gt;&lt;Image Name='c31Hidden'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
   <si>
     <t>&lt;Bold&gt;r23.1 Artillery Support Resolution&lt;/Bold&gt;
@@ -3930,20 +3915,6 @@
 A tank with no fuel may not perform the above movement actions, nor may the tank pivot.</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r11.11 Throwing a Track&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A tank with a thrown track may not move or pivot for the remainder of the battle. Your tank sits where it is until it is knocked out or until all enemy units withdraw or are eliminated.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the Battle Board is cleared of enemy units, the day of combat is finished for your tank. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-The crew of a disabled tank may abandon the vehicle, but each man must roll once on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-Table while making his escape. Afterwards, go to Evening Debriefing 
-&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-                                      &lt;InlineUIContainer&gt;&lt;Image Name='c106ThrownTrack'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;Bold&gt;r4.74.4  Crew Actions Phase - Miscellaenous Actions&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 a.) Replace periscopes: Mark off a periscope replacement on the After Action Report 
@@ -4031,6 +4002,35 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r29.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Movement Board Fuel Use&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r29.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Battle Board Fuel Use</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r11.11 Throwing a Track&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A tank with a thrown track may not move or pivot for the remainder of the battle. Your tank sits where it is until it is knocked out or until all enemy units withdraw or are eliminated. Enemy units that are supposed to move are indicated with 'Do Nothing (TT)'.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the Battle Board is cleared of enemy units, the day of combat is finished for your tank. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+The crew of a disabled tank may abandon the vehicle, but each man must roll once on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Wounds' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+Table while making his escape. Afterwards, go to Evening Debriefing 
+&lt;InlineUIContainer&gt;&lt;Button Content='r4.9' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                      &lt;InlineUIContainer&gt;&lt;Image Name='c106ThrownTrack'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r17.24 Weather Restrictions&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During falling snow and fog weather, spotting is only possible at close range. Also, enemy  attacks can only at close range. An enemy that is supposed to attack is indicated by 'Do Nothing (W)'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r17.3 Hidden Units&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Hidden enemy units cannot be spotted, cannot be fired on, and cannot fire at you. An enemy that is supposed to attack is indicated by 'Do Nothing (H)'. This changes when your tank moves or the hidden unit moves during the Enemy Action Phase 
+&lt;InlineUIContainer&gt;&lt;Button Content='r17.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If either event occurs, remove the Hidden marker. You may attempt to spot this unit during the next Spotting Phase.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+                                     &lt;InlineUIContainer&gt;&lt;Image Name='c31Hidden'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
   </si>
 </sst>
 </file>
@@ -4405,25 +4405,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B291" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B292" sqref="B292"/>
+    <sheetView tabSelected="1" topLeftCell="B203" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="216.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="216.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="146.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -4447,23 +4447,23 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>51</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
@@ -4487,15 +4487,15 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -4511,15 +4511,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -4527,23 +4527,23 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>87</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>88</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>89</v>
       </c>
@@ -4567,15 +4567,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>90</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>95</v>
       </c>
@@ -4583,447 +4583,447 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+      <c r="B23" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="B24" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="B25" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>521</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="345.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>439</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
-        <v>531</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="288" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
-        <v>521</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="B54" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B55" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B58" s="2" t="s">
+    <row r="60" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+      <c r="B72" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
+      <c r="B73" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B74" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" ht="136.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="92.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>28</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>29</v>
       </c>
@@ -5039,879 +5039,879 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="5" t="s">
+      <c r="B80" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A81" s="5" t="s">
+      <c r="B81" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B82" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A111" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A112" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A113" s="5" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A85" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A86" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A87" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A89" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A91" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A92" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A94" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A95" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A96" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A97" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A102" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A103" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A104" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A106" s="5" t="s">
-        <v>293</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A111" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A112" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A113" s="5" t="s">
+      <c r="B113" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A114" s="5" t="s">
         <v>330</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="5" t="s">
+    <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B115" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A116" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A117" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A118" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="B116" s="2" t="s">
+    <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>334</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="B118" s="2" t="s">
+    <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="B119" s="2" t="s">
+    <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A121" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A122" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A123" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B123" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A120" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="B120" s="2" t="s">
+    <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A127" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B127" s="2" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A121" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A122" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A123" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A124" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A125" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="B125" s="2" t="s">
+    <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A128" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A129" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A130" s="5" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A126" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A127" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A128" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="B129" s="2" t="s">
+      <c r="B130" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A130" s="5" t="s">
+    <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
+      <c r="A131" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B131" s="2" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A131" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A133" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A135" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A136" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A137" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A138" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A139" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A133" s="5" t="s">
-        <v>371</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A134" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A135" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="B136" s="2" t="s">
+      <c r="B139" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A140" s="5" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A137" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A138" s="5" t="s">
-        <v>376</v>
-      </c>
-      <c r="B138" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A139" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="B139" s="2" t="s">
+    <row r="141" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A142" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="B142" s="2" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="5" t="s">
+    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A141" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A142" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="5" t="s">
+      <c r="B143" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A144" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B144" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A145" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A146" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="B146" s="2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="B144" s="2" t="s">
+    <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A147" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A148" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B148" s="2" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A145" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A146" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A147" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A148" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="B148" s="2" t="s">
+    <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A149" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="330" x14ac:dyDescent="0.25">
+      <c r="A150" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A151" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
+      <c r="A152" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A153" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A154" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A155" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A157" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A158" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A159" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A161" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A162" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A163" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A164" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A165" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A166" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A167" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A168" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A169" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A170" s="5" t="s">
+        <v>414</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A171" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A172" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A173" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A174" s="5" t="s">
+        <v>417</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A175" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A176" s="5" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A149" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="316.8" x14ac:dyDescent="0.3">
-      <c r="A150" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B150" s="2" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A151" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="216" x14ac:dyDescent="0.3">
-      <c r="A152" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A153" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B153" s="2" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A154" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A155" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A156" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B156" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A157" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A158" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A159" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A160" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A161" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B161" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A162" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A163" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A164" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A165" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A166" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A167" s="5" t="s">
-        <v>412</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A168" s="5" t="s">
-        <v>413</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A169" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A170" s="5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A171" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A172" s="5" t="s">
-        <v>417</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A173" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B173" s="2" t="s">
+      <c r="B176" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A178" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A179" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B179" s="2" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A174" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A175" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A176" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="B176" s="2" t="s">
+    <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A180" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A181" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A182" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A183" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A184" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A185" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A186" s="5" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A177" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A178" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A179" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="B179" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A180" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A181" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A182" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A183" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A184" s="5" t="s">
-        <v>409</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A185" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A186" s="5" t="s">
+      <c r="B186" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    </row>
+    <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>72</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>73</v>
       </c>
@@ -5919,7 +5919,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>74</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>75</v>
       </c>
@@ -5935,15 +5935,15 @@
         <v>81</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>78</v>
       </c>
@@ -5951,39 +5951,39 @@
         <v>83</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>97</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>98</v>
       </c>
@@ -5991,15 +5991,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>100</v>
       </c>
@@ -6007,15 +6007,15 @@
         <v>109</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>102</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>103</v>
       </c>
@@ -6031,15 +6031,15 @@
         <v>112</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>104</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>105</v>
       </c>
@@ -6047,7 +6047,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>106</v>
       </c>
@@ -6055,175 +6055,175 @@
         <v>114</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>107</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>108</v>
       </c>
       <c r="B207" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A208" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="208" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A208" s="5" t="s">
+      <c r="B208" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A209" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A209" s="5" t="s">
+      <c r="B209" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
+      <c r="A210" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A210" s="5" t="s">
+      <c r="B210" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A211" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B210" s="2" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A211" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="B211" s="2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A213" s="5" t="s">
         <v>450</v>
       </c>
-      <c r="B212" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A213" s="5" t="s">
+      <c r="B213" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B213" s="2" t="s">
+    </row>
+    <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A214" s="5" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A214" s="5" t="s">
+      <c r="B214" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A215" s="5" t="s">
         <v>453</v>
       </c>
-      <c r="B214" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A215" s="5" t="s">
+      <c r="B215" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A216" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B216" s="2" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A216" s="5" t="s">
+    <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A217" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B217" s="2" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A217" s="5" t="s">
+    <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A218" s="5" t="s">
         <v>456</v>
       </c>
-      <c r="B217" s="2" t="s">
+      <c r="B218" s="2" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A218" s="5" t="s">
+    <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A219" s="5" t="s">
         <v>457</v>
       </c>
-      <c r="B218" s="2" t="s">
+      <c r="B219" s="2" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A219" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="B219" s="2" t="s">
+    <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="220" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A220" s="5" t="s">
+      <c r="B220" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A221" s="5" t="s">
         <v>466</v>
       </c>
-      <c r="B220" s="2" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A221" s="5" t="s">
+      <c r="B221" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A222" s="5" t="s">
         <v>467</v>
       </c>
-      <c r="B221" s="2" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A222" s="5" t="s">
+      <c r="B222" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A223" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="B222" s="2" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A223" s="5" t="s">
+      <c r="B223" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B223" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A225" s="5" t="s">
         <v>473</v>
       </c>
-      <c r="B224" s="2" t="s">
+      <c r="B225" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A226" s="5" t="s">
+        <v>474</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A225" s="5" t="s">
-        <v>474</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A226" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="5" t="s">
         <v>30</v>
       </c>
@@ -6231,15 +6231,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A228" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A229" s="5" t="s">
         <v>32</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="78.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" ht="78.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="5" t="s">
         <v>33</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A231" s="5" t="s">
         <v>34</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" ht="119.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5" t="s">
         <v>35</v>
       </c>
@@ -6271,7 +6271,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A233" s="5" t="s">
         <v>36</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A234" s="5" t="s">
         <v>39</v>
       </c>
@@ -6287,15 +6287,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A235" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="181.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="5" t="s">
         <v>38</v>
       </c>
@@ -6303,23 +6303,23 @@
         <v>61</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A237" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A238" s="5" t="s">
         <v>43</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="64.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
         <v>44</v>
       </c>
@@ -6327,15 +6327,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A240" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A241" s="5" t="s">
         <v>0</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
         <v>1</v>
       </c>
@@ -6351,15 +6351,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="91.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A244" s="5" t="s">
         <v>12</v>
       </c>
@@ -6367,7 +6367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="5" t="s">
         <v>2</v>
       </c>
@@ -6375,7 +6375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="75.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" ht="75.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="5" t="s">
         <v>3</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A247" s="5" t="s">
         <v>4</v>
       </c>
@@ -6391,39 +6391,39 @@
         <v>63</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="90.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" ht="90.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A249" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A250" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" ht="104.7" customHeight="1" x14ac:dyDescent="0.3">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="5" t="s">
         <v>9</v>
       </c>
@@ -6431,386 +6431,386 @@
         <v>24</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B256" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A257" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A257" s="1" t="s">
+      <c r="B257" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B257" s="3" t="s">
+      <c r="B258" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A258" s="1" t="s">
+    <row r="259" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="300" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B258" s="3" t="s">
+      <c r="B262" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B263" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A259" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B259" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A260" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B260" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A261" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" ht="288" x14ac:dyDescent="0.3">
-      <c r="A262" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B262" s="3" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A263" s="1" t="s">
+    <row r="264" spans="1:2" ht="240" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B263" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A264" s="1" t="s">
+      <c r="B264" s="3" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B264" s="3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A265" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A266" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="B266" s="3" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B269" s="3" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A267" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A268" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="B268" s="3" t="s">
+    <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B280" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B290" s="3" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B291" s="3" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A269" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A270" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A271" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A272" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A273" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A274" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A275" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A276" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A277" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A278" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A279" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="B279" s="3" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A280" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A281" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="B281" s="3" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
-      <c r="A282" s="1" t="s">
-        <v>549</v>
-      </c>
-      <c r="B282" s="3" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A283" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="B283" s="3" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A284" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="B284" s="3" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A285" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="B285" s="3" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A286" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="B286" s="3" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A287" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="B287" s="3" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A288" s="1" t="s">
-        <v>555</v>
-      </c>
-      <c r="B288" s="3" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A289" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B289" s="3" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A290" s="1" t="s">
-        <v>557</v>
-      </c>
-      <c r="B290" s="3" t="s">
+      <c r="B292" s="3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A293" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B294" s="3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="B298" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B299" s="3" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A291" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="B291" s="3" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A292" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="B292" s="3" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A293" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B293" s="3" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A294" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="B294" s="3" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A295" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A296" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="B296" s="3" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A297" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="B297" s="3" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A298" s="1" t="s">
-        <v>544</v>
-      </c>
-      <c r="B298" s="3" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A299" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="B299" s="3" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B303" s="4"/>
     </row>
-    <row r="382" ht="154.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="382" ht="154.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A310:B485">
     <sortCondition ref="A310:A485"/>

</xml_diff>

<commit_message>
support e045 change. Make getting feats a static variable. Fixed table names.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CBCAD56-9BC8-4FB2-8A33-581BFCE8B31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B289C9A0-9A1C-44EA-922A-7038E081E4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -2597,16 +2597,6 @@
                                       &lt;InlineUIContainer&gt;&lt;Image Name='c107Panzerfaust'  Height='50' Width='50'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r15.6 Harassing Fire&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-This event represents the random spraying of fire at your tank in the hopes of causing casualties to exposed crewmen. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-It was also possible for tis type of fire to cause collateral damage to your tank such as the damaging of periscopes, sights, adn the AA MG. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When this event is rolled, roll on the 
-&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table.</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r15.8 Enemy Reinforcement&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 When this event occurs, immediately activate one additional enemy unit for an Advance scenario and two additional for Battle/Counterattack scenarios.
@@ -4031,6 +4021,16 @@
 If either event occurs, remove the Hidden marker. You may attempt to spot this unit during the next Spotting Phase.
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
                                      &lt;InlineUIContainer&gt;&lt;Image Name='c31Hidden'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r15.6 Harassing Fire&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+This event represents the random spraying of fire at your tank in the hopes of causing casualties to exposed crewmen. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+It was also possible for this type of fire to cause collateral damage to your tank such as the damaging of periscopes, sights, and the AA MG. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When this event is rolled, roll on the 
+&lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table.</t>
   </si>
 </sst>
 </file>
@@ -4405,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B203" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4420,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4452,7 +4452,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4460,7 +4460,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4636,7 +4636,7 @@
         <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4644,7 +4644,7 @@
         <v>132</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4652,7 +4652,7 @@
         <v>133</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4676,7 +4676,7 @@
         <v>226</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4708,135 +4708,135 @@
         <v>230</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4964,7 +4964,7 @@
         <v>210</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4988,7 +4988,7 @@
         <v>191</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5044,7 +5044,7 @@
         <v>265</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5052,7 +5052,7 @@
         <v>266</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5068,7 +5068,7 @@
         <v>268</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5124,7 +5124,7 @@
         <v>275</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5276,7 +5276,7 @@
         <v>295</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5380,7 +5380,7 @@
         <v>345</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5388,7 +5388,7 @@
         <v>337</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5476,7 +5476,7 @@
         <v>370</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5540,7 +5540,7 @@
         <v>383</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>233</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5636,7 +5636,7 @@
         <v>236</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5732,7 +5732,7 @@
         <v>366</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5740,7 +5740,7 @@
         <v>410</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5788,7 +5788,7 @@
         <v>416</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5796,7 +5796,7 @@
         <v>415</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5820,7 +5820,7 @@
         <v>400</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5844,7 +5844,7 @@
         <v>403</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5868,7 +5868,7 @@
         <v>406</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>429</v>
+        <v>597</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5876,7 +5876,7 @@
         <v>407</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5884,7 +5884,7 @@
         <v>408</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5892,15 +5892,15 @@
         <v>409</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5940,7 +5940,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5956,15 +5956,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
+        <v>532</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -5996,7 +5996,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6060,7 +6060,7 @@
         <v>107</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6076,7 +6076,7 @@
         <v>116</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6084,7 +6084,7 @@
         <v>117</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>118</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6100,127 +6100,127 @@
         <v>119</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6236,7 +6236,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6332,7 +6332,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6356,7 +6356,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6396,7 +6396,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6404,7 +6404,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6412,7 +6412,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6420,7 +6420,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6524,7 +6524,7 @@
         <v>157</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6532,7 +6532,7 @@
         <v>160</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6540,31 +6540,31 @@
         <v>158</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6625,186 +6625,186 @@
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>538</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moved crewmembers to GameInstance. Renamed and fixed tank images for VIe and VIb.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B289C9A0-9A1C-44EA-922A-7038E081E4F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFAE0193-92EC-4248-8B27-320C824EDFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -1502,21 +1502,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r16.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;  Loading Ammo</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r12.11 Tanks or Panzerkampfwagen (Pz)&lt;/Bold&gt; 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Panzer (armored) + kampf (fighting) + wagen (vehicle) = armored fighting vehicle (AFV). Tanks have turrets and appear in four types: 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
- -- Pz IV: medium tank&lt;LineBreak/&gt;
- -- Pz V: Pather medium tank&lt;LineBreak/&gt;
- -- Pz VIe: Tiger heavy tank&lt;LineBreak/&gt;
- -- Pz VIb: King Tiger heavy tank
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c79PzIV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c80PzV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c81PzVIe'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
-     &lt;InlineUIContainer&gt;&lt;Image Name='c82PzVIb'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r12.14 Panzerspahwagen (PSW)&lt;/Bold&gt; 
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 Armored scout car.
@@ -4031,6 +4016,21 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 When this event is rolled, roll on the 
 &lt;InlineUIContainer&gt;&lt;Button Content='Collateral' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Damage Table.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r12.11 Tanks or Panzerkampfwagen (Pz)&lt;/Bold&gt; 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Panzer (armored) + kampf (fighting) + wagen (vehicle) = armored fighting vehicle (AFV). Tanks have turrets and appear in four types: 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+ -- Pz IV: medium tank&lt;LineBreak/&gt;
+ -- Pz V: Pather medium tank&lt;LineBreak/&gt;
+ -- Pz VIe: Tiger heavy tank&lt;LineBreak/&gt;
+ -- Pz VIb: King Tiger heavy tank
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c79PzIV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c80PzV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c82PzVIe'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
+     &lt;InlineUIContainer&gt;&lt;Image Name='c81PzVIb'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
   </si>
 </sst>
 </file>
@@ -4405,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4420,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4452,7 +4452,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4460,7 +4460,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4492,7 +4492,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4636,7 +4636,7 @@
         <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4644,7 +4644,7 @@
         <v>132</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4652,7 +4652,7 @@
         <v>133</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4676,7 +4676,7 @@
         <v>226</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4708,135 +4708,135 @@
         <v>230</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>167</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4964,7 +4964,7 @@
         <v>210</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4988,7 +4988,7 @@
         <v>191</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5041,562 +5041,562 @@
     </row>
     <row r="79" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>293</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="255" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>233</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5620,7 +5620,7 @@
         <v>234</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>253</v>
+        <v>597</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -5628,7 +5628,7 @@
         <v>235</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5636,7 +5636,7 @@
         <v>236</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5644,7 +5644,7 @@
         <v>237</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5652,7 +5652,7 @@
         <v>238</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5660,7 +5660,7 @@
         <v>239</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5668,7 +5668,7 @@
         <v>240</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5676,7 +5676,7 @@
         <v>241</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5708,7 +5708,7 @@
         <v>245</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5716,7 +5716,7 @@
         <v>246</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -5724,183 +5724,183 @@
         <v>247</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="B175" s="2" t="s">
         <v>263</v>
-      </c>
-      <c r="B175" s="2" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="185" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -5940,7 +5940,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5956,15 +5956,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -5996,7 +5996,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6060,7 +6060,7 @@
         <v>107</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6076,7 +6076,7 @@
         <v>116</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6084,7 +6084,7 @@
         <v>117</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="210" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>118</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6100,127 +6100,127 @@
         <v>119</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A213" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>449</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="214" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A214" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="215" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A215" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="216" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A216" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A217" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A218" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A219" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="220" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A220" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A222" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A223" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="224" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="225" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A225" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="226" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A226" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="227" spans="1:2" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6236,7 +6236,7 @@
         <v>31</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="229" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6332,7 +6332,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6356,7 +6356,7 @@
         <v>11</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="244" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6396,7 +6396,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6404,7 +6404,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6412,7 +6412,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6420,7 +6420,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6508,7 +6508,7 @@
         <v>150</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="263" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -6524,7 +6524,7 @@
         <v>157</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6532,7 +6532,7 @@
         <v>160</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6540,31 +6540,31 @@
         <v>158</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6625,186 +6625,186 @@
     </row>
     <row r="277" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="279" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>537</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix issue with decorations: commander pulls cm from buring tank and applying offcier bonus for CMO. Fix issue with HVSS.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFAE0193-92EC-4248-8B27-320C824EDFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61D9B325-1817-4F1F-B5DD-FB1DA734A612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -2984,19 +2984,6 @@
     <t>r27.22</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r27.0 Retrofitting&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During the periods on the Combat Calendar marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining new crews. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-During a refit period, you have the option of replacing your current tank per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-If the refit takes at least 7 days, you may attempt to improve your crew ratings per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
-and train your crew to use the gyrostablilizer per 
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
-  </si>
-  <si>
     <t>r24.0</t>
   </si>
   <si>
@@ -3695,27 +3682,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='AAR' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; that the crew is gyroStabilizer trained.</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;Bold&gt;r27.22 Stabilizer Use&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In order to use the stabilizer, your crew must be trained in its use. If not trained, you may not fire the main gun during rounds when the tank is moved or pivoted. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Trained crews may fire the main gun when the tank is moving or pivoting, although with the pentalty shown on the To Hit Tables. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Gyrostabilizer training takes place during Refitting periods. </t>
-  </si>
-  <si>
-    <t>&lt;Bold&gt;r27.2 Gyrostabilizer&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-A gyrostabilizer was attached to the main gun of the Sherman tank is to keep the gun stabilized, or steady, in the vertical axis (up-down). 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-When turned on, it would keep the gun in a level position while the tank moved.  In theory, this allowed the gunner to keep the gun aimed at a target when moving by adjusting only the turret&amp;apos;s rotation. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-In practice, most crews found the Stabilizer dangerous (the gun would move up and down on its own) and difficult to use. However, others thought the Stabilizer was a great asset if properly used.
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Training Crew&lt;LineBreak/&gt;
-&lt;InlineUIContainer&gt;&lt;Button Content='r27.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Stabilizer Use</t>
-  </si>
-  <si>
     <t>&lt;Bold&gt;r20.41 Counterattack - Preparations&lt;/Bold&gt;
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 For step &lt;InlineUIContainer&gt;&lt;Button Content='r4.41' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;, 
@@ -4031,6 +3997,40 @@
      &lt;InlineUIContainer&gt;&lt;Image Name='c80PzV'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
      &lt;InlineUIContainer&gt;&lt;Image Name='c82PzVIe'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;
      &lt;InlineUIContainer&gt;&lt;Image Name='c81PzVIb'  Height='100' Width='100'&gt;&lt;/Image&gt;&lt;/InlineUIContainer&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r27.0 Retrofitting and Horizontal Volute Spring Suspension (HVSS)&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During the periods on the Combat Calendar marked Refitting, the Division is building itself back up to strength, replacing tanks, and retraining new crews. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+During a refit period, you have the option of replacing your current tank per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r24.0' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+If the refit takes at least 7 days, you may attempt to improve your crew ratings per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.1' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; 
+and train your crew to use the gyrostablilizer per 
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;.</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r27.2 Gyrostabilizer, a.k.a., HVSS&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+A gyrostabilizer, a.k.a., Horizontal Volute Spring Suspension, was attached to the main gun of the Sherman tank is to keep the gun stabilized, or steady, in the vertical axis (up-down). 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+When turned on, it would keep the gun in a level position while the tank moved.  In theory, this allowed the gunner to keep the gun aimed at a target when moving by adjusting only the turret&amp;apos;s rotation. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In practice, most crews found the Stabilizer dangerous (the gun would move up and down on its own) and difficult to use. However, others thought the Stabilizer was a great asset if properly used.
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Training Crew&lt;LineBreak/&gt;
+&lt;InlineUIContainer&gt;&lt;Button Content='r27.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Stabilizer Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Bold&gt;r27.22 Stabilizer Use&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+In order to use the stabilizer, a.k.a, Horizontal Volute Spring Suspension, your crew must be trained in its use. If not trained, you may not fire the main gun during rounds when the tank is moved or pivoted. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Trained crews may fire the main gun when the tank is moving or pivoting, although with the pentalty shown on the To Hit Tables. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Gyrostabilizer training takes place during Refitting periods. </t>
   </si>
 </sst>
 </file>
@@ -4405,8 +4405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B281" sqref="B281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4420,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4452,7 +4452,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4460,7 +4460,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4636,7 +4636,7 @@
         <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4644,7 +4644,7 @@
         <v>132</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4652,7 +4652,7 @@
         <v>133</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4676,7 +4676,7 @@
         <v>226</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
         <v>230</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4748,39 +4748,39 @@
         <v>442</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -4788,7 +4788,7 @@
         <v>443</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4796,7 +4796,7 @@
         <v>444</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4804,7 +4804,7 @@
         <v>445</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4812,31 +4812,31 @@
         <v>446</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4956,7 +4956,7 @@
         <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4964,7 +4964,7 @@
         <v>210</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4988,7 +4988,7 @@
         <v>191</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5044,7 +5044,7 @@
         <v>264</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5052,7 +5052,7 @@
         <v>265</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5068,7 +5068,7 @@
         <v>267</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5124,7 +5124,7 @@
         <v>274</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5380,7 +5380,7 @@
         <v>344</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5388,7 +5388,7 @@
         <v>336</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5476,7 +5476,7 @@
         <v>369</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5540,7 +5540,7 @@
         <v>382</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>233</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5620,7 +5620,7 @@
         <v>234</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -5636,7 +5636,7 @@
         <v>236</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5732,7 +5732,7 @@
         <v>365</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5740,7 +5740,7 @@
         <v>409</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5868,7 +5868,7 @@
         <v>405</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5940,7 +5940,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5956,15 +5956,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -6060,7 +6060,7 @@
         <v>107</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6076,7 +6076,7 @@
         <v>116</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>118</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6100,7 +6100,7 @@
         <v>119</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -6172,7 +6172,7 @@
         <v>463</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6180,7 +6180,7 @@
         <v>464</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6188,7 +6188,7 @@
         <v>465</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6332,7 +6332,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6396,7 +6396,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6404,7 +6404,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6412,7 +6412,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6420,7 +6420,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6524,7 +6524,7 @@
         <v>157</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6532,7 +6532,7 @@
         <v>160</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6540,31 +6540,31 @@
         <v>158</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="267" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="268" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="270" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -6628,7 +6628,7 @@
         <v>482</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>488</v>
+        <v>595</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -6644,7 +6644,7 @@
         <v>484</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>571</v>
+        <v>596</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -6652,7 +6652,7 @@
         <v>486</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -6660,151 +6660,151 @@
         <v>487</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>570</v>
+        <v>597</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>536</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added text to explain how to start new game in option dialog.
</commit_message>
<xml_diff>
--- a/DesignDocs/Rules.xlsx
+++ b/DesignDocs/Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstew\source\repos\PattonsBest\DesignDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cstewa01\source\repos\happysulla\PattonsBest\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB5BA6A-99EE-4C35-99E6-50D651540562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEBE35C8-8B3D-45FC-9047-B830EF5BEEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{89590866-6083-4176-8CBF-8C95C9BA24C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules" sheetId="1" r:id="rId1"/>
@@ -3032,17 +3032,6 @@
 &lt;InlineUIContainer&gt;&lt;Button Content='r24.2' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Tank Replacement Table</t>
   </si>
   <si>
-    <t>&lt;Bold&gt;r24.1 Tank Replacement&lt;/Bold&gt;
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Players beginning a campaign game are issued an M4 tank with a type A turret with a 75 gun (Tank #1).
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-Tanks may be replaced udner two circumstances: after you have had a tank shot out from under you (knoched out) in combat or during a refit period on the Campaign 
-&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
-&lt;LineBreak/&gt;&lt;LineBreak/&gt;
-There is no historical basis for replacing tanks during refits, and players may keep their old model as long as they can. Destroyed tanks must be replaced per the Tank 
-&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.</t>
-  </si>
-  <si>
     <t>r29.0</t>
   </si>
   <si>
@@ -4035,6 +4024,17 @@
 &lt;LineBreak/&gt;&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.21' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Training Crew&lt;LineBreak/&gt;
 &lt;InlineUIContainer&gt;&lt;Button Content='r27.22' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Stabilizer Use</t>
+  </si>
+  <si>
+    <t>&lt;Bold&gt;r24.1 Tank Replacement&lt;/Bold&gt;
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Players beginning a campaign game are issued an M4 tank with a type A turret with a 75 gun (Tank #1).
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+Tanks may be replaced under two circumstances: after you have had a tank shot out from under you (knocked out) in combat or during a refit period on the Campaign 
+&lt;InlineUIContainer&gt;&lt;Button Content='Calendar' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt;. 
+&lt;LineBreak/&gt;&lt;LineBreak/&gt;
+There is no historical basis for replacing tanks during refits, and players may keep their old model as long as they can. Destroyed tanks must be replaced per the Tank 
+&lt;InlineUIContainer&gt;&lt;Button Content='Replacement' FontFamily='Courier New'  FontSize='12'&gt;&lt;/Button&gt;&lt;/InlineUIContainer&gt; Table.</t>
   </si>
 </sst>
 </file>
@@ -4409,8 +4409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7370C4-35CC-4CF6-93A4-4A91468DAED0}">
   <dimension ref="A1:B382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B281" sqref="B280:B281"/>
+    <sheetView tabSelected="1" topLeftCell="A267" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B268" sqref="B268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4424,7 +4424,7 @@
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="91.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -4456,7 +4456,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4464,7 +4464,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -4600,7 +4600,7 @@
         <v>126</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4640,7 +4640,7 @@
         <v>131</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4648,7 +4648,7 @@
         <v>132</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -4656,7 +4656,7 @@
         <v>133</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="360" x14ac:dyDescent="0.25">
@@ -4680,7 +4680,7 @@
         <v>226</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -4712,7 +4712,7 @@
         <v>230</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4752,39 +4752,39 @@
         <v>442</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="300" x14ac:dyDescent="0.25">
@@ -4792,7 +4792,7 @@
         <v>443</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -4800,7 +4800,7 @@
         <v>444</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -4808,7 +4808,7 @@
         <v>445</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -4816,31 +4816,31 @@
         <v>446</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="240" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="390" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -4960,7 +4960,7 @@
         <v>209</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -4968,7 +4968,7 @@
         <v>210</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -4992,7 +4992,7 @@
         <v>191</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5048,7 +5048,7 @@
         <v>264</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5056,7 +5056,7 @@
         <v>265</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5072,7 +5072,7 @@
         <v>267</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="135" x14ac:dyDescent="0.25">
@@ -5128,7 +5128,7 @@
         <v>274</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5384,7 +5384,7 @@
         <v>344</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5392,7 +5392,7 @@
         <v>336</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5480,7 +5480,7 @@
         <v>369</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -5544,7 +5544,7 @@
         <v>382</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -5616,7 +5616,7 @@
         <v>233</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5624,7 +5624,7 @@
         <v>234</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="225" x14ac:dyDescent="0.25">
@@ -5640,7 +5640,7 @@
         <v>236</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5736,7 +5736,7 @@
         <v>365</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="195" x14ac:dyDescent="0.25">
@@ -5744,7 +5744,7 @@
         <v>409</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="75" x14ac:dyDescent="0.25">
@@ -5872,7 +5872,7 @@
         <v>405</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="183" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -5944,7 +5944,7 @@
         <v>77</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="192" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -5960,15 +5960,15 @@
         <v>79</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
+        <v>529</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>530</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="195" spans="1:2" ht="240" x14ac:dyDescent="0.25">
@@ -6064,7 +6064,7 @@
         <v>107</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6080,7 +6080,7 @@
         <v>116</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6096,7 +6096,7 @@
         <v>118</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="211" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6104,7 +6104,7 @@
         <v>119</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="285" x14ac:dyDescent="0.25">
@@ -6176,7 +6176,7 @@
         <v>463</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6184,7 +6184,7 @@
         <v>464</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="222" spans="1:2" ht="180" x14ac:dyDescent="0.25">
@@ -6192,7 +6192,7 @@
         <v>465</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="223" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -6336,7 +6336,7 @@
         <v>67</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="241" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6400,7 +6400,7 @@
         <v>5</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="249" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6408,7 +6408,7 @@
         <v>6</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="255" x14ac:dyDescent="0.25">
@@ -6416,7 +6416,7 @@
         <v>7</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="251" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6424,7 +6424,7 @@
         <v>8</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="104.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6528,7 +6528,7 @@
         <v>157</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="265" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6536,7 +6536,7 @@
         <v>160</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="266" spans="1:2" ht="165" x14ac:dyDescent="0.25">
@@ -6560,7 +6560,7 @@
         <v>489</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>494</v>
+        <v>597</v>
       </c>
     </row>
     <row r="269" spans="1:2" ht="150" x14ac:dyDescent="0.25">
@@ -6632,7 +6632,7 @@
         <v>482</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="278" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -6648,7 +6648,7 @@
         <v>484</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="280" spans="1:2" ht="120" x14ac:dyDescent="0.25">
@@ -6656,7 +6656,7 @@
         <v>486</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="281" spans="1:2" ht="105" x14ac:dyDescent="0.25">
@@ -6664,151 +6664,151 @@
         <v>487</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="282" spans="1:2" ht="270" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="283" spans="1:2" ht="150" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="284" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="285" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="286" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B286" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="287" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="288" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B288" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="289" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="290" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="291" spans="1:2" ht="195" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="292" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="293" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="294" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="295" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B295" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="B295" s="3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="296" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="297" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B297" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="298" spans="1:2" ht="135" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B298" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="299" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B299" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>